<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add_taz_num_is_unique_row & add_taz_num_count_row functions & add_percentage_growth_row function
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df.xlsx
+++ b/create_forecast_basic/utils/monitoring_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>2020</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Taz_U_Orthodox</t>
   </si>
   <si>
+    <t>Taz_Palestinian</t>
+  </si>
+  <si>
     <t>Taz_arabs_behined_seperation_wall</t>
   </si>
   <si>
@@ -52,6 +55,12 @@
     <t>Taz_Jewish</t>
   </si>
   <si>
+    <t>univ_2020</t>
+  </si>
+  <si>
+    <t>univ_2050</t>
+  </si>
+  <si>
     <t>student_2020</t>
   </si>
   <si>
@@ -64,6 +73,48 @@
     <t>student_yeshiva_and_kollim_2050</t>
   </si>
   <si>
+    <t>zonetype_Jerusalem</t>
+  </si>
+  <si>
+    <t>zonetype_Judea and Samaria</t>
+  </si>
+  <si>
+    <t>zonetype_Ramla</t>
+  </si>
+  <si>
+    <t>jeru_metro_0</t>
+  </si>
+  <si>
+    <t>jeru_metro_1</t>
+  </si>
+  <si>
+    <t>in_jerusal_yes</t>
+  </si>
+  <si>
+    <t>in_jerusal_no</t>
+  </si>
+  <si>
+    <t>taz_num_is_unique</t>
+  </si>
+  <si>
+    <t>taz_num_count</t>
+  </si>
+  <si>
+    <t>percentage growth 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth 2045-2050</t>
+  </si>
+  <si>
     <t>1,758,461</t>
   </si>
   <si>
@@ -71,6 +122,9 @@
   </si>
   <si>
     <t>482,716</t>
+  </si>
+  <si>
+    <t>81,184</t>
   </si>
   <si>
     <t>412,854</t>
@@ -470,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,16 +549,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -512,16 +566,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -529,16 +583,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -546,16 +600,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -580,16 +634,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -597,16 +651,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>86</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -614,33 +668,33 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>482</v>
+        <v>86</v>
       </c>
       <c r="C9">
-        <v>482</v>
+        <v>86</v>
       </c>
       <c r="D9">
-        <v>472</v>
+        <v>86</v>
       </c>
       <c r="E9">
-        <v>450</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
+      <c r="B10">
+        <v>482</v>
+      </c>
+      <c r="C10">
+        <v>482</v>
+      </c>
+      <c r="D10">
+        <v>472</v>
+      </c>
+      <c r="E10">
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -648,16 +702,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -665,16 +719,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -682,16 +736,305 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>580</v>
+      </c>
+      <c r="C17">
+        <v>580</v>
+      </c>
+      <c r="D17">
+        <v>580</v>
+      </c>
+      <c r="E17">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>288</v>
+      </c>
+      <c r="C18">
+        <v>288</v>
+      </c>
+      <c r="D18">
+        <v>288</v>
+      </c>
+      <c r="E18">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <v>36</v>
+      </c>
+      <c r="E19">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>74</v>
+      </c>
+      <c r="C20">
+        <v>74</v>
+      </c>
+      <c r="D20">
+        <v>74</v>
+      </c>
+      <c r="E20">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>830</v>
+      </c>
+      <c r="C21">
+        <v>830</v>
+      </c>
+      <c r="D21">
+        <v>830</v>
+      </c>
+      <c r="E21">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B22">
+        <v>460</v>
+      </c>
+      <c r="C22">
+        <v>460</v>
+      </c>
+      <c r="D22">
+        <v>460</v>
+      </c>
+      <c r="E22">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>444</v>
+      </c>
+      <c r="C23">
+        <v>444</v>
+      </c>
+      <c r="D23">
+        <v>444</v>
+      </c>
+      <c r="E23">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>904</v>
+      </c>
+      <c r="C25">
+        <v>904</v>
+      </c>
+      <c r="D25">
+        <v>904</v>
+      </c>
+      <c r="E25">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26">
+        <v>288</v>
+      </c>
+      <c r="D26">
+        <v>283</v>
+      </c>
+      <c r="E26">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>110</v>
+      </c>
+      <c r="D27">
+        <v>109</v>
+      </c>
+      <c r="E27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>109</v>
+      </c>
+      <c r="D28">
+        <v>108</v>
+      </c>
+      <c r="E28">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>109</v>
+      </c>
+      <c r="D29">
+        <v>107</v>
+      </c>
+      <c r="E29">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30">
+        <v>94</v>
+      </c>
+      <c r="D30">
+        <v>93</v>
+      </c>
+      <c r="E30">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add_students_by_SCHOOLDIST function
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df.xlsx
+++ b/create_forecast_basic/utils/monitoring_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="205">
   <si>
     <t>2020</t>
   </si>
@@ -40,19 +40,19 @@
     <t>emp_2050</t>
   </si>
   <si>
-    <t>Taz_U_Orthodox</t>
-  </si>
-  <si>
-    <t>Taz_Palestinian</t>
-  </si>
-  <si>
-    <t>Taz_arabs_behined_seperation_wall</t>
-  </si>
-  <si>
-    <t>Taz_Arab</t>
-  </si>
-  <si>
-    <t>Taz_Jewish</t>
+    <t>Taz_U_Jewish</t>
+  </si>
+  <si>
+    <t>Taz_U_U_Orthodox</t>
+  </si>
+  <si>
+    <t>Taz_U_Palestinian</t>
+  </si>
+  <si>
+    <t>Taz_U_Arab</t>
+  </si>
+  <si>
+    <t>Taz_U_arabs_behined_seperation_wall</t>
   </si>
   <si>
     <t>univ_2020</t>
@@ -82,12 +82,12 @@
     <t>zonetype_Ramla</t>
   </si>
   <si>
+    <t>jeru_metro_1</t>
+  </si>
+  <si>
     <t>jeru_metro_0</t>
   </si>
   <si>
-    <t>jeru_metro_1</t>
-  </si>
-  <si>
     <t>in_jerusal_yes</t>
   </si>
   <si>
@@ -113,6 +113,468 @@
   </si>
   <si>
     <t>percentage growth 2045-2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_5_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_0_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_18_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_6_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_7_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_16_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_3_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_20_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_17_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_4_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_2_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_14_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_15_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_19_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_13_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_12_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_1_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_21_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_11_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_9_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_10_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_8_2020</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_5_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_0_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_18_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_6_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_7_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_16_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_3_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_20_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_17_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_4_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_2_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_14_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_15_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_19_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_13_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_12_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_1_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_21_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_11_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_9_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_10_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_8_2025</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_5_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_0_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_18_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_6_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_7_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_16_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_3_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_20_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_17_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_4_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_2_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_14_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_15_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_19_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_13_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_12_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_1_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_21_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_11_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_9_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_10_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_8_2030</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_5_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_0_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_18_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_6_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_7_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_16_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_3_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_20_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_17_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_4_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_2_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_14_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_15_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_19_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_13_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_12_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_1_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_21_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_11_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_9_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_10_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_8_2035</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_5_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_0_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_18_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_6_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_7_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_16_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_3_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_20_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_17_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_4_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_2_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_14_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_15_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_19_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_13_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_12_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_1_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_21_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_11_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_9_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_10_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_8_2040</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_5_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_0_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_18_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_6_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_7_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_16_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_3_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_20_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_17_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_4_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_2_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_14_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_15_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_19_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_13_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_12_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_1_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_21_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_11_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_9_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_10_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_8_2045</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_5_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_0_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_18_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_6_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_7_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_16_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_3_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_20_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_17_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_4_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_2_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_14_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_15_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_19_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_13_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_12_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_1_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_21_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_11_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_9_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_10_2050</t>
+  </si>
+  <si>
+    <t>SCHOOLDIST_8_2050</t>
   </si>
   <si>
     <t>1,758,461</t>
@@ -524,7 +986,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,16 +1011,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -566,16 +1028,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>197</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -583,16 +1045,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -600,16 +1062,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>198</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -617,16 +1079,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>174</v>
+        <v>482</v>
       </c>
       <c r="C6">
-        <v>174</v>
+        <v>482</v>
       </c>
       <c r="D6">
-        <v>184</v>
+        <v>472</v>
       </c>
       <c r="E6">
-        <v>206</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -634,16 +1096,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="C7">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D7">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E7">
-        <v>157</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -651,16 +1113,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -685,16 +1147,16 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>482</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>482</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>472</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>450</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -702,16 +1164,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -719,16 +1181,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -736,16 +1198,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -753,16 +1215,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>199</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -770,16 +1232,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -787,16 +1249,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -855,16 +1317,16 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>74</v>
+        <v>830</v>
       </c>
       <c r="C20">
-        <v>74</v>
+        <v>830</v>
       </c>
       <c r="D20">
-        <v>74</v>
+        <v>830</v>
       </c>
       <c r="E20">
-        <v>74</v>
+        <v>830</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -872,16 +1334,16 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>830</v>
+        <v>74</v>
       </c>
       <c r="C21">
-        <v>830</v>
+        <v>74</v>
       </c>
       <c r="D21">
-        <v>830</v>
+        <v>74</v>
       </c>
       <c r="E21">
-        <v>830</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -957,7 +1419,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C26">
         <v>288</v>
@@ -974,7 +1436,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C27">
         <v>110</v>
@@ -991,7 +1453,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C28">
         <v>109</v>
@@ -1008,7 +1470,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C29">
         <v>109</v>
@@ -1025,7 +1487,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="C30">
         <v>94</v>
@@ -1035,6 +1497,2624 @@
       </c>
       <c r="E30">
         <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>213239.3333333333</v>
+      </c>
+      <c r="C31">
+        <v>213239.3333333333</v>
+      </c>
+      <c r="D31">
+        <v>213239.3333333333</v>
+      </c>
+      <c r="E31">
+        <v>213239.3333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>28627.66666666667</v>
+      </c>
+      <c r="C32">
+        <v>28627.66666666667</v>
+      </c>
+      <c r="D32">
+        <v>28627.66666666667</v>
+      </c>
+      <c r="E32">
+        <v>28627.66666666667</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>46063</v>
+      </c>
+      <c r="C33">
+        <v>46063</v>
+      </c>
+      <c r="D33">
+        <v>46063</v>
+      </c>
+      <c r="E33">
+        <v>46063</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>23828</v>
+      </c>
+      <c r="C34">
+        <v>23828</v>
+      </c>
+      <c r="D34">
+        <v>23828</v>
+      </c>
+      <c r="E34">
+        <v>23828</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>8538</v>
+      </c>
+      <c r="C35">
+        <v>8538</v>
+      </c>
+      <c r="D35">
+        <v>8538</v>
+      </c>
+      <c r="E35">
+        <v>8538</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>5048</v>
+      </c>
+      <c r="C36">
+        <v>5048</v>
+      </c>
+      <c r="D36">
+        <v>5048</v>
+      </c>
+      <c r="E36">
+        <v>5048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>21988.00000000001</v>
+      </c>
+      <c r="C37">
+        <v>21988</v>
+      </c>
+      <c r="D37">
+        <v>21988</v>
+      </c>
+      <c r="E37">
+        <v>21988</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>27262</v>
+      </c>
+      <c r="C38">
+        <v>27262</v>
+      </c>
+      <c r="D38">
+        <v>27262</v>
+      </c>
+      <c r="E38">
+        <v>27262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>2804</v>
+      </c>
+      <c r="C39">
+        <v>2804</v>
+      </c>
+      <c r="D39">
+        <v>2804</v>
+      </c>
+      <c r="E39">
+        <v>2804</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>1331</v>
+      </c>
+      <c r="C40">
+        <v>1331</v>
+      </c>
+      <c r="D40">
+        <v>1331</v>
+      </c>
+      <c r="E40">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>7375</v>
+      </c>
+      <c r="C41">
+        <v>7375</v>
+      </c>
+      <c r="D41">
+        <v>7375</v>
+      </c>
+      <c r="E41">
+        <v>7375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>8805</v>
+      </c>
+      <c r="C42">
+        <v>8805</v>
+      </c>
+      <c r="D42">
+        <v>8805</v>
+      </c>
+      <c r="E42">
+        <v>8805</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>1218</v>
+      </c>
+      <c r="C43">
+        <v>1218</v>
+      </c>
+      <c r="D43">
+        <v>1218</v>
+      </c>
+      <c r="E43">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>1673</v>
+      </c>
+      <c r="C44">
+        <v>1673</v>
+      </c>
+      <c r="D44">
+        <v>1673</v>
+      </c>
+      <c r="E44">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>2401</v>
+      </c>
+      <c r="C45">
+        <v>2401</v>
+      </c>
+      <c r="D45">
+        <v>2401</v>
+      </c>
+      <c r="E45">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <v>2488</v>
+      </c>
+      <c r="C46">
+        <v>2488</v>
+      </c>
+      <c r="D46">
+        <v>2488</v>
+      </c>
+      <c r="E46">
+        <v>2488</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <v>2148</v>
+      </c>
+      <c r="C47">
+        <v>2148</v>
+      </c>
+      <c r="D47">
+        <v>2148</v>
+      </c>
+      <c r="E47">
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48">
+        <v>3242</v>
+      </c>
+      <c r="C48">
+        <v>3242</v>
+      </c>
+      <c r="D48">
+        <v>3242</v>
+      </c>
+      <c r="E48">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>3637</v>
+      </c>
+      <c r="C49">
+        <v>3637</v>
+      </c>
+      <c r="D49">
+        <v>3637</v>
+      </c>
+      <c r="E49">
+        <v>3637</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>301</v>
+      </c>
+      <c r="C50">
+        <v>301</v>
+      </c>
+      <c r="D50">
+        <v>301</v>
+      </c>
+      <c r="E50">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51">
+        <v>537</v>
+      </c>
+      <c r="C51">
+        <v>537</v>
+      </c>
+      <c r="D51">
+        <v>537</v>
+      </c>
+      <c r="E51">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <v>300</v>
+      </c>
+      <c r="C52">
+        <v>300</v>
+      </c>
+      <c r="D52">
+        <v>300</v>
+      </c>
+      <c r="E52">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>188</v>
+      </c>
+      <c r="C53">
+        <v>285733.3218235314</v>
+      </c>
+      <c r="D53">
+        <v>274161.0000038777</v>
+      </c>
+      <c r="E53">
+        <v>275663.3373324008</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54">
+        <v>36057.66373063793</v>
+      </c>
+      <c r="D54">
+        <v>33344.22909790605</v>
+      </c>
+      <c r="E54">
+        <v>34286.84568702983</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>188</v>
+      </c>
+      <c r="C55">
+        <v>66822.51137331135</v>
+      </c>
+      <c r="D55">
+        <v>61855.23107261454</v>
+      </c>
+      <c r="E55">
+        <v>63948.66570649843</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56">
+        <v>33156.30459804353</v>
+      </c>
+      <c r="D56">
+        <v>33335.50923218194</v>
+      </c>
+      <c r="E56">
+        <v>33397.07322472375</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57">
+        <v>9986.417617537509</v>
+      </c>
+      <c r="D57">
+        <v>10194.62059102478</v>
+      </c>
+      <c r="E57">
+        <v>10338.40358091756</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>188</v>
+      </c>
+      <c r="C58">
+        <v>8306.813376518987</v>
+      </c>
+      <c r="D58">
+        <v>6946.591660718233</v>
+      </c>
+      <c r="E58">
+        <v>8135.667377017133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59">
+        <v>29427.44116169451</v>
+      </c>
+      <c r="D59">
+        <v>30953.22576377643</v>
+      </c>
+      <c r="E59">
+        <v>31386.31536916655</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60">
+        <v>37145.33462606892</v>
+      </c>
+      <c r="D60">
+        <v>39041.11738664036</v>
+      </c>
+      <c r="E60">
+        <v>40239.51136715176</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" t="s">
+        <v>188</v>
+      </c>
+      <c r="C61">
+        <v>5309.478782988256</v>
+      </c>
+      <c r="D61">
+        <v>5060.408660766857</v>
+      </c>
+      <c r="E61">
+        <v>5201.12526897965</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62">
+        <v>5521.895631861405</v>
+      </c>
+      <c r="D62">
+        <v>6073.616715538182</v>
+      </c>
+      <c r="E62">
+        <v>6265.692004112236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" t="s">
+        <v>188</v>
+      </c>
+      <c r="C63">
+        <v>7012.74256878429</v>
+      </c>
+      <c r="D63">
+        <v>6467.15326810131</v>
+      </c>
+      <c r="E63">
+        <v>6547.602648720247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64">
+        <v>7317.313641591267</v>
+      </c>
+      <c r="D64">
+        <v>7240.499364931959</v>
+      </c>
+      <c r="E64">
+        <v>7309.076098225414</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" t="s">
+        <v>188</v>
+      </c>
+      <c r="C65">
+        <v>2166.404734331622</v>
+      </c>
+      <c r="D65">
+        <v>2013.947393383935</v>
+      </c>
+      <c r="E65">
+        <v>2067.009181064854</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66">
+        <v>3081.965248662672</v>
+      </c>
+      <c r="D66">
+        <v>3137.447595991872</v>
+      </c>
+      <c r="E66">
+        <v>3186.615419267629</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67">
+        <v>443.1341918519325</v>
+      </c>
+      <c r="D67">
+        <v>421.887538681912</v>
+      </c>
+      <c r="E67">
+        <v>433.4544189987498</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" t="s">
+        <v>188</v>
+      </c>
+      <c r="C68">
+        <v>2895.085614458657</v>
+      </c>
+      <c r="D68">
+        <v>2909.362870154178</v>
+      </c>
+      <c r="E68">
+        <v>2924.168116891962</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" t="s">
+        <v>188</v>
+      </c>
+      <c r="C69">
+        <v>3653.831655445544</v>
+      </c>
+      <c r="D69">
+        <v>3598.638480494133</v>
+      </c>
+      <c r="E69">
+        <v>3616.404971165329</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70">
+        <v>3542.454003930634</v>
+      </c>
+      <c r="D70">
+        <v>3648.230892236539</v>
+      </c>
+      <c r="E70">
+        <v>3678.324608989895</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71">
+        <v>4257.401768859199</v>
+      </c>
+      <c r="D71">
+        <v>4324.862744573556</v>
+      </c>
+      <c r="E71">
+        <v>4363.718311116243</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" t="s">
+        <v>188</v>
+      </c>
+      <c r="C72">
+        <v>881.1481005457115</v>
+      </c>
+      <c r="D72">
+        <v>922.4946308419028</v>
+      </c>
+      <c r="E72">
+        <v>951.6553445648265</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" t="s">
+        <v>188</v>
+      </c>
+      <c r="C73">
+        <v>911.7413777070067</v>
+      </c>
+      <c r="D73">
+        <v>868.7478168054034</v>
+      </c>
+      <c r="E73">
+        <v>883.9572064300576</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" t="s">
+        <v>188</v>
+      </c>
+      <c r="C75">
+        <v>310887.0551086462</v>
+      </c>
+      <c r="D75">
+        <v>290797.302000507</v>
+      </c>
+      <c r="E75">
+        <v>292306.0034436272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" t="s">
+        <v>188</v>
+      </c>
+      <c r="C76">
+        <v>51074.32436027069</v>
+      </c>
+      <c r="D76">
+        <v>26072.86402002085</v>
+      </c>
+      <c r="E76">
+        <v>44744.53526801307</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>188</v>
+      </c>
+      <c r="C77">
+        <v>84109.82719823082</v>
+      </c>
+      <c r="D77">
+        <v>77937.73156609248</v>
+      </c>
+      <c r="E77">
+        <v>84581.97612214876</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" t="s">
+        <v>188</v>
+      </c>
+      <c r="C78">
+        <v>39310.49274971832</v>
+      </c>
+      <c r="D78">
+        <v>38683.92515358835</v>
+      </c>
+      <c r="E78">
+        <v>38875.73769831542</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" t="s">
+        <v>188</v>
+      </c>
+      <c r="C79">
+        <v>11932.38400809033</v>
+      </c>
+      <c r="D79">
+        <v>10681.35241281803</v>
+      </c>
+      <c r="E79">
+        <v>11035.70441498311</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" t="s">
+        <v>188</v>
+      </c>
+      <c r="C80">
+        <v>9548.28031721313</v>
+      </c>
+      <c r="D80">
+        <v>7703.305735153427</v>
+      </c>
+      <c r="E80">
+        <v>8161.797271070729</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" t="s">
+        <v>188</v>
+      </c>
+      <c r="C81">
+        <v>35810.66989709945</v>
+      </c>
+      <c r="D81">
+        <v>36601.69575249061</v>
+      </c>
+      <c r="E81">
+        <v>39241.8615517352</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" t="s">
+        <v>188</v>
+      </c>
+      <c r="C82">
+        <v>40274.91199119319</v>
+      </c>
+      <c r="D82">
+        <v>41351.35312049399</v>
+      </c>
+      <c r="E82">
+        <v>44632.82113421193</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83">
+        <v>5702.582508173264</v>
+      </c>
+      <c r="D83">
+        <v>5197.04316560074</v>
+      </c>
+      <c r="E83">
+        <v>5490.350510109492</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>188</v>
+      </c>
+      <c r="C84">
+        <v>6531.454941380145</v>
+      </c>
+      <c r="D84">
+        <v>6914.424310549415</v>
+      </c>
+      <c r="E84">
+        <v>7565.494786531661</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" t="s">
+        <v>188</v>
+      </c>
+      <c r="C85">
+        <v>11086.07248419944</v>
+      </c>
+      <c r="D85">
+        <v>9081.046501582416</v>
+      </c>
+      <c r="E85">
+        <v>9712.39919620127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" t="s">
+        <v>188</v>
+      </c>
+      <c r="C86">
+        <v>11235.01770760014</v>
+      </c>
+      <c r="D86">
+        <v>7294.264487669744</v>
+      </c>
+      <c r="E86">
+        <v>7393.954728795917</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87" t="s">
+        <v>188</v>
+      </c>
+      <c r="C87">
+        <v>2313.18743770475</v>
+      </c>
+      <c r="D87">
+        <v>2050.379609518187</v>
+      </c>
+      <c r="E87">
+        <v>2158.015018647229</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88">
+        <v>4487.422497745161</v>
+      </c>
+      <c r="D88">
+        <v>3251.340662315742</v>
+      </c>
+      <c r="E88">
+        <v>3680.595601936531</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" t="s">
+        <v>188</v>
+      </c>
+      <c r="C89">
+        <v>3291.571394333075</v>
+      </c>
+      <c r="D89">
+        <v>453.0691373312048</v>
+      </c>
+      <c r="E89">
+        <v>505.4945456516502</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" t="s">
+        <v>188</v>
+      </c>
+      <c r="C90">
+        <v>2962.271032197586</v>
+      </c>
+      <c r="D90">
+        <v>2922.939603860779</v>
+      </c>
+      <c r="E90">
+        <v>2944.717615440521</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" t="s">
+        <v>188</v>
+      </c>
+      <c r="C91">
+        <v>3978.851277647058</v>
+      </c>
+      <c r="D91">
+        <v>1566.476580450332</v>
+      </c>
+      <c r="E91">
+        <v>1592.42779801514</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" t="s">
+        <v>188</v>
+      </c>
+      <c r="C92">
+        <v>3624.875154413226</v>
+      </c>
+      <c r="D92">
+        <v>3677.660725632635</v>
+      </c>
+      <c r="E92">
+        <v>3727.402937205914</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" t="s">
+        <v>188</v>
+      </c>
+      <c r="C93">
+        <v>4499.453713305816</v>
+      </c>
+      <c r="D93">
+        <v>4389.339541465134</v>
+      </c>
+      <c r="E93">
+        <v>4489.156966460471</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94">
+        <v>1176.375213333053</v>
+      </c>
+      <c r="D94">
+        <v>1229.853805184373</v>
+      </c>
+      <c r="E94">
+        <v>1330.656790249233</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B95" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95">
+        <v>1013.219479989464</v>
+      </c>
+      <c r="D95">
+        <v>873.6169022987777</v>
+      </c>
+      <c r="E95">
+        <v>911.1327501980686</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96">
+        <v>857.2621118872319</v>
+      </c>
+      <c r="D96">
+        <v>772.2734198315197</v>
+      </c>
+      <c r="E96">
+        <v>801.0018403865388</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" t="s">
+        <v>188</v>
+      </c>
+      <c r="C97">
+        <v>345179.8540918057</v>
+      </c>
+      <c r="D97">
+        <v>306070.7824845224</v>
+      </c>
+      <c r="E97">
+        <v>311915.8222954976</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" t="s">
+        <v>188</v>
+      </c>
+      <c r="C98">
+        <v>57843.05696310467</v>
+      </c>
+      <c r="D98">
+        <v>41761.14805054816</v>
+      </c>
+      <c r="E98">
+        <v>48660.60638720006</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" t="s">
+        <v>188</v>
+      </c>
+      <c r="C99">
+        <v>106400.8113634808</v>
+      </c>
+      <c r="D99">
+        <v>97376.26626200562</v>
+      </c>
+      <c r="E99">
+        <v>107457.7153467231</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="s">
+        <v>188</v>
+      </c>
+      <c r="C100">
+        <v>47754.67592555143</v>
+      </c>
+      <c r="D100">
+        <v>46917.82385382168</v>
+      </c>
+      <c r="E100">
+        <v>47285.0706371487</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" t="s">
+        <v>188</v>
+      </c>
+      <c r="C101">
+        <v>13642.04328300475</v>
+      </c>
+      <c r="D101">
+        <v>12594.12090677959</v>
+      </c>
+      <c r="E101">
+        <v>14151.68818183644</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="s">
+        <v>188</v>
+      </c>
+      <c r="C102">
+        <v>10166.68671320246</v>
+      </c>
+      <c r="D102">
+        <v>7870.660600118454</v>
+      </c>
+      <c r="E102">
+        <v>8448.569974010888</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" t="s">
+        <v>188</v>
+      </c>
+      <c r="C103">
+        <v>40056.29615048355</v>
+      </c>
+      <c r="D103">
+        <v>39938.78970433185</v>
+      </c>
+      <c r="E103">
+        <v>44520.15917103966</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" t="s">
+        <v>188</v>
+      </c>
+      <c r="C104">
+        <v>42099.78280750295</v>
+      </c>
+      <c r="D104">
+        <v>42299.87775020443</v>
+      </c>
+      <c r="E104">
+        <v>47328.28098195308</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="s">
+        <v>188</v>
+      </c>
+      <c r="C105">
+        <v>6780.581746217548</v>
+      </c>
+      <c r="D105">
+        <v>5344.462556042371</v>
+      </c>
+      <c r="E105">
+        <v>5852.587839854697</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" t="s">
+        <v>188</v>
+      </c>
+      <c r="C106">
+        <v>7052.041776574091</v>
+      </c>
+      <c r="D106">
+        <v>2387.833946905571</v>
+      </c>
+      <c r="E106">
+        <v>2653.360912751024</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" t="s">
+        <v>188</v>
+      </c>
+      <c r="C107">
+        <v>12491.64080553533</v>
+      </c>
+      <c r="D107">
+        <v>7553.961214696117</v>
+      </c>
+      <c r="E107">
+        <v>8823.015551678049</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" t="s">
+        <v>188</v>
+      </c>
+      <c r="C108">
+        <v>11918.07029478611</v>
+      </c>
+      <c r="D108">
+        <v>10755.76769609013</v>
+      </c>
+      <c r="E108">
+        <v>11073.8263395291</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" t="s">
+        <v>188</v>
+      </c>
+      <c r="C109">
+        <v>2510.791313969085</v>
+      </c>
+      <c r="D109">
+        <v>2080.311820058766</v>
+      </c>
+      <c r="E109">
+        <v>2225.787307207039</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" t="s">
+        <v>188</v>
+      </c>
+      <c r="C110">
+        <v>5559.189168957029</v>
+      </c>
+      <c r="D110">
+        <v>3507.429258284409</v>
+      </c>
+      <c r="E110">
+        <v>4514.632917614302</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" t="s">
+        <v>188</v>
+      </c>
+      <c r="C111">
+        <v>3740.698985412615</v>
+      </c>
+      <c r="D111">
+        <v>456.0519360615073</v>
+      </c>
+      <c r="E111">
+        <v>595.516072795263</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" t="s">
+        <v>188</v>
+      </c>
+      <c r="C112">
+        <v>3025.982972811596</v>
+      </c>
+      <c r="D112">
+        <v>2930.200017528361</v>
+      </c>
+      <c r="E112">
+        <v>2972.156458241908</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" t="s">
+        <v>188</v>
+      </c>
+      <c r="C113">
+        <v>4384.134004159239</v>
+      </c>
+      <c r="D113">
+        <v>3877.68979844253</v>
+      </c>
+      <c r="E113">
+        <v>3984.413723700878</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114" t="s">
+        <v>188</v>
+      </c>
+      <c r="C114">
+        <v>3818.113674370041</v>
+      </c>
+      <c r="D114">
+        <v>3677.660725632635</v>
+      </c>
+      <c r="E114">
+        <v>3773.270697207371</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B115" t="s">
+        <v>188</v>
+      </c>
+      <c r="C115">
+        <v>5697.549039481555</v>
+      </c>
+      <c r="D115">
+        <v>4449.270708440607</v>
+      </c>
+      <c r="E115">
+        <v>4794.85366801385</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" t="s">
+        <v>188</v>
+      </c>
+      <c r="C116">
+        <v>1675.03137312741</v>
+      </c>
+      <c r="D116">
+        <v>1815.4386330182</v>
+      </c>
+      <c r="E116">
+        <v>2049.263941768266</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117" t="s">
+        <v>188</v>
+      </c>
+      <c r="C117">
+        <v>1388.615296125427</v>
+      </c>
+      <c r="D117">
+        <v>898.8243487684732</v>
+      </c>
+      <c r="E117">
+        <v>1101.853615098803</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B118" t="s">
+        <v>188</v>
+      </c>
+      <c r="C118">
+        <v>915.4210068592286</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B119" t="s">
+        <v>188</v>
+      </c>
+      <c r="C119">
+        <v>379833.2126030341</v>
+      </c>
+      <c r="D119">
+        <v>323789.1870151541</v>
+      </c>
+      <c r="E119">
+        <v>342305.1273678984</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B120" t="s">
+        <v>188</v>
+      </c>
+      <c r="C120">
+        <v>66636.46327624648</v>
+      </c>
+      <c r="D120">
+        <v>57885.11081377808</v>
+      </c>
+      <c r="E120">
+        <v>65450.5214985832</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B121" t="s">
+        <v>188</v>
+      </c>
+      <c r="C121">
+        <v>122447.4212601383</v>
+      </c>
+      <c r="D121">
+        <v>106273.0478090824</v>
+      </c>
+      <c r="E121">
+        <v>119530.3850553175</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B122" t="s">
+        <v>188</v>
+      </c>
+      <c r="C122">
+        <v>55098.14072490651</v>
+      </c>
+      <c r="D122">
+        <v>53997.08352943832</v>
+      </c>
+      <c r="E122">
+        <v>54429.29718809373</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B123" t="s">
+        <v>188</v>
+      </c>
+      <c r="C123">
+        <v>17436.20392355449</v>
+      </c>
+      <c r="D123">
+        <v>19678.07818882393</v>
+      </c>
+      <c r="E123">
+        <v>23411.63616688988</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B124" t="s">
+        <v>188</v>
+      </c>
+      <c r="C124">
+        <v>11477.1443269179</v>
+      </c>
+      <c r="D124">
+        <v>7941.17271971979</v>
+      </c>
+      <c r="E124">
+        <v>8685.454438123739</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" t="s">
+        <v>188</v>
+      </c>
+      <c r="C125">
+        <v>44788.85407568982</v>
+      </c>
+      <c r="D125">
+        <v>42290.86139964137</v>
+      </c>
+      <c r="E125">
+        <v>48116.24030242601</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" t="s">
+        <v>188</v>
+      </c>
+      <c r="C126">
+        <v>43854.83257609577</v>
+      </c>
+      <c r="D126">
+        <v>42446.11108034404</v>
+      </c>
+      <c r="E126">
+        <v>48048.47217811201</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" t="s">
+        <v>188</v>
+      </c>
+      <c r="C127">
+        <v>7818.02330571639</v>
+      </c>
+      <c r="D127">
+        <v>5653.095564499369</v>
+      </c>
+      <c r="E127">
+        <v>6625.371912088781</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B128" t="s">
+        <v>188</v>
+      </c>
+      <c r="C128">
+        <v>8085.182658295945</v>
+      </c>
+      <c r="D128">
+        <v>7503.614943774021</v>
+      </c>
+      <c r="E128">
+        <v>8938.0868588093</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B129" t="s">
+        <v>188</v>
+      </c>
+      <c r="C129">
+        <v>14492.94704346139</v>
+      </c>
+      <c r="D129">
+        <v>11209.84775023005</v>
+      </c>
+      <c r="E129">
+        <v>10752.42132399964</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" t="s">
+        <v>188</v>
+      </c>
+      <c r="C130">
+        <v>14025.08468897277</v>
+      </c>
+      <c r="D130">
+        <v>11232.84453326727</v>
+      </c>
+      <c r="E130">
+        <v>12584.87999504888</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131" t="s">
+        <v>188</v>
+      </c>
+      <c r="C131">
+        <v>2660.082565212768</v>
+      </c>
+      <c r="D131">
+        <v>2118.88338047299</v>
+      </c>
+      <c r="E131">
+        <v>2317.74860784036</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132" t="s">
+        <v>188</v>
+      </c>
+      <c r="C132">
+        <v>6699.919359426849</v>
+      </c>
+      <c r="D132">
+        <v>3926.964562863937</v>
+      </c>
+      <c r="E132">
+        <v>5419.280756815793</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B133" t="s">
+        <v>188</v>
+      </c>
+      <c r="C133">
+        <v>4240.498957073307</v>
+      </c>
+      <c r="D133">
+        <v>2799.802017040321</v>
+      </c>
+      <c r="E133">
+        <v>3370.629266244694</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B134" t="s">
+        <v>188</v>
+      </c>
+      <c r="C134">
+        <v>3104.11640049039</v>
+      </c>
+      <c r="D134">
+        <v>2945.585161856526</v>
+      </c>
+      <c r="E134">
+        <v>3032.000269374993</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B135" t="s">
+        <v>188</v>
+      </c>
+      <c r="C135">
+        <v>4758.923090909089</v>
+      </c>
+      <c r="D135">
+        <v>4052.36859619171</v>
+      </c>
+      <c r="E135">
+        <v>4241.271500156832</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136" t="s">
+        <v>188</v>
+      </c>
+      <c r="C136">
+        <v>4582.423026269129</v>
+      </c>
+      <c r="D136">
+        <v>3677.660725632635</v>
+      </c>
+      <c r="E136">
+        <v>3936.041511138754</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B137" t="s">
+        <v>188</v>
+      </c>
+      <c r="C137">
+        <v>8274.311032145955</v>
+      </c>
+      <c r="D137">
+        <v>4554.906523253632</v>
+      </c>
+      <c r="E137">
+        <v>6530.74208924048</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B138" t="s">
+        <v>188</v>
+      </c>
+      <c r="C138">
+        <v>2362.496887971177</v>
+      </c>
+      <c r="D138">
+        <v>4552.94161730676</v>
+      </c>
+      <c r="E138">
+        <v>7699.768813994026</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B139" t="s">
+        <v>188</v>
+      </c>
+      <c r="C139">
+        <v>1764.352253203638</v>
+      </c>
+      <c r="D139">
+        <v>974.5725435688446</v>
+      </c>
+      <c r="E139">
+        <v>1393.90973989574</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B140" t="s">
+        <v>188</v>
+      </c>
+      <c r="C140">
+        <v>921.2368963564281</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B141" t="s">
+        <v>188</v>
+      </c>
+      <c r="C141">
+        <v>409436.7691592983</v>
+      </c>
+      <c r="D141">
+        <v>355341.7534723968</v>
+      </c>
+      <c r="E141">
+        <v>387999.3260030203</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B142" t="s">
+        <v>188</v>
+      </c>
+      <c r="C142">
+        <v>66424.65479531829</v>
+      </c>
+      <c r="D142">
+        <v>67311.96044664056</v>
+      </c>
+      <c r="E142">
+        <v>76231.77993843338</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B143" t="s">
+        <v>188</v>
+      </c>
+      <c r="C143">
+        <v>125858.7401545331</v>
+      </c>
+      <c r="D143">
+        <v>95923.88790038624</v>
+      </c>
+      <c r="E143">
+        <v>124140.5773429784</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144" t="s">
+        <v>188</v>
+      </c>
+      <c r="C144">
+        <v>55158.37308241575</v>
+      </c>
+      <c r="D144">
+        <v>54194.17670445503</v>
+      </c>
+      <c r="E144">
+        <v>54731.6463609033</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145" t="s">
+        <v>188</v>
+      </c>
+      <c r="C145">
+        <v>18810.64774314864</v>
+      </c>
+      <c r="D145">
+        <v>26985.75868185313</v>
+      </c>
+      <c r="E145">
+        <v>33814.25416223275</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B146" t="s">
+        <v>188</v>
+      </c>
+      <c r="C146">
+        <v>11786.58854248258</v>
+      </c>
+      <c r="D146">
+        <v>9267.503482344102</v>
+      </c>
+      <c r="E146">
+        <v>10151.93626108859</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B147" t="s">
+        <v>188</v>
+      </c>
+      <c r="C147">
+        <v>41809.31820607139</v>
+      </c>
+      <c r="D147">
+        <v>39732.01918427406</v>
+      </c>
+      <c r="E147">
+        <v>46033.76592047335</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B148" t="s">
+        <v>188</v>
+      </c>
+      <c r="C148">
+        <v>44322.79570608526</v>
+      </c>
+      <c r="D148">
+        <v>42997.62304068729</v>
+      </c>
+      <c r="E148">
+        <v>49150.09462369821</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B149" t="s">
+        <v>188</v>
+      </c>
+      <c r="C149">
+        <v>7830.871226366395</v>
+      </c>
+      <c r="D149">
+        <v>5653.095564499369</v>
+      </c>
+      <c r="E149">
+        <v>6625.371912088781</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B150" t="s">
+        <v>188</v>
+      </c>
+      <c r="C150">
+        <v>8817.535269776827</v>
+      </c>
+      <c r="D150">
+        <v>9011.059942949789</v>
+      </c>
+      <c r="E150">
+        <v>10838.71267389012</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B151" t="s">
+        <v>188</v>
+      </c>
+      <c r="C151">
+        <v>15730.7337703995</v>
+      </c>
+      <c r="D151">
+        <v>12870.92751701806</v>
+      </c>
+      <c r="E151">
+        <v>16028.57827823479</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152" t="s">
+        <v>188</v>
+      </c>
+      <c r="C152">
+        <v>14763.70638988416</v>
+      </c>
+      <c r="D152">
+        <v>11353.82086139094</v>
+      </c>
+      <c r="E152">
+        <v>15744.22408353954</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B153" t="s">
+        <v>188</v>
+      </c>
+      <c r="C153">
+        <v>2664.581838046233</v>
+      </c>
+      <c r="D153">
+        <v>2118.88338047299</v>
+      </c>
+      <c r="E153">
+        <v>2317.74860784036</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B154" t="s">
+        <v>188</v>
+      </c>
+      <c r="C154">
+        <v>7118.299388486004</v>
+      </c>
+      <c r="D154">
+        <v>4387.796042371227</v>
+      </c>
+      <c r="E154">
+        <v>6214.950571608244</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B155" t="s">
+        <v>188</v>
+      </c>
+      <c r="C155">
+        <v>1256.930682890124</v>
+      </c>
+      <c r="D155">
+        <v>634.2799162905493</v>
+      </c>
+      <c r="E155">
+        <v>1060.520130278657</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B156" t="s">
+        <v>188</v>
+      </c>
+      <c r="C156">
+        <v>3104.11640049039</v>
+      </c>
+      <c r="D156">
+        <v>2953.473502833881</v>
+      </c>
+      <c r="E156">
+        <v>3032.074436227733</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B157" t="s">
+        <v>188</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>1927.316250691574</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B158" t="s">
+        <v>188</v>
+      </c>
+      <c r="C158">
+        <v>4982.658106436934</v>
+      </c>
+      <c r="D158">
+        <v>3682.745087885083</v>
+      </c>
+      <c r="E158">
+        <v>4606.149113368056</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B159" t="s">
+        <v>188</v>
+      </c>
+      <c r="C159">
+        <v>9858.7475739898</v>
+      </c>
+      <c r="D159">
+        <v>4988.549100871839</v>
+      </c>
+      <c r="E159">
+        <v>9051.622561655677</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B160" t="s">
+        <v>188</v>
+      </c>
+      <c r="C160">
+        <v>3049.962402814945</v>
+      </c>
+      <c r="D160">
+        <v>7885.799173422068</v>
+      </c>
+      <c r="E160">
+        <v>14476.78741030169</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B161" t="s">
+        <v>188</v>
+      </c>
+      <c r="C161">
+        <v>1932.537890358078</v>
+      </c>
+      <c r="D161">
+        <v>1092.439628676345</v>
+      </c>
+      <c r="E161">
+        <v>1729.767824059069</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B162" t="s">
+        <v>188</v>
+      </c>
+      <c r="C162">
+        <v>927.0527858536279</v>
+      </c>
+      <c r="D162">
+        <v>885.4644642160963</v>
+      </c>
+      <c r="E162">
+        <v>854.6967352460968</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B163" t="s">
+        <v>188</v>
+      </c>
+      <c r="C163">
+        <v>425667.2304377211</v>
+      </c>
+      <c r="D163">
+        <v>379452.4458343688</v>
+      </c>
+      <c r="E163">
+        <v>422462.404769241</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B164" t="s">
+        <v>188</v>
+      </c>
+      <c r="C164">
+        <v>74824.1776942108</v>
+      </c>
+      <c r="D164">
+        <v>75532.04105321791</v>
+      </c>
+      <c r="E164">
+        <v>86492.52473873404</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B165" t="s">
+        <v>188</v>
+      </c>
+      <c r="C165">
+        <v>128549.8642605276</v>
+      </c>
+      <c r="D165">
+        <v>114702.4949950556</v>
+      </c>
+      <c r="E165">
+        <v>134200.4554046213</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B166" t="s">
+        <v>188</v>
+      </c>
+      <c r="C166">
+        <v>55242.88725228325</v>
+      </c>
+      <c r="D166">
+        <v>54348.67956945477</v>
+      </c>
+      <c r="E166">
+        <v>54823.8158790419</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B167" t="s">
+        <v>188</v>
+      </c>
+      <c r="C167">
+        <v>21186.42152206995</v>
+      </c>
+      <c r="D167">
+        <v>32192.86399794241</v>
+      </c>
+      <c r="E167">
+        <v>40091.29523030741</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B168" t="s">
+        <v>188</v>
+      </c>
+      <c r="C168">
+        <v>12108.98627481771</v>
+      </c>
+      <c r="D168">
+        <v>9710.044517252907</v>
+      </c>
+      <c r="E168">
+        <v>9820.712234959921</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B169" t="s">
+        <v>188</v>
+      </c>
+      <c r="C169">
+        <v>44818.4592191087</v>
+      </c>
+      <c r="D169">
+        <v>43318.43942297382</v>
+      </c>
+      <c r="E169">
+        <v>50430.2444258372</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B170" t="s">
+        <v>188</v>
+      </c>
+      <c r="C170">
+        <v>45410.20682375576</v>
+      </c>
+      <c r="D170">
+        <v>44140.29328236685</v>
+      </c>
+      <c r="E170">
+        <v>50777.920807722</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B171" t="s">
+        <v>188</v>
+      </c>
+      <c r="C171">
+        <v>7877.356799130208</v>
+      </c>
+      <c r="D171">
+        <v>5653.095564499369</v>
+      </c>
+      <c r="E171">
+        <v>6662.276843942194</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B172" t="s">
+        <v>188</v>
+      </c>
+      <c r="C172">
+        <v>7081.366168574467</v>
+      </c>
+      <c r="D172">
+        <v>7237.854347805022</v>
+      </c>
+      <c r="E172">
+        <v>8761.01660377788</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B173" t="s">
+        <v>188</v>
+      </c>
+      <c r="C173">
+        <v>17240.04215367412</v>
+      </c>
+      <c r="D173">
+        <v>13942.82778271549</v>
+      </c>
+      <c r="E173">
+        <v>14713.17492592106</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B174" t="s">
+        <v>188</v>
+      </c>
+      <c r="C174">
+        <v>17324.03456184319</v>
+      </c>
+      <c r="D174">
+        <v>13476.54727078326</v>
+      </c>
+      <c r="E174">
+        <v>22628.13038686703</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B175" t="s">
+        <v>188</v>
+      </c>
+      <c r="C175">
+        <v>2689.033001442709</v>
+      </c>
+      <c r="D175">
+        <v>2118.88338047299</v>
+      </c>
+      <c r="E175">
+        <v>2326.478289412053</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B176" t="s">
+        <v>188</v>
+      </c>
+      <c r="C176">
+        <v>7330.001934671265</v>
+      </c>
+      <c r="D176">
+        <v>4696.892936408833</v>
+      </c>
+      <c r="E176">
+        <v>6336.909947377137</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B177" t="s">
+        <v>188</v>
+      </c>
+      <c r="C177">
+        <v>3666.34991690552</v>
+      </c>
+      <c r="D177">
+        <v>2659.16265449915</v>
+      </c>
+      <c r="E177">
+        <v>3251.428044629679</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B178" t="s">
+        <v>188</v>
+      </c>
+      <c r="C178">
+        <v>3110.615608057638</v>
+      </c>
+      <c r="D178">
+        <v>2966.871688417814</v>
+      </c>
+      <c r="E178">
+        <v>3044.077493176301</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B179" t="s">
+        <v>188</v>
+      </c>
+      <c r="C179">
+        <v>4955.203939982344</v>
+      </c>
+      <c r="D179">
+        <v>4437.491921939725</v>
+      </c>
+      <c r="E179">
+        <v>4802.656681354792</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B180" t="s">
+        <v>188</v>
+      </c>
+      <c r="C180">
+        <v>5584.532853170555</v>
+      </c>
+      <c r="D180">
+        <v>3696.358431113311</v>
+      </c>
+      <c r="E180">
+        <v>5041.150517084573</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B181" t="s">
+        <v>188</v>
+      </c>
+      <c r="C181">
+        <v>12228.85287007065</v>
+      </c>
+      <c r="D181">
+        <v>5315.793599021267</v>
+      </c>
+      <c r="E181">
+        <v>10793.64798057903</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B182" t="s">
+        <v>188</v>
+      </c>
+      <c r="C182">
+        <v>3909.407627315059</v>
+      </c>
+      <c r="D182">
+        <v>12148.67547071851</v>
+      </c>
+      <c r="E182">
+        <v>24644.07599310096</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B183" t="s">
+        <v>188</v>
+      </c>
+      <c r="C183">
+        <v>2078.961774546943</v>
+      </c>
+      <c r="D183">
+        <v>1179.897477494976</v>
+      </c>
+      <c r="E183">
+        <v>1832.168256550158</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B184" t="s">
+        <v>188</v>
+      </c>
+      <c r="C184">
+        <v>932.8686753508275</v>
+      </c>
+      <c r="D184">
+        <v>920.6062716110156</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add_students_by_BaseProjections function
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df.xlsx
+++ b/create_forecast_basic/utils/monitoring_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="229">
   <si>
     <t>2020</t>
   </si>
@@ -575,6 +575,78 @@
   </si>
   <si>
     <t>SCHOOLDIST_8_2050</t>
+  </si>
+  <si>
+    <t>BaseProjections_2025</t>
+  </si>
+  <si>
+    <t>BaseProjections_2030</t>
+  </si>
+  <si>
+    <t>BaseProjections_2035</t>
+  </si>
+  <si>
+    <t>BaseProjections_2040</t>
+  </si>
+  <si>
+    <t>BaseProjections_2045</t>
+  </si>
+  <si>
+    <t>BaseProjections_2050</t>
+  </si>
+  <si>
+    <t>BaseProjections_2025_age5_9</t>
+  </si>
+  <si>
+    <t>BaseProjections_2030_age5_9</t>
+  </si>
+  <si>
+    <t>BaseProjections_2035_age5_9</t>
+  </si>
+  <si>
+    <t>BaseProjections_2040_age5_9</t>
+  </si>
+  <si>
+    <t>BaseProjections_2045_age5_9</t>
+  </si>
+  <si>
+    <t>BaseProjections_2050_age5_9</t>
+  </si>
+  <si>
+    <t>BaseProjections_2025_age10_14</t>
+  </si>
+  <si>
+    <t>BaseProjections_2030_age10_14</t>
+  </si>
+  <si>
+    <t>BaseProjections_2035_age10_14</t>
+  </si>
+  <si>
+    <t>BaseProjections_2040_age10_14</t>
+  </si>
+  <si>
+    <t>BaseProjections_2045_age10_14</t>
+  </si>
+  <si>
+    <t>BaseProjections_2050_age10_14</t>
+  </si>
+  <si>
+    <t>BaseProjections_2025_age15_19</t>
+  </si>
+  <si>
+    <t>BaseProjections_2030_age15_19</t>
+  </si>
+  <si>
+    <t>BaseProjections_2035_age15_19</t>
+  </si>
+  <si>
+    <t>BaseProjections_2040_age15_19</t>
+  </si>
+  <si>
+    <t>BaseProjections_2045_age15_19</t>
+  </si>
+  <si>
+    <t>BaseProjections_2050_age15_19</t>
   </si>
   <si>
     <t>1,758,461</t>
@@ -986,7 +1058,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1011,16 +1083,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="E2" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1028,16 +1100,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="E3" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1045,16 +1117,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1062,16 +1134,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1164,16 +1236,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1181,16 +1253,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1198,16 +1270,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1215,16 +1287,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="E14" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1232,16 +1304,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="D15" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="E15" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1249,16 +1321,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="E16" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1419,7 +1491,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C26">
         <v>288</v>
@@ -1436,7 +1508,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C27">
         <v>110</v>
@@ -1453,7 +1525,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C28">
         <v>109</v>
@@ -1470,7 +1542,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C29">
         <v>109</v>
@@ -1487,7 +1559,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C30">
         <v>94</v>
@@ -1878,7 +1950,7 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C53">
         <v>285733.3218235314</v>
@@ -1895,7 +1967,7 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C54">
         <v>36057.66373063793</v>
@@ -1912,7 +1984,7 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C55">
         <v>66822.51137331135</v>
@@ -1929,7 +2001,7 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C56">
         <v>33156.30459804353</v>
@@ -1946,7 +2018,7 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C57">
         <v>9986.417617537509</v>
@@ -1963,7 +2035,7 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C58">
         <v>8306.813376518987</v>
@@ -1980,7 +2052,7 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C59">
         <v>29427.44116169451</v>
@@ -1997,7 +2069,7 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C60">
         <v>37145.33462606892</v>
@@ -2014,7 +2086,7 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C61">
         <v>5309.478782988256</v>
@@ -2031,7 +2103,7 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C62">
         <v>5521.895631861405</v>
@@ -2048,7 +2120,7 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C63">
         <v>7012.74256878429</v>
@@ -2065,7 +2137,7 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C64">
         <v>7317.313641591267</v>
@@ -2082,7 +2154,7 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C65">
         <v>2166.404734331622</v>
@@ -2099,7 +2171,7 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C66">
         <v>3081.965248662672</v>
@@ -2116,7 +2188,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C67">
         <v>443.1341918519325</v>
@@ -2133,7 +2205,7 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C68">
         <v>2895.085614458657</v>
@@ -2150,7 +2222,7 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C69">
         <v>3653.831655445544</v>
@@ -2167,7 +2239,7 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C70">
         <v>3542.454003930634</v>
@@ -2184,7 +2256,7 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C71">
         <v>4257.401768859199</v>
@@ -2201,7 +2273,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C72">
         <v>881.1481005457115</v>
@@ -2218,7 +2290,7 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C73">
         <v>911.7413777070067</v>
@@ -2235,7 +2307,7 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2252,7 +2324,7 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C75">
         <v>310887.0551086462</v>
@@ -2269,7 +2341,7 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C76">
         <v>51074.32436027069</v>
@@ -2286,7 +2358,7 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C77">
         <v>84109.82719823082</v>
@@ -2303,7 +2375,7 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C78">
         <v>39310.49274971832</v>
@@ -2320,7 +2392,7 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C79">
         <v>11932.38400809033</v>
@@ -2337,7 +2409,7 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C80">
         <v>9548.28031721313</v>
@@ -2354,7 +2426,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C81">
         <v>35810.66989709945</v>
@@ -2371,7 +2443,7 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C82">
         <v>40274.91199119319</v>
@@ -2388,7 +2460,7 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C83">
         <v>5702.582508173264</v>
@@ -2405,7 +2477,7 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C84">
         <v>6531.454941380145</v>
@@ -2422,7 +2494,7 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C85">
         <v>11086.07248419944</v>
@@ -2439,7 +2511,7 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C86">
         <v>11235.01770760014</v>
@@ -2456,7 +2528,7 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C87">
         <v>2313.18743770475</v>
@@ -2473,7 +2545,7 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C88">
         <v>4487.422497745161</v>
@@ -2490,7 +2562,7 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C89">
         <v>3291.571394333075</v>
@@ -2507,7 +2579,7 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C90">
         <v>2962.271032197586</v>
@@ -2524,7 +2596,7 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C91">
         <v>3978.851277647058</v>
@@ -2541,7 +2613,7 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C92">
         <v>3624.875154413226</v>
@@ -2558,7 +2630,7 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C93">
         <v>4499.453713305816</v>
@@ -2575,7 +2647,7 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C94">
         <v>1176.375213333053</v>
@@ -2592,7 +2664,7 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C95">
         <v>1013.219479989464</v>
@@ -2609,7 +2681,7 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C96">
         <v>857.2621118872319</v>
@@ -2626,7 +2698,7 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C97">
         <v>345179.8540918057</v>
@@ -2643,7 +2715,7 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C98">
         <v>57843.05696310467</v>
@@ -2660,7 +2732,7 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C99">
         <v>106400.8113634808</v>
@@ -2677,7 +2749,7 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C100">
         <v>47754.67592555143</v>
@@ -2694,7 +2766,7 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C101">
         <v>13642.04328300475</v>
@@ -2711,7 +2783,7 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C102">
         <v>10166.68671320246</v>
@@ -2728,7 +2800,7 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C103">
         <v>40056.29615048355</v>
@@ -2745,7 +2817,7 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C104">
         <v>42099.78280750295</v>
@@ -2762,7 +2834,7 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C105">
         <v>6780.581746217548</v>
@@ -2779,7 +2851,7 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C106">
         <v>7052.041776574091</v>
@@ -2796,7 +2868,7 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C107">
         <v>12491.64080553533</v>
@@ -2813,7 +2885,7 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C108">
         <v>11918.07029478611</v>
@@ -2830,7 +2902,7 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C109">
         <v>2510.791313969085</v>
@@ -2847,7 +2919,7 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C110">
         <v>5559.189168957029</v>
@@ -2864,7 +2936,7 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C111">
         <v>3740.698985412615</v>
@@ -2881,7 +2953,7 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C112">
         <v>3025.982972811596</v>
@@ -2898,7 +2970,7 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C113">
         <v>4384.134004159239</v>
@@ -2915,7 +2987,7 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C114">
         <v>3818.113674370041</v>
@@ -2932,7 +3004,7 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C115">
         <v>5697.549039481555</v>
@@ -2949,7 +3021,7 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C116">
         <v>1675.03137312741</v>
@@ -2966,7 +3038,7 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C117">
         <v>1388.615296125427</v>
@@ -2983,7 +3055,7 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C118">
         <v>915.4210068592286</v>
@@ -3000,7 +3072,7 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C119">
         <v>379833.2126030341</v>
@@ -3017,7 +3089,7 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C120">
         <v>66636.46327624648</v>
@@ -3034,7 +3106,7 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C121">
         <v>122447.4212601383</v>
@@ -3051,7 +3123,7 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C122">
         <v>55098.14072490651</v>
@@ -3068,7 +3140,7 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C123">
         <v>17436.20392355449</v>
@@ -3085,7 +3157,7 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C124">
         <v>11477.1443269179</v>
@@ -3102,7 +3174,7 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C125">
         <v>44788.85407568982</v>
@@ -3119,7 +3191,7 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C126">
         <v>43854.83257609577</v>
@@ -3136,7 +3208,7 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C127">
         <v>7818.02330571639</v>
@@ -3153,7 +3225,7 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C128">
         <v>8085.182658295945</v>
@@ -3170,7 +3242,7 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C129">
         <v>14492.94704346139</v>
@@ -3187,7 +3259,7 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C130">
         <v>14025.08468897277</v>
@@ -3204,7 +3276,7 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C131">
         <v>2660.082565212768</v>
@@ -3221,7 +3293,7 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C132">
         <v>6699.919359426849</v>
@@ -3238,7 +3310,7 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C133">
         <v>4240.498957073307</v>
@@ -3255,7 +3327,7 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C134">
         <v>3104.11640049039</v>
@@ -3272,7 +3344,7 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C135">
         <v>4758.923090909089</v>
@@ -3289,7 +3361,7 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C136">
         <v>4582.423026269129</v>
@@ -3306,7 +3378,7 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C137">
         <v>8274.311032145955</v>
@@ -3323,7 +3395,7 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C138">
         <v>2362.496887971177</v>
@@ -3340,7 +3412,7 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C139">
         <v>1764.352253203638</v>
@@ -3357,7 +3429,7 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C140">
         <v>921.2368963564281</v>
@@ -3374,7 +3446,7 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C141">
         <v>409436.7691592983</v>
@@ -3391,7 +3463,7 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C142">
         <v>66424.65479531829</v>
@@ -3408,7 +3480,7 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C143">
         <v>125858.7401545331</v>
@@ -3425,7 +3497,7 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C144">
         <v>55158.37308241575</v>
@@ -3442,7 +3514,7 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C145">
         <v>18810.64774314864</v>
@@ -3459,7 +3531,7 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C146">
         <v>11786.58854248258</v>
@@ -3476,7 +3548,7 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C147">
         <v>41809.31820607139</v>
@@ -3493,7 +3565,7 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C148">
         <v>44322.79570608526</v>
@@ -3510,7 +3582,7 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C149">
         <v>7830.871226366395</v>
@@ -3527,7 +3599,7 @@
         <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C150">
         <v>8817.535269776827</v>
@@ -3544,7 +3616,7 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C151">
         <v>15730.7337703995</v>
@@ -3561,7 +3633,7 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C152">
         <v>14763.70638988416</v>
@@ -3578,7 +3650,7 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C153">
         <v>2664.581838046233</v>
@@ -3595,7 +3667,7 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C154">
         <v>7118.299388486004</v>
@@ -3612,7 +3684,7 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C155">
         <v>1256.930682890124</v>
@@ -3629,7 +3701,7 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C156">
         <v>3104.11640049039</v>
@@ -3646,7 +3718,7 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -3663,7 +3735,7 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C158">
         <v>4982.658106436934</v>
@@ -3680,7 +3752,7 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C159">
         <v>9858.7475739898</v>
@@ -3697,7 +3769,7 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C160">
         <v>3049.962402814945</v>
@@ -3714,7 +3786,7 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C161">
         <v>1932.537890358078</v>
@@ -3731,7 +3803,7 @@
         <v>164</v>
       </c>
       <c r="B162" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C162">
         <v>927.0527858536279</v>
@@ -3748,7 +3820,7 @@
         <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C163">
         <v>425667.2304377211</v>
@@ -3765,7 +3837,7 @@
         <v>166</v>
       </c>
       <c r="B164" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C164">
         <v>74824.1776942108</v>
@@ -3782,7 +3854,7 @@
         <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C165">
         <v>128549.8642605276</v>
@@ -3799,7 +3871,7 @@
         <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C166">
         <v>55242.88725228325</v>
@@ -3816,7 +3888,7 @@
         <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C167">
         <v>21186.42152206995</v>
@@ -3833,7 +3905,7 @@
         <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C168">
         <v>12108.98627481771</v>
@@ -3850,7 +3922,7 @@
         <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C169">
         <v>44818.4592191087</v>
@@ -3867,7 +3939,7 @@
         <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C170">
         <v>45410.20682375576</v>
@@ -3884,7 +3956,7 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C171">
         <v>7877.356799130208</v>
@@ -3901,7 +3973,7 @@
         <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C172">
         <v>7081.366168574467</v>
@@ -3918,7 +3990,7 @@
         <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C173">
         <v>17240.04215367412</v>
@@ -3935,7 +4007,7 @@
         <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C174">
         <v>17324.03456184319</v>
@@ -3952,7 +4024,7 @@
         <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C175">
         <v>2689.033001442709</v>
@@ -3969,7 +4041,7 @@
         <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C176">
         <v>7330.001934671265</v>
@@ -3986,7 +4058,7 @@
         <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C177">
         <v>3666.34991690552</v>
@@ -4003,7 +4075,7 @@
         <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C178">
         <v>3110.615608057638</v>
@@ -4020,7 +4092,7 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C179">
         <v>4955.203939982344</v>
@@ -4037,7 +4109,7 @@
         <v>182</v>
       </c>
       <c r="B180" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C180">
         <v>5584.532853170555</v>
@@ -4054,7 +4126,7 @@
         <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C181">
         <v>12228.85287007065</v>
@@ -4071,7 +4143,7 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C182">
         <v>3909.407627315059</v>
@@ -4088,7 +4160,7 @@
         <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C183">
         <v>2078.961774546943</v>
@@ -4105,7 +4177,7 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C184">
         <v>932.8686753508275</v>
@@ -4115,6 +4187,414 @@
       </c>
       <c r="E184">
         <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B185" t="s">
+        <v>212</v>
+      </c>
+      <c r="C185">
+        <v>195705.6</v>
+      </c>
+      <c r="D185">
+        <v>184867.2</v>
+      </c>
+      <c r="E185">
+        <v>187784</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B186" t="s">
+        <v>212</v>
+      </c>
+      <c r="C186">
+        <v>223624</v>
+      </c>
+      <c r="D186">
+        <v>205627.2</v>
+      </c>
+      <c r="E186">
+        <v>214700.8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B187" t="s">
+        <v>212</v>
+      </c>
+      <c r="C187">
+        <v>253637.6</v>
+      </c>
+      <c r="D187">
+        <v>224994.4</v>
+      </c>
+      <c r="E187">
+        <v>242126.4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B188" t="s">
+        <v>212</v>
+      </c>
+      <c r="C188">
+        <v>284854.4</v>
+      </c>
+      <c r="D188">
+        <v>242956.8</v>
+      </c>
+      <c r="E188">
+        <v>270748</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B189" t="s">
+        <v>212</v>
+      </c>
+      <c r="C189">
+        <v>275764.8</v>
+      </c>
+      <c r="D189">
+        <v>258018.4</v>
+      </c>
+      <c r="E189">
+        <v>296766.4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B190" t="s">
+        <v>212</v>
+      </c>
+      <c r="C190">
+        <v>285775.2</v>
+      </c>
+      <c r="D190">
+        <v>276530.4</v>
+      </c>
+      <c r="E190">
+        <v>326134.4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B191" t="s">
+        <v>212</v>
+      </c>
+      <c r="C191">
+        <v>195705.6</v>
+      </c>
+      <c r="D191">
+        <v>184867.2</v>
+      </c>
+      <c r="E191">
+        <v>187784</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B192" t="s">
+        <v>212</v>
+      </c>
+      <c r="C192">
+        <v>223624</v>
+      </c>
+      <c r="D192">
+        <v>205627.2</v>
+      </c>
+      <c r="E192">
+        <v>214700.8</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B193" t="s">
+        <v>212</v>
+      </c>
+      <c r="C193">
+        <v>253637.6</v>
+      </c>
+      <c r="D193">
+        <v>224994.4</v>
+      </c>
+      <c r="E193">
+        <v>242126.4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B194" t="s">
+        <v>212</v>
+      </c>
+      <c r="C194">
+        <v>284854.4</v>
+      </c>
+      <c r="D194">
+        <v>242956.8</v>
+      </c>
+      <c r="E194">
+        <v>270748</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B195" t="s">
+        <v>212</v>
+      </c>
+      <c r="C195">
+        <v>275764.8</v>
+      </c>
+      <c r="D195">
+        <v>258018.4</v>
+      </c>
+      <c r="E195">
+        <v>296766.4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B196" t="s">
+        <v>212</v>
+      </c>
+      <c r="C196">
+        <v>285775.2</v>
+      </c>
+      <c r="D196">
+        <v>276530.4</v>
+      </c>
+      <c r="E196">
+        <v>326134.4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B197" t="s">
+        <v>212</v>
+      </c>
+      <c r="C197">
+        <v>181481.6</v>
+      </c>
+      <c r="D197">
+        <v>171418.4</v>
+      </c>
+      <c r="E197">
+        <v>173696</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B198" t="s">
+        <v>212</v>
+      </c>
+      <c r="C198">
+        <v>206952</v>
+      </c>
+      <c r="D198">
+        <v>183019.2</v>
+      </c>
+      <c r="E198">
+        <v>189584.8</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B199" t="s">
+        <v>212</v>
+      </c>
+      <c r="C199">
+        <v>236529.6</v>
+      </c>
+      <c r="D199">
+        <v>204145.6</v>
+      </c>
+      <c r="E199">
+        <v>217076.8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B200" t="s">
+        <v>212</v>
+      </c>
+      <c r="C200">
+        <v>266166.4</v>
+      </c>
+      <c r="D200">
+        <v>221178.4</v>
+      </c>
+      <c r="E200">
+        <v>243465.6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B201" t="s">
+        <v>212</v>
+      </c>
+      <c r="C201">
+        <v>266616</v>
+      </c>
+      <c r="D201">
+        <v>234677.6</v>
+      </c>
+      <c r="E201">
+        <v>267149.6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" t="s">
+        <v>212</v>
+      </c>
+      <c r="C202">
+        <v>275787.2</v>
+      </c>
+      <c r="D202">
+        <v>252004</v>
+      </c>
+      <c r="E202">
+        <v>295416</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B203" t="s">
+        <v>212</v>
+      </c>
+      <c r="C203">
+        <v>166797.6</v>
+      </c>
+      <c r="D203">
+        <v>173032.8</v>
+      </c>
+      <c r="E203">
+        <v>175456.8</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B204" t="s">
+        <v>212</v>
+      </c>
+      <c r="C204">
+        <v>187860.8</v>
+      </c>
+      <c r="D204">
+        <v>192721.6</v>
+      </c>
+      <c r="E204">
+        <v>199666.4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" t="s">
+        <v>212</v>
+      </c>
+      <c r="C205">
+        <v>214399.2</v>
+      </c>
+      <c r="D205">
+        <v>208928.8</v>
+      </c>
+      <c r="E205">
+        <v>221102.4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206" t="s">
+        <v>212</v>
+      </c>
+      <c r="C206">
+        <v>240393.6</v>
+      </c>
+      <c r="D206">
+        <v>232657.6</v>
+      </c>
+      <c r="E206">
+        <v>254091.2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B207" t="s">
+        <v>212</v>
+      </c>
+      <c r="C207">
+        <v>266132</v>
+      </c>
+      <c r="D207">
+        <v>251892</v>
+      </c>
+      <c r="E207">
+        <v>284350.4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B208" t="s">
+        <v>212</v>
+      </c>
+      <c r="C208">
+        <v>277836.8</v>
+      </c>
+      <c r="D208">
+        <v>271554.4</v>
+      </c>
+      <c r="E208">
+        <v>316714.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add_percentage_growth_row: percentage growth univ
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df.xlsx
+++ b/create_forecast_basic/utils/monitoring_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="228">
   <si>
     <t>2020</t>
   </si>
@@ -100,19 +100,34 @@
     <t>taz_num_count</t>
   </si>
   <si>
-    <t>percentage growth 2020-2025</t>
-  </si>
-  <si>
-    <t>percentage growth 2025-2030</t>
-  </si>
-  <si>
-    <t>percentage growth 2030-2035</t>
-  </si>
-  <si>
-    <t>percentage growth 2035-2040</t>
-  </si>
-  <si>
-    <t>percentage growth 2045-2050</t>
+    <t>percentage growth pop 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth pop 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth pop 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth pop 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth pop 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth univ 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth univ 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth univ 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth univ 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth univ 2045-2050</t>
   </si>
   <si>
     <t>SCHOOLDIST_5_2020</t>
@@ -575,24 +590,6 @@
   </si>
   <si>
     <t>SCHOOLDIST_8_2050</t>
-  </si>
-  <si>
-    <t>BaseProjections_2025</t>
-  </si>
-  <si>
-    <t>BaseProjections_2030</t>
-  </si>
-  <si>
-    <t>BaseProjections_2035</t>
-  </si>
-  <si>
-    <t>BaseProjections_2040</t>
-  </si>
-  <si>
-    <t>BaseProjections_2045</t>
-  </si>
-  <si>
-    <t>BaseProjections_2050</t>
   </si>
   <si>
     <t>BaseProjections_2025_age5_9</t>
@@ -1058,7 +1055,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E208"/>
+  <dimension ref="A1:E207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1083,16 +1080,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1100,16 +1097,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1117,16 +1114,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1134,16 +1131,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1236,16 +1233,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1253,16 +1250,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1270,16 +1267,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1287,16 +1284,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1304,16 +1301,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1321,16 +1318,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1491,7 +1488,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C26">
         <v>288</v>
@@ -1508,7 +1505,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C27">
         <v>110</v>
@@ -1525,7 +1522,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C28">
         <v>109</v>
@@ -1542,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C29">
         <v>109</v>
@@ -1559,7 +1556,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C30">
         <v>94</v>
@@ -1575,85 +1572,85 @@
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B31">
-        <v>213239.3333333333</v>
+      <c r="B31" t="s">
+        <v>211</v>
       </c>
       <c r="C31">
-        <v>213239.3333333333</v>
+        <v>100</v>
       </c>
       <c r="D31">
-        <v>213239.3333333333</v>
+        <v>100</v>
       </c>
       <c r="E31">
-        <v>213239.3333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B32">
-        <v>28627.66666666667</v>
+      <c r="B32" t="s">
+        <v>211</v>
       </c>
       <c r="C32">
-        <v>28627.66666666667</v>
+        <v>100</v>
       </c>
       <c r="D32">
-        <v>28627.66666666667</v>
+        <v>100</v>
       </c>
       <c r="E32">
-        <v>28627.66666666667</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B33">
-        <v>46063</v>
+      <c r="B33" t="s">
+        <v>211</v>
       </c>
       <c r="C33">
-        <v>46063</v>
+        <v>100</v>
       </c>
       <c r="D33">
-        <v>46063</v>
+        <v>100</v>
       </c>
       <c r="E33">
-        <v>46063</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B34">
-        <v>23828</v>
+      <c r="B34" t="s">
+        <v>211</v>
       </c>
       <c r="C34">
-        <v>23828</v>
+        <v>100</v>
       </c>
       <c r="D34">
-        <v>23828</v>
+        <v>100</v>
       </c>
       <c r="E34">
-        <v>23828</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35">
-        <v>8538</v>
+      <c r="B35" t="s">
+        <v>211</v>
       </c>
       <c r="C35">
-        <v>8538</v>
+        <v>100</v>
       </c>
       <c r="D35">
-        <v>8538</v>
+        <v>100</v>
       </c>
       <c r="E35">
-        <v>8538</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1661,16 +1658,16 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="C36">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="D36">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="E36">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1678,16 +1675,16 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>21988.00000000001</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="C37">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="D37">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="E37">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1695,16 +1692,16 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="C38">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="D38">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="E38">
-        <v>27262</v>
+        <v>46063</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1712,16 +1709,16 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="C39">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="D39">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="E39">
-        <v>2804</v>
+        <v>23828</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1729,16 +1726,16 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="C40">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="D40">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="E40">
-        <v>1331</v>
+        <v>8538</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1746,16 +1743,16 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="C41">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="D41">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="E41">
-        <v>7375</v>
+        <v>5048</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1763,16 +1760,16 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>8805</v>
+        <v>21988.00000000001</v>
       </c>
       <c r="C42">
-        <v>8805</v>
+        <v>21988</v>
       </c>
       <c r="D42">
-        <v>8805</v>
+        <v>21988</v>
       </c>
       <c r="E42">
-        <v>8805</v>
+        <v>21988</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1780,16 +1777,16 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="C43">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="D43">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="E43">
-        <v>1218</v>
+        <v>27262</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1797,16 +1794,16 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="C44">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="D44">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="E44">
-        <v>1673</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1814,16 +1811,16 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="C45">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="D45">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="E45">
-        <v>2401</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1831,16 +1828,16 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="C46">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="D46">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="E46">
-        <v>2488</v>
+        <v>7375</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1848,16 +1845,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="C47">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="D47">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="E47">
-        <v>2148</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1865,16 +1862,16 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="C48">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="D48">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="E48">
-        <v>3242</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1882,16 +1879,16 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="C49">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="D49">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="E49">
-        <v>3637</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1899,16 +1896,16 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="C50">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="D50">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="E50">
-        <v>301</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1916,16 +1913,16 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="C51">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="D51">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="E51">
-        <v>537</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1933,101 +1930,101 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="C52">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="D52">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="E52">
-        <v>300</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B53" t="s">
-        <v>212</v>
+      <c r="B53">
+        <v>3242</v>
       </c>
       <c r="C53">
-        <v>285733.3218235314</v>
+        <v>3242</v>
       </c>
       <c r="D53">
-        <v>274161.0000038777</v>
+        <v>3242</v>
       </c>
       <c r="E53">
-        <v>275663.3373324008</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B54" t="s">
-        <v>212</v>
+      <c r="B54">
+        <v>3637</v>
       </c>
       <c r="C54">
-        <v>36057.66373063793</v>
+        <v>3637</v>
       </c>
       <c r="D54">
-        <v>33344.22909790605</v>
+        <v>3637</v>
       </c>
       <c r="E54">
-        <v>34286.84568702983</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B55" t="s">
-        <v>212</v>
+      <c r="B55">
+        <v>301</v>
       </c>
       <c r="C55">
-        <v>66822.51137331135</v>
+        <v>301</v>
       </c>
       <c r="D55">
-        <v>61855.23107261454</v>
+        <v>301</v>
       </c>
       <c r="E55">
-        <v>63948.66570649843</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B56" t="s">
-        <v>212</v>
+      <c r="B56">
+        <v>537</v>
       </c>
       <c r="C56">
-        <v>33156.30459804353</v>
+        <v>537</v>
       </c>
       <c r="D56">
-        <v>33335.50923218194</v>
+        <v>537</v>
       </c>
       <c r="E56">
-        <v>33397.07322472375</v>
+        <v>537</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B57" t="s">
-        <v>212</v>
+      <c r="B57">
+        <v>300</v>
       </c>
       <c r="C57">
-        <v>9986.417617537509</v>
+        <v>300</v>
       </c>
       <c r="D57">
-        <v>10194.62059102478</v>
+        <v>300</v>
       </c>
       <c r="E57">
-        <v>10338.40358091756</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2035,16 +2032,16 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C58">
-        <v>8306.813376518987</v>
+        <v>285733.3218235314</v>
       </c>
       <c r="D58">
-        <v>6946.591660718233</v>
+        <v>274161.0000038777</v>
       </c>
       <c r="E58">
-        <v>8135.667377017133</v>
+        <v>275663.3373324008</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2052,16 +2049,16 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C59">
-        <v>29427.44116169451</v>
+        <v>36057.66373063793</v>
       </c>
       <c r="D59">
-        <v>30953.22576377643</v>
+        <v>33344.22909790605</v>
       </c>
       <c r="E59">
-        <v>31386.31536916655</v>
+        <v>34286.84568702983</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2069,16 +2066,16 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C60">
-        <v>37145.33462606892</v>
+        <v>66822.51137331135</v>
       </c>
       <c r="D60">
-        <v>39041.11738664036</v>
+        <v>61855.23107261454</v>
       </c>
       <c r="E60">
-        <v>40239.51136715176</v>
+        <v>63948.66570649843</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2086,16 +2083,16 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C61">
-        <v>5309.478782988256</v>
+        <v>33156.30459804353</v>
       </c>
       <c r="D61">
-        <v>5060.408660766857</v>
+        <v>33335.50923218194</v>
       </c>
       <c r="E61">
-        <v>5201.12526897965</v>
+        <v>33397.07322472375</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2103,16 +2100,16 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C62">
-        <v>5521.895631861405</v>
+        <v>9986.417617537509</v>
       </c>
       <c r="D62">
-        <v>6073.616715538182</v>
+        <v>10194.62059102478</v>
       </c>
       <c r="E62">
-        <v>6265.692004112236</v>
+        <v>10338.40358091756</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2120,16 +2117,16 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C63">
-        <v>7012.74256878429</v>
+        <v>8306.813376518987</v>
       </c>
       <c r="D63">
-        <v>6467.15326810131</v>
+        <v>6946.591660718233</v>
       </c>
       <c r="E63">
-        <v>6547.602648720247</v>
+        <v>8135.667377017133</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2137,16 +2134,16 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C64">
-        <v>7317.313641591267</v>
+        <v>29427.44116169451</v>
       </c>
       <c r="D64">
-        <v>7240.499364931959</v>
+        <v>30953.22576377643</v>
       </c>
       <c r="E64">
-        <v>7309.076098225414</v>
+        <v>31386.31536916655</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2154,16 +2151,16 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C65">
-        <v>2166.404734331622</v>
+        <v>37145.33462606892</v>
       </c>
       <c r="D65">
-        <v>2013.947393383935</v>
+        <v>39041.11738664036</v>
       </c>
       <c r="E65">
-        <v>2067.009181064854</v>
+        <v>40239.51136715176</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2171,16 +2168,16 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C66">
-        <v>3081.965248662672</v>
+        <v>5309.478782988256</v>
       </c>
       <c r="D66">
-        <v>3137.447595991872</v>
+        <v>5060.408660766857</v>
       </c>
       <c r="E66">
-        <v>3186.615419267629</v>
+        <v>5201.12526897965</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2188,16 +2185,16 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C67">
-        <v>443.1341918519325</v>
+        <v>5521.895631861405</v>
       </c>
       <c r="D67">
-        <v>421.887538681912</v>
+        <v>6073.616715538182</v>
       </c>
       <c r="E67">
-        <v>433.4544189987498</v>
+        <v>6265.692004112236</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2205,16 +2202,16 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C68">
-        <v>2895.085614458657</v>
+        <v>7012.74256878429</v>
       </c>
       <c r="D68">
-        <v>2909.362870154178</v>
+        <v>6467.15326810131</v>
       </c>
       <c r="E68">
-        <v>2924.168116891962</v>
+        <v>6547.602648720247</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2222,16 +2219,16 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C69">
-        <v>3653.831655445544</v>
+        <v>7317.313641591267</v>
       </c>
       <c r="D69">
-        <v>3598.638480494133</v>
+        <v>7240.499364931959</v>
       </c>
       <c r="E69">
-        <v>3616.404971165329</v>
+        <v>7309.076098225414</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2239,16 +2236,16 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C70">
-        <v>3542.454003930634</v>
+        <v>2166.404734331622</v>
       </c>
       <c r="D70">
-        <v>3648.230892236539</v>
+        <v>2013.947393383935</v>
       </c>
       <c r="E70">
-        <v>3678.324608989895</v>
+        <v>2067.009181064854</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2256,16 +2253,16 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C71">
-        <v>4257.401768859199</v>
+        <v>3081.965248662672</v>
       </c>
       <c r="D71">
-        <v>4324.862744573556</v>
+        <v>3137.447595991872</v>
       </c>
       <c r="E71">
-        <v>4363.718311116243</v>
+        <v>3186.615419267629</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2273,16 +2270,16 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C72">
-        <v>881.1481005457115</v>
+        <v>443.1341918519325</v>
       </c>
       <c r="D72">
-        <v>922.4946308419028</v>
+        <v>421.887538681912</v>
       </c>
       <c r="E72">
-        <v>951.6553445648265</v>
+        <v>433.4544189987498</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2290,16 +2287,16 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C73">
-        <v>911.7413777070067</v>
+        <v>2895.085614458657</v>
       </c>
       <c r="D73">
-        <v>868.7478168054034</v>
+        <v>2909.362870154178</v>
       </c>
       <c r="E73">
-        <v>883.9572064300576</v>
+        <v>2924.168116891962</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2307,16 +2304,16 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>3653.831655445544</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>3598.638480494133</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>3616.404971165329</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2324,16 +2321,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C75">
-        <v>310887.0551086462</v>
+        <v>3542.454003930634</v>
       </c>
       <c r="D75">
-        <v>290797.302000507</v>
+        <v>3648.230892236539</v>
       </c>
       <c r="E75">
-        <v>292306.0034436272</v>
+        <v>3678.324608989895</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2341,16 +2338,16 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C76">
-        <v>51074.32436027069</v>
+        <v>4257.401768859199</v>
       </c>
       <c r="D76">
-        <v>26072.86402002085</v>
+        <v>4324.862744573556</v>
       </c>
       <c r="E76">
-        <v>44744.53526801307</v>
+        <v>4363.718311116243</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2358,16 +2355,16 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C77">
-        <v>84109.82719823082</v>
+        <v>881.1481005457115</v>
       </c>
       <c r="D77">
-        <v>77937.73156609248</v>
+        <v>922.4946308419028</v>
       </c>
       <c r="E77">
-        <v>84581.97612214876</v>
+        <v>951.6553445648265</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2375,16 +2372,16 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C78">
-        <v>39310.49274971832</v>
+        <v>911.7413777070067</v>
       </c>
       <c r="D78">
-        <v>38683.92515358835</v>
+        <v>868.7478168054034</v>
       </c>
       <c r="E78">
-        <v>38875.73769831542</v>
+        <v>883.9572064300576</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2392,16 +2389,16 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C79">
-        <v>11932.38400809033</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>10681.35241281803</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>11035.70441498311</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2409,16 +2406,16 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C80">
-        <v>9548.28031721313</v>
+        <v>310887.0551086462</v>
       </c>
       <c r="D80">
-        <v>7703.305735153427</v>
+        <v>290797.302000507</v>
       </c>
       <c r="E80">
-        <v>8161.797271070729</v>
+        <v>292306.0034436272</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2426,16 +2423,16 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C81">
-        <v>35810.66989709945</v>
+        <v>51074.32436027069</v>
       </c>
       <c r="D81">
-        <v>36601.69575249061</v>
+        <v>26072.86402002085</v>
       </c>
       <c r="E81">
-        <v>39241.8615517352</v>
+        <v>44744.53526801307</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2443,16 +2440,16 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C82">
-        <v>40274.91199119319</v>
+        <v>84109.82719823082</v>
       </c>
       <c r="D82">
-        <v>41351.35312049399</v>
+        <v>77937.73156609248</v>
       </c>
       <c r="E82">
-        <v>44632.82113421193</v>
+        <v>84581.97612214876</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2460,16 +2457,16 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C83">
-        <v>5702.582508173264</v>
+        <v>39310.49274971832</v>
       </c>
       <c r="D83">
-        <v>5197.04316560074</v>
+        <v>38683.92515358835</v>
       </c>
       <c r="E83">
-        <v>5490.350510109492</v>
+        <v>38875.73769831542</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2477,16 +2474,16 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C84">
-        <v>6531.454941380145</v>
+        <v>11932.38400809033</v>
       </c>
       <c r="D84">
-        <v>6914.424310549415</v>
+        <v>10681.35241281803</v>
       </c>
       <c r="E84">
-        <v>7565.494786531661</v>
+        <v>11035.70441498311</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2494,16 +2491,16 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C85">
-        <v>11086.07248419944</v>
+        <v>9548.28031721313</v>
       </c>
       <c r="D85">
-        <v>9081.046501582416</v>
+        <v>7703.305735153427</v>
       </c>
       <c r="E85">
-        <v>9712.39919620127</v>
+        <v>8161.797271070729</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2511,16 +2508,16 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C86">
-        <v>11235.01770760014</v>
+        <v>35810.66989709945</v>
       </c>
       <c r="D86">
-        <v>7294.264487669744</v>
+        <v>36601.69575249061</v>
       </c>
       <c r="E86">
-        <v>7393.954728795917</v>
+        <v>39241.8615517352</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2528,16 +2525,16 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C87">
-        <v>2313.18743770475</v>
+        <v>40274.91199119319</v>
       </c>
       <c r="D87">
-        <v>2050.379609518187</v>
+        <v>41351.35312049399</v>
       </c>
       <c r="E87">
-        <v>2158.015018647229</v>
+        <v>44632.82113421193</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2545,16 +2542,16 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C88">
-        <v>4487.422497745161</v>
+        <v>5702.582508173264</v>
       </c>
       <c r="D88">
-        <v>3251.340662315742</v>
+        <v>5197.04316560074</v>
       </c>
       <c r="E88">
-        <v>3680.595601936531</v>
+        <v>5490.350510109492</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2562,16 +2559,16 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C89">
-        <v>3291.571394333075</v>
+        <v>6531.454941380145</v>
       </c>
       <c r="D89">
-        <v>453.0691373312048</v>
+        <v>6914.424310549415</v>
       </c>
       <c r="E89">
-        <v>505.4945456516502</v>
+        <v>7565.494786531661</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2579,16 +2576,16 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C90">
-        <v>2962.271032197586</v>
+        <v>11086.07248419944</v>
       </c>
       <c r="D90">
-        <v>2922.939603860779</v>
+        <v>9081.046501582416</v>
       </c>
       <c r="E90">
-        <v>2944.717615440521</v>
+        <v>9712.39919620127</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2596,16 +2593,16 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C91">
-        <v>3978.851277647058</v>
+        <v>11235.01770760014</v>
       </c>
       <c r="D91">
-        <v>1566.476580450332</v>
+        <v>7294.264487669744</v>
       </c>
       <c r="E91">
-        <v>1592.42779801514</v>
+        <v>7393.954728795917</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2613,16 +2610,16 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C92">
-        <v>3624.875154413226</v>
+        <v>2313.18743770475</v>
       </c>
       <c r="D92">
-        <v>3677.660725632635</v>
+        <v>2050.379609518187</v>
       </c>
       <c r="E92">
-        <v>3727.402937205914</v>
+        <v>2158.015018647229</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2630,16 +2627,16 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C93">
-        <v>4499.453713305816</v>
+        <v>4487.422497745161</v>
       </c>
       <c r="D93">
-        <v>4389.339541465134</v>
+        <v>3251.340662315742</v>
       </c>
       <c r="E93">
-        <v>4489.156966460471</v>
+        <v>3680.595601936531</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2647,16 +2644,16 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C94">
-        <v>1176.375213333053</v>
+        <v>3291.571394333075</v>
       </c>
       <c r="D94">
-        <v>1229.853805184373</v>
+        <v>453.0691373312048</v>
       </c>
       <c r="E94">
-        <v>1330.656790249233</v>
+        <v>505.4945456516502</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2664,16 +2661,16 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C95">
-        <v>1013.219479989464</v>
+        <v>2962.271032197586</v>
       </c>
       <c r="D95">
-        <v>873.6169022987777</v>
+        <v>2922.939603860779</v>
       </c>
       <c r="E95">
-        <v>911.1327501980686</v>
+        <v>2944.717615440521</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2681,16 +2678,16 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C96">
-        <v>857.2621118872319</v>
+        <v>3978.851277647058</v>
       </c>
       <c r="D96">
-        <v>772.2734198315197</v>
+        <v>1566.476580450332</v>
       </c>
       <c r="E96">
-        <v>801.0018403865388</v>
+        <v>1592.42779801514</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2698,16 +2695,16 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C97">
-        <v>345179.8540918057</v>
+        <v>3624.875154413226</v>
       </c>
       <c r="D97">
-        <v>306070.7824845224</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E97">
-        <v>311915.8222954976</v>
+        <v>3727.402937205914</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2715,16 +2712,16 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C98">
-        <v>57843.05696310467</v>
+        <v>4499.453713305816</v>
       </c>
       <c r="D98">
-        <v>41761.14805054816</v>
+        <v>4389.339541465134</v>
       </c>
       <c r="E98">
-        <v>48660.60638720006</v>
+        <v>4489.156966460471</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2732,16 +2729,16 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C99">
-        <v>106400.8113634808</v>
+        <v>1176.375213333053</v>
       </c>
       <c r="D99">
-        <v>97376.26626200562</v>
+        <v>1229.853805184373</v>
       </c>
       <c r="E99">
-        <v>107457.7153467231</v>
+        <v>1330.656790249233</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2749,16 +2746,16 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C100">
-        <v>47754.67592555143</v>
+        <v>1013.219479989464</v>
       </c>
       <c r="D100">
-        <v>46917.82385382168</v>
+        <v>873.6169022987777</v>
       </c>
       <c r="E100">
-        <v>47285.0706371487</v>
+        <v>911.1327501980686</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2766,16 +2763,16 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C101">
-        <v>13642.04328300475</v>
+        <v>857.2621118872319</v>
       </c>
       <c r="D101">
-        <v>12594.12090677959</v>
+        <v>772.2734198315197</v>
       </c>
       <c r="E101">
-        <v>14151.68818183644</v>
+        <v>801.0018403865388</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2783,16 +2780,16 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C102">
-        <v>10166.68671320246</v>
+        <v>345179.8540918057</v>
       </c>
       <c r="D102">
-        <v>7870.660600118454</v>
+        <v>306070.7824845224</v>
       </c>
       <c r="E102">
-        <v>8448.569974010888</v>
+        <v>311915.8222954976</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2800,16 +2797,16 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C103">
-        <v>40056.29615048355</v>
+        <v>57843.05696310467</v>
       </c>
       <c r="D103">
-        <v>39938.78970433185</v>
+        <v>41761.14805054816</v>
       </c>
       <c r="E103">
-        <v>44520.15917103966</v>
+        <v>48660.60638720006</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2817,16 +2814,16 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C104">
-        <v>42099.78280750295</v>
+        <v>106400.8113634808</v>
       </c>
       <c r="D104">
-        <v>42299.87775020443</v>
+        <v>97376.26626200562</v>
       </c>
       <c r="E104">
-        <v>47328.28098195308</v>
+        <v>107457.7153467231</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2834,16 +2831,16 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C105">
-        <v>6780.581746217548</v>
+        <v>47754.67592555143</v>
       </c>
       <c r="D105">
-        <v>5344.462556042371</v>
+        <v>46917.82385382168</v>
       </c>
       <c r="E105">
-        <v>5852.587839854697</v>
+        <v>47285.0706371487</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2851,16 +2848,16 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C106">
-        <v>7052.041776574091</v>
+        <v>13642.04328300475</v>
       </c>
       <c r="D106">
-        <v>2387.833946905571</v>
+        <v>12594.12090677959</v>
       </c>
       <c r="E106">
-        <v>2653.360912751024</v>
+        <v>14151.68818183644</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2868,16 +2865,16 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C107">
-        <v>12491.64080553533</v>
+        <v>10166.68671320246</v>
       </c>
       <c r="D107">
-        <v>7553.961214696117</v>
+        <v>7870.660600118454</v>
       </c>
       <c r="E107">
-        <v>8823.015551678049</v>
+        <v>8448.569974010888</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2885,16 +2882,16 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C108">
-        <v>11918.07029478611</v>
+        <v>40056.29615048355</v>
       </c>
       <c r="D108">
-        <v>10755.76769609013</v>
+        <v>39938.78970433185</v>
       </c>
       <c r="E108">
-        <v>11073.8263395291</v>
+        <v>44520.15917103966</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2902,16 +2899,16 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C109">
-        <v>2510.791313969085</v>
+        <v>42099.78280750295</v>
       </c>
       <c r="D109">
-        <v>2080.311820058766</v>
+        <v>42299.87775020443</v>
       </c>
       <c r="E109">
-        <v>2225.787307207039</v>
+        <v>47328.28098195308</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2919,16 +2916,16 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C110">
-        <v>5559.189168957029</v>
+        <v>6780.581746217548</v>
       </c>
       <c r="D110">
-        <v>3507.429258284409</v>
+        <v>5344.462556042371</v>
       </c>
       <c r="E110">
-        <v>4514.632917614302</v>
+        <v>5852.587839854697</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2936,16 +2933,16 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C111">
-        <v>3740.698985412615</v>
+        <v>7052.041776574091</v>
       </c>
       <c r="D111">
-        <v>456.0519360615073</v>
+        <v>2387.833946905571</v>
       </c>
       <c r="E111">
-        <v>595.516072795263</v>
+        <v>2653.360912751024</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2953,16 +2950,16 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C112">
-        <v>3025.982972811596</v>
+        <v>12491.64080553533</v>
       </c>
       <c r="D112">
-        <v>2930.200017528361</v>
+        <v>7553.961214696117</v>
       </c>
       <c r="E112">
-        <v>2972.156458241908</v>
+        <v>8823.015551678049</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2970,16 +2967,16 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C113">
-        <v>4384.134004159239</v>
+        <v>11918.07029478611</v>
       </c>
       <c r="D113">
-        <v>3877.68979844253</v>
+        <v>10755.76769609013</v>
       </c>
       <c r="E113">
-        <v>3984.413723700878</v>
+        <v>11073.8263395291</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2987,16 +2984,16 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C114">
-        <v>3818.113674370041</v>
+        <v>2510.791313969085</v>
       </c>
       <c r="D114">
-        <v>3677.660725632635</v>
+        <v>2080.311820058766</v>
       </c>
       <c r="E114">
-        <v>3773.270697207371</v>
+        <v>2225.787307207039</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3004,16 +3001,16 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C115">
-        <v>5697.549039481555</v>
+        <v>5559.189168957029</v>
       </c>
       <c r="D115">
-        <v>4449.270708440607</v>
+        <v>3507.429258284409</v>
       </c>
       <c r="E115">
-        <v>4794.85366801385</v>
+        <v>4514.632917614302</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3021,16 +3018,16 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C116">
-        <v>1675.03137312741</v>
+        <v>3740.698985412615</v>
       </c>
       <c r="D116">
-        <v>1815.4386330182</v>
+        <v>456.0519360615073</v>
       </c>
       <c r="E116">
-        <v>2049.263941768266</v>
+        <v>595.516072795263</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3038,16 +3035,16 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C117">
-        <v>1388.615296125427</v>
+        <v>3025.982972811596</v>
       </c>
       <c r="D117">
-        <v>898.8243487684732</v>
+        <v>2930.200017528361</v>
       </c>
       <c r="E117">
-        <v>1101.853615098803</v>
+        <v>2972.156458241908</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3055,16 +3052,16 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C118">
-        <v>915.4210068592286</v>
+        <v>4384.134004159239</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>3877.68979844253</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>3984.413723700878</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3072,16 +3069,16 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C119">
-        <v>379833.2126030341</v>
+        <v>3818.113674370041</v>
       </c>
       <c r="D119">
-        <v>323789.1870151541</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E119">
-        <v>342305.1273678984</v>
+        <v>3773.270697207371</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3089,16 +3086,16 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C120">
-        <v>66636.46327624648</v>
+        <v>5697.549039481555</v>
       </c>
       <c r="D120">
-        <v>57885.11081377808</v>
+        <v>4449.270708440607</v>
       </c>
       <c r="E120">
-        <v>65450.5214985832</v>
+        <v>4794.85366801385</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3106,16 +3103,16 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C121">
-        <v>122447.4212601383</v>
+        <v>1675.03137312741</v>
       </c>
       <c r="D121">
-        <v>106273.0478090824</v>
+        <v>1815.4386330182</v>
       </c>
       <c r="E121">
-        <v>119530.3850553175</v>
+        <v>2049.263941768266</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3123,16 +3120,16 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C122">
-        <v>55098.14072490651</v>
+        <v>1388.615296125427</v>
       </c>
       <c r="D122">
-        <v>53997.08352943832</v>
+        <v>898.8243487684732</v>
       </c>
       <c r="E122">
-        <v>54429.29718809373</v>
+        <v>1101.853615098803</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3140,16 +3137,16 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C123">
-        <v>17436.20392355449</v>
+        <v>915.4210068592286</v>
       </c>
       <c r="D123">
-        <v>19678.07818882393</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>23411.63616688988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3157,16 +3154,16 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C124">
-        <v>11477.1443269179</v>
+        <v>379833.2126030341</v>
       </c>
       <c r="D124">
-        <v>7941.17271971979</v>
+        <v>323789.1870151541</v>
       </c>
       <c r="E124">
-        <v>8685.454438123739</v>
+        <v>342305.1273678984</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3174,16 +3171,16 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C125">
-        <v>44788.85407568982</v>
+        <v>66636.46327624648</v>
       </c>
       <c r="D125">
-        <v>42290.86139964137</v>
+        <v>57885.11081377808</v>
       </c>
       <c r="E125">
-        <v>48116.24030242601</v>
+        <v>65450.5214985832</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3191,16 +3188,16 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C126">
-        <v>43854.83257609577</v>
+        <v>122447.4212601383</v>
       </c>
       <c r="D126">
-        <v>42446.11108034404</v>
+        <v>106273.0478090824</v>
       </c>
       <c r="E126">
-        <v>48048.47217811201</v>
+        <v>119530.3850553175</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3208,16 +3205,16 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C127">
-        <v>7818.02330571639</v>
+        <v>55098.14072490651</v>
       </c>
       <c r="D127">
-        <v>5653.095564499369</v>
+        <v>53997.08352943832</v>
       </c>
       <c r="E127">
-        <v>6625.371912088781</v>
+        <v>54429.29718809373</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3225,16 +3222,16 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C128">
-        <v>8085.182658295945</v>
+        <v>17436.20392355449</v>
       </c>
       <c r="D128">
-        <v>7503.614943774021</v>
+        <v>19678.07818882393</v>
       </c>
       <c r="E128">
-        <v>8938.0868588093</v>
+        <v>23411.63616688988</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3242,16 +3239,16 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C129">
-        <v>14492.94704346139</v>
+        <v>11477.1443269179</v>
       </c>
       <c r="D129">
-        <v>11209.84775023005</v>
+        <v>7941.17271971979</v>
       </c>
       <c r="E129">
-        <v>10752.42132399964</v>
+        <v>8685.454438123739</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3259,16 +3256,16 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C130">
-        <v>14025.08468897277</v>
+        <v>44788.85407568982</v>
       </c>
       <c r="D130">
-        <v>11232.84453326727</v>
+        <v>42290.86139964137</v>
       </c>
       <c r="E130">
-        <v>12584.87999504888</v>
+        <v>48116.24030242601</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3276,16 +3273,16 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C131">
-        <v>2660.082565212768</v>
+        <v>43854.83257609577</v>
       </c>
       <c r="D131">
-        <v>2118.88338047299</v>
+        <v>42446.11108034404</v>
       </c>
       <c r="E131">
-        <v>2317.74860784036</v>
+        <v>48048.47217811201</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3293,16 +3290,16 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C132">
-        <v>6699.919359426849</v>
+        <v>7818.02330571639</v>
       </c>
       <c r="D132">
-        <v>3926.964562863937</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E132">
-        <v>5419.280756815793</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3310,16 +3307,16 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C133">
-        <v>4240.498957073307</v>
+        <v>8085.182658295945</v>
       </c>
       <c r="D133">
-        <v>2799.802017040321</v>
+        <v>7503.614943774021</v>
       </c>
       <c r="E133">
-        <v>3370.629266244694</v>
+        <v>8938.0868588093</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3327,16 +3324,16 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C134">
-        <v>3104.11640049039</v>
+        <v>14492.94704346139</v>
       </c>
       <c r="D134">
-        <v>2945.585161856526</v>
+        <v>11209.84775023005</v>
       </c>
       <c r="E134">
-        <v>3032.000269374993</v>
+        <v>10752.42132399964</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3344,16 +3341,16 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C135">
-        <v>4758.923090909089</v>
+        <v>14025.08468897277</v>
       </c>
       <c r="D135">
-        <v>4052.36859619171</v>
+        <v>11232.84453326727</v>
       </c>
       <c r="E135">
-        <v>4241.271500156832</v>
+        <v>12584.87999504888</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3361,16 +3358,16 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C136">
-        <v>4582.423026269129</v>
+        <v>2660.082565212768</v>
       </c>
       <c r="D136">
-        <v>3677.660725632635</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E136">
-        <v>3936.041511138754</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3378,16 +3375,16 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C137">
-        <v>8274.311032145955</v>
+        <v>6699.919359426849</v>
       </c>
       <c r="D137">
-        <v>4554.906523253632</v>
+        <v>3926.964562863937</v>
       </c>
       <c r="E137">
-        <v>6530.74208924048</v>
+        <v>5419.280756815793</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3395,16 +3392,16 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C138">
-        <v>2362.496887971177</v>
+        <v>4240.498957073307</v>
       </c>
       <c r="D138">
-        <v>4552.94161730676</v>
+        <v>2799.802017040321</v>
       </c>
       <c r="E138">
-        <v>7699.768813994026</v>
+        <v>3370.629266244694</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3412,16 +3409,16 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C139">
-        <v>1764.352253203638</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D139">
-        <v>974.5725435688446</v>
+        <v>2945.585161856526</v>
       </c>
       <c r="E139">
-        <v>1393.90973989574</v>
+        <v>3032.000269374993</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3429,16 +3426,16 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C140">
-        <v>921.2368963564281</v>
+        <v>4758.923090909089</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>4052.36859619171</v>
       </c>
       <c r="E140">
-        <v>0</v>
+        <v>4241.271500156832</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3446,16 +3443,16 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C141">
-        <v>409436.7691592983</v>
+        <v>4582.423026269129</v>
       </c>
       <c r="D141">
-        <v>355341.7534723968</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E141">
-        <v>387999.3260030203</v>
+        <v>3936.041511138754</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3463,16 +3460,16 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C142">
-        <v>66424.65479531829</v>
+        <v>8274.311032145955</v>
       </c>
       <c r="D142">
-        <v>67311.96044664056</v>
+        <v>4554.906523253632</v>
       </c>
       <c r="E142">
-        <v>76231.77993843338</v>
+        <v>6530.74208924048</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3480,16 +3477,16 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C143">
-        <v>125858.7401545331</v>
+        <v>2362.496887971177</v>
       </c>
       <c r="D143">
-        <v>95923.88790038624</v>
+        <v>4552.94161730676</v>
       </c>
       <c r="E143">
-        <v>124140.5773429784</v>
+        <v>7699.768813994026</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3497,16 +3494,16 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C144">
-        <v>55158.37308241575</v>
+        <v>1764.352253203638</v>
       </c>
       <c r="D144">
-        <v>54194.17670445503</v>
+        <v>974.5725435688446</v>
       </c>
       <c r="E144">
-        <v>54731.6463609033</v>
+        <v>1393.90973989574</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3514,16 +3511,16 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C145">
-        <v>18810.64774314864</v>
+        <v>921.2368963564281</v>
       </c>
       <c r="D145">
-        <v>26985.75868185313</v>
+        <v>0</v>
       </c>
       <c r="E145">
-        <v>33814.25416223275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3531,16 +3528,16 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C146">
-        <v>11786.58854248258</v>
+        <v>409436.7691592983</v>
       </c>
       <c r="D146">
-        <v>9267.503482344102</v>
+        <v>355341.7534723968</v>
       </c>
       <c r="E146">
-        <v>10151.93626108859</v>
+        <v>387999.3260030203</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3548,16 +3545,16 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C147">
-        <v>41809.31820607139</v>
+        <v>66424.65479531829</v>
       </c>
       <c r="D147">
-        <v>39732.01918427406</v>
+        <v>67311.96044664056</v>
       </c>
       <c r="E147">
-        <v>46033.76592047335</v>
+        <v>76231.77993843338</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3565,16 +3562,16 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C148">
-        <v>44322.79570608526</v>
+        <v>125858.7401545331</v>
       </c>
       <c r="D148">
-        <v>42997.62304068729</v>
+        <v>95923.88790038624</v>
       </c>
       <c r="E148">
-        <v>49150.09462369821</v>
+        <v>124140.5773429784</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3582,16 +3579,16 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C149">
-        <v>7830.871226366395</v>
+        <v>55158.37308241575</v>
       </c>
       <c r="D149">
-        <v>5653.095564499369</v>
+        <v>54194.17670445503</v>
       </c>
       <c r="E149">
-        <v>6625.371912088781</v>
+        <v>54731.6463609033</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3599,16 +3596,16 @@
         <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C150">
-        <v>8817.535269776827</v>
+        <v>18810.64774314864</v>
       </c>
       <c r="D150">
-        <v>9011.059942949789</v>
+        <v>26985.75868185313</v>
       </c>
       <c r="E150">
-        <v>10838.71267389012</v>
+        <v>33814.25416223275</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -3616,16 +3613,16 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C151">
-        <v>15730.7337703995</v>
+        <v>11786.58854248258</v>
       </c>
       <c r="D151">
-        <v>12870.92751701806</v>
+        <v>9267.503482344102</v>
       </c>
       <c r="E151">
-        <v>16028.57827823479</v>
+        <v>10151.93626108859</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3633,16 +3630,16 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C152">
-        <v>14763.70638988416</v>
+        <v>41809.31820607139</v>
       </c>
       <c r="D152">
-        <v>11353.82086139094</v>
+        <v>39732.01918427406</v>
       </c>
       <c r="E152">
-        <v>15744.22408353954</v>
+        <v>46033.76592047335</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3650,16 +3647,16 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C153">
-        <v>2664.581838046233</v>
+        <v>44322.79570608526</v>
       </c>
       <c r="D153">
-        <v>2118.88338047299</v>
+        <v>42997.62304068729</v>
       </c>
       <c r="E153">
-        <v>2317.74860784036</v>
+        <v>49150.09462369821</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3667,16 +3664,16 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C154">
-        <v>7118.299388486004</v>
+        <v>7830.871226366395</v>
       </c>
       <c r="D154">
-        <v>4387.796042371227</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E154">
-        <v>6214.950571608244</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3684,16 +3681,16 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C155">
-        <v>1256.930682890124</v>
+        <v>8817.535269776827</v>
       </c>
       <c r="D155">
-        <v>634.2799162905493</v>
+        <v>9011.059942949789</v>
       </c>
       <c r="E155">
-        <v>1060.520130278657</v>
+        <v>10838.71267389012</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3701,16 +3698,16 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C156">
-        <v>3104.11640049039</v>
+        <v>15730.7337703995</v>
       </c>
       <c r="D156">
-        <v>2953.473502833881</v>
+        <v>12870.92751701806</v>
       </c>
       <c r="E156">
-        <v>3032.074436227733</v>
+        <v>16028.57827823479</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3718,16 +3715,16 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>14763.70638988416</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>11353.82086139094</v>
       </c>
       <c r="E157">
-        <v>1927.316250691574</v>
+        <v>15744.22408353954</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3735,16 +3732,16 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C158">
-        <v>4982.658106436934</v>
+        <v>2664.581838046233</v>
       </c>
       <c r="D158">
-        <v>3682.745087885083</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E158">
-        <v>4606.149113368056</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3752,16 +3749,16 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C159">
-        <v>9858.7475739898</v>
+        <v>7118.299388486004</v>
       </c>
       <c r="D159">
-        <v>4988.549100871839</v>
+        <v>4387.796042371227</v>
       </c>
       <c r="E159">
-        <v>9051.622561655677</v>
+        <v>6214.950571608244</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3769,16 +3766,16 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C160">
-        <v>3049.962402814945</v>
+        <v>1256.930682890124</v>
       </c>
       <c r="D160">
-        <v>7885.799173422068</v>
+        <v>634.2799162905493</v>
       </c>
       <c r="E160">
-        <v>14476.78741030169</v>
+        <v>1060.520130278657</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3786,16 +3783,16 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C161">
-        <v>1932.537890358078</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D161">
-        <v>1092.439628676345</v>
+        <v>2953.473502833881</v>
       </c>
       <c r="E161">
-        <v>1729.767824059069</v>
+        <v>3032.074436227733</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3803,16 +3800,16 @@
         <v>164</v>
       </c>
       <c r="B162" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C162">
-        <v>927.0527858536279</v>
+        <v>0</v>
       </c>
       <c r="D162">
-        <v>885.4644642160963</v>
+        <v>0</v>
       </c>
       <c r="E162">
-        <v>854.6967352460968</v>
+        <v>1927.316250691574</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3820,16 +3817,16 @@
         <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C163">
-        <v>425667.2304377211</v>
+        <v>4982.658106436934</v>
       </c>
       <c r="D163">
-        <v>379452.4458343688</v>
+        <v>3682.745087885083</v>
       </c>
       <c r="E163">
-        <v>422462.404769241</v>
+        <v>4606.149113368056</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3837,16 +3834,16 @@
         <v>166</v>
       </c>
       <c r="B164" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C164">
-        <v>74824.1776942108</v>
+        <v>9858.7475739898</v>
       </c>
       <c r="D164">
-        <v>75532.04105321791</v>
+        <v>4988.549100871839</v>
       </c>
       <c r="E164">
-        <v>86492.52473873404</v>
+        <v>9051.622561655677</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3854,16 +3851,16 @@
         <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C165">
-        <v>128549.8642605276</v>
+        <v>3049.962402814945</v>
       </c>
       <c r="D165">
-        <v>114702.4949950556</v>
+        <v>7885.799173422068</v>
       </c>
       <c r="E165">
-        <v>134200.4554046213</v>
+        <v>14476.78741030169</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3871,16 +3868,16 @@
         <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C166">
-        <v>55242.88725228325</v>
+        <v>1932.537890358078</v>
       </c>
       <c r="D166">
-        <v>54348.67956945477</v>
+        <v>1092.439628676345</v>
       </c>
       <c r="E166">
-        <v>54823.8158790419</v>
+        <v>1729.767824059069</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3888,16 +3885,16 @@
         <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C167">
-        <v>21186.42152206995</v>
+        <v>927.0527858536279</v>
       </c>
       <c r="D167">
-        <v>32192.86399794241</v>
+        <v>885.4644642160963</v>
       </c>
       <c r="E167">
-        <v>40091.29523030741</v>
+        <v>854.6967352460968</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3905,16 +3902,16 @@
         <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C168">
-        <v>12108.98627481771</v>
+        <v>425667.2304377211</v>
       </c>
       <c r="D168">
-        <v>9710.044517252907</v>
+        <v>379452.4458343688</v>
       </c>
       <c r="E168">
-        <v>9820.712234959921</v>
+        <v>422462.404769241</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3922,16 +3919,16 @@
         <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C169">
-        <v>44818.4592191087</v>
+        <v>74824.1776942108</v>
       </c>
       <c r="D169">
-        <v>43318.43942297382</v>
+        <v>75532.04105321791</v>
       </c>
       <c r="E169">
-        <v>50430.2444258372</v>
+        <v>86492.52473873404</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3939,16 +3936,16 @@
         <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C170">
-        <v>45410.20682375576</v>
+        <v>128549.8642605276</v>
       </c>
       <c r="D170">
-        <v>44140.29328236685</v>
+        <v>114702.4949950556</v>
       </c>
       <c r="E170">
-        <v>50777.920807722</v>
+        <v>134200.4554046213</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3956,16 +3953,16 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C171">
-        <v>7877.356799130208</v>
+        <v>55242.88725228325</v>
       </c>
       <c r="D171">
-        <v>5653.095564499369</v>
+        <v>54348.67956945477</v>
       </c>
       <c r="E171">
-        <v>6662.276843942194</v>
+        <v>54823.8158790419</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3973,16 +3970,16 @@
         <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C172">
-        <v>7081.366168574467</v>
+        <v>21186.42152206995</v>
       </c>
       <c r="D172">
-        <v>7237.854347805022</v>
+        <v>32192.86399794241</v>
       </c>
       <c r="E172">
-        <v>8761.01660377788</v>
+        <v>40091.29523030741</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -3990,16 +3987,16 @@
         <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C173">
-        <v>17240.04215367412</v>
+        <v>12108.98627481771</v>
       </c>
       <c r="D173">
-        <v>13942.82778271549</v>
+        <v>9710.044517252907</v>
       </c>
       <c r="E173">
-        <v>14713.17492592106</v>
+        <v>9820.712234959921</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4007,16 +4004,16 @@
         <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C174">
-        <v>17324.03456184319</v>
+        <v>44818.4592191087</v>
       </c>
       <c r="D174">
-        <v>13476.54727078326</v>
+        <v>43318.43942297382</v>
       </c>
       <c r="E174">
-        <v>22628.13038686703</v>
+        <v>50430.2444258372</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -4024,16 +4021,16 @@
         <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C175">
-        <v>2689.033001442709</v>
+        <v>45410.20682375576</v>
       </c>
       <c r="D175">
-        <v>2118.88338047299</v>
+        <v>44140.29328236685</v>
       </c>
       <c r="E175">
-        <v>2326.478289412053</v>
+        <v>50777.920807722</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4041,16 +4038,16 @@
         <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C176">
-        <v>7330.001934671265</v>
+        <v>7877.356799130208</v>
       </c>
       <c r="D176">
-        <v>4696.892936408833</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E176">
-        <v>6336.909947377137</v>
+        <v>6662.276843942194</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4058,16 +4055,16 @@
         <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C177">
-        <v>3666.34991690552</v>
+        <v>7081.366168574467</v>
       </c>
       <c r="D177">
-        <v>2659.16265449915</v>
+        <v>7237.854347805022</v>
       </c>
       <c r="E177">
-        <v>3251.428044629679</v>
+        <v>8761.01660377788</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -4075,16 +4072,16 @@
         <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C178">
-        <v>3110.615608057638</v>
+        <v>17240.04215367412</v>
       </c>
       <c r="D178">
-        <v>2966.871688417814</v>
+        <v>13942.82778271549</v>
       </c>
       <c r="E178">
-        <v>3044.077493176301</v>
+        <v>14713.17492592106</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -4092,16 +4089,16 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C179">
-        <v>4955.203939982344</v>
+        <v>17324.03456184319</v>
       </c>
       <c r="D179">
-        <v>4437.491921939725</v>
+        <v>13476.54727078326</v>
       </c>
       <c r="E179">
-        <v>4802.656681354792</v>
+        <v>22628.13038686703</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -4109,16 +4106,16 @@
         <v>182</v>
       </c>
       <c r="B180" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C180">
-        <v>5584.532853170555</v>
+        <v>2689.033001442709</v>
       </c>
       <c r="D180">
-        <v>3696.358431113311</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E180">
-        <v>5041.150517084573</v>
+        <v>2326.478289412053</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4126,16 +4123,16 @@
         <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C181">
-        <v>12228.85287007065</v>
+        <v>7330.001934671265</v>
       </c>
       <c r="D181">
-        <v>5315.793599021267</v>
+        <v>4696.892936408833</v>
       </c>
       <c r="E181">
-        <v>10793.64798057903</v>
+        <v>6336.909947377137</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -4143,16 +4140,16 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C182">
-        <v>3909.407627315059</v>
+        <v>3666.34991690552</v>
       </c>
       <c r="D182">
-        <v>12148.67547071851</v>
+        <v>2659.16265449915</v>
       </c>
       <c r="E182">
-        <v>24644.07599310096</v>
+        <v>3251.428044629679</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -4160,16 +4157,16 @@
         <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C183">
-        <v>2078.961774546943</v>
+        <v>3110.615608057638</v>
       </c>
       <c r="D183">
-        <v>1179.897477494976</v>
+        <v>2966.871688417814</v>
       </c>
       <c r="E183">
-        <v>1832.168256550158</v>
+        <v>3044.077493176301</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4177,16 +4174,16 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C184">
-        <v>932.8686753508275</v>
+        <v>4955.203939982344</v>
       </c>
       <c r="D184">
-        <v>920.6062716110156</v>
+        <v>4437.491921939725</v>
       </c>
       <c r="E184">
-        <v>0</v>
+        <v>4802.656681354792</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -4194,16 +4191,16 @@
         <v>187</v>
       </c>
       <c r="B185" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C185">
-        <v>195705.6</v>
+        <v>5584.532853170555</v>
       </c>
       <c r="D185">
-        <v>184867.2</v>
+        <v>3696.358431113311</v>
       </c>
       <c r="E185">
-        <v>187784</v>
+        <v>5041.150517084573</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -4211,16 +4208,16 @@
         <v>188</v>
       </c>
       <c r="B186" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C186">
-        <v>223624</v>
+        <v>12228.85287007065</v>
       </c>
       <c r="D186">
-        <v>205627.2</v>
+        <v>5315.793599021267</v>
       </c>
       <c r="E186">
-        <v>214700.8</v>
+        <v>10793.64798057903</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -4228,16 +4225,16 @@
         <v>189</v>
       </c>
       <c r="B187" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C187">
-        <v>253637.6</v>
+        <v>3909.407627315059</v>
       </c>
       <c r="D187">
-        <v>224994.4</v>
+        <v>12148.67547071851</v>
       </c>
       <c r="E187">
-        <v>242126.4</v>
+        <v>24644.07599310096</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -4245,16 +4242,16 @@
         <v>190</v>
       </c>
       <c r="B188" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C188">
-        <v>284854.4</v>
+        <v>2078.961774546943</v>
       </c>
       <c r="D188">
-        <v>242956.8</v>
+        <v>1179.897477494976</v>
       </c>
       <c r="E188">
-        <v>270748</v>
+        <v>1832.168256550158</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -4262,16 +4259,16 @@
         <v>191</v>
       </c>
       <c r="B189" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C189">
-        <v>275764.8</v>
+        <v>932.8686753508275</v>
       </c>
       <c r="D189">
-        <v>258018.4</v>
+        <v>920.6062716110156</v>
       </c>
       <c r="E189">
-        <v>296766.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -4279,16 +4276,16 @@
         <v>192</v>
       </c>
       <c r="B190" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C190">
-        <v>285775.2</v>
+        <v>195705.6</v>
       </c>
       <c r="D190">
-        <v>276530.4</v>
+        <v>184867.2</v>
       </c>
       <c r="E190">
-        <v>326134.4</v>
+        <v>187784</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4296,16 +4293,16 @@
         <v>193</v>
       </c>
       <c r="B191" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C191">
-        <v>195705.6</v>
+        <v>223624</v>
       </c>
       <c r="D191">
-        <v>184867.2</v>
+        <v>205627.2</v>
       </c>
       <c r="E191">
-        <v>187784</v>
+        <v>214700.8</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4313,16 +4310,16 @@
         <v>194</v>
       </c>
       <c r="B192" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C192">
-        <v>223624</v>
+        <v>253637.6</v>
       </c>
       <c r="D192">
-        <v>205627.2</v>
+        <v>224994.4</v>
       </c>
       <c r="E192">
-        <v>214700.8</v>
+        <v>242126.4</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4330,16 +4327,16 @@
         <v>195</v>
       </c>
       <c r="B193" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C193">
-        <v>253637.6</v>
+        <v>284854.4</v>
       </c>
       <c r="D193">
-        <v>224994.4</v>
+        <v>242956.8</v>
       </c>
       <c r="E193">
-        <v>242126.4</v>
+        <v>270748</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4347,16 +4344,16 @@
         <v>196</v>
       </c>
       <c r="B194" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C194">
-        <v>284854.4</v>
+        <v>275764.8</v>
       </c>
       <c r="D194">
-        <v>242956.8</v>
+        <v>258018.4</v>
       </c>
       <c r="E194">
-        <v>270748</v>
+        <v>296766.4</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -4364,16 +4361,16 @@
         <v>197</v>
       </c>
       <c r="B195" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C195">
-        <v>275764.8</v>
+        <v>285775.2</v>
       </c>
       <c r="D195">
-        <v>258018.4</v>
+        <v>276530.4</v>
       </c>
       <c r="E195">
-        <v>296766.4</v>
+        <v>326134.4</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -4381,16 +4378,16 @@
         <v>198</v>
       </c>
       <c r="B196" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C196">
-        <v>285775.2</v>
+        <v>181481.6</v>
       </c>
       <c r="D196">
-        <v>276530.4</v>
+        <v>171418.4</v>
       </c>
       <c r="E196">
-        <v>326134.4</v>
+        <v>173696</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4398,16 +4395,16 @@
         <v>199</v>
       </c>
       <c r="B197" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C197">
-        <v>181481.6</v>
+        <v>206952</v>
       </c>
       <c r="D197">
-        <v>171418.4</v>
+        <v>183019.2</v>
       </c>
       <c r="E197">
-        <v>173696</v>
+        <v>189584.8</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4415,16 +4412,16 @@
         <v>200</v>
       </c>
       <c r="B198" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C198">
-        <v>206952</v>
+        <v>236529.6</v>
       </c>
       <c r="D198">
-        <v>183019.2</v>
+        <v>204145.6</v>
       </c>
       <c r="E198">
-        <v>189584.8</v>
+        <v>217076.8</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4432,16 +4429,16 @@
         <v>201</v>
       </c>
       <c r="B199" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C199">
-        <v>236529.6</v>
+        <v>266166.4</v>
       </c>
       <c r="D199">
-        <v>204145.6</v>
+        <v>221178.4</v>
       </c>
       <c r="E199">
-        <v>217076.8</v>
+        <v>243465.6</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4449,16 +4446,16 @@
         <v>202</v>
       </c>
       <c r="B200" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C200">
-        <v>266166.4</v>
+        <v>266616</v>
       </c>
       <c r="D200">
-        <v>221178.4</v>
+        <v>234677.6</v>
       </c>
       <c r="E200">
-        <v>243465.6</v>
+        <v>267149.6</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4466,16 +4463,16 @@
         <v>203</v>
       </c>
       <c r="B201" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C201">
-        <v>266616</v>
+        <v>275787.2</v>
       </c>
       <c r="D201">
-        <v>234677.6</v>
+        <v>252004</v>
       </c>
       <c r="E201">
-        <v>267149.6</v>
+        <v>295416</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4483,16 +4480,16 @@
         <v>204</v>
       </c>
       <c r="B202" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C202">
-        <v>275787.2</v>
+        <v>166797.6</v>
       </c>
       <c r="D202">
-        <v>252004</v>
+        <v>173032.8</v>
       </c>
       <c r="E202">
-        <v>295416</v>
+        <v>175456.8</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4500,16 +4497,16 @@
         <v>205</v>
       </c>
       <c r="B203" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C203">
-        <v>166797.6</v>
+        <v>187860.8</v>
       </c>
       <c r="D203">
-        <v>173032.8</v>
+        <v>192721.6</v>
       </c>
       <c r="E203">
-        <v>175456.8</v>
+        <v>199666.4</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4517,16 +4514,16 @@
         <v>206</v>
       </c>
       <c r="B204" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C204">
-        <v>187860.8</v>
+        <v>214399.2</v>
       </c>
       <c r="D204">
-        <v>192721.6</v>
+        <v>208928.8</v>
       </c>
       <c r="E204">
-        <v>199666.4</v>
+        <v>221102.4</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4534,16 +4531,16 @@
         <v>207</v>
       </c>
       <c r="B205" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C205">
-        <v>214399.2</v>
+        <v>240393.6</v>
       </c>
       <c r="D205">
-        <v>208928.8</v>
+        <v>232657.6</v>
       </c>
       <c r="E205">
-        <v>221102.4</v>
+        <v>254091.2</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4551,16 +4548,16 @@
         <v>208</v>
       </c>
       <c r="B206" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C206">
-        <v>240393.6</v>
+        <v>266132</v>
       </c>
       <c r="D206">
-        <v>232657.6</v>
+        <v>251892</v>
       </c>
       <c r="E206">
-        <v>254091.2</v>
+        <v>284350.4</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -4568,32 +4565,15 @@
         <v>209</v>
       </c>
       <c r="B207" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C207">
-        <v>266132</v>
+        <v>277836.8</v>
       </c>
       <c r="D207">
-        <v>251892</v>
+        <v>271554.4</v>
       </c>
       <c r="E207">
-        <v>284350.4</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5">
-      <c r="A208" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B208" t="s">
-        <v>212</v>
-      </c>
-      <c r="C208">
-        <v>277836.8</v>
-      </c>
-      <c r="D208">
-        <v>271554.4</v>
-      </c>
-      <c r="E208">
         <v>316714.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - percentage growth BaseProjections age20_29
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df.xlsx
+++ b/create_forecast_basic/utils/monitoring_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="233">
   <si>
     <t>2020</t>
   </si>
@@ -128,6 +128,21 @@
   </si>
   <si>
     <t>percentage growth univ 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections age20_29 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections age20_29 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections age20_29 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections age20_29 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth BaseProjections age20_29 2045-2050</t>
   </si>
   <si>
     <t>SCHOOLDIST_5_2020</t>
@@ -1055,7 +1070,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E207"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1080,16 +1095,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1097,16 +1112,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1114,16 +1129,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E4" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1131,16 +1146,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1233,16 +1248,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E11" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1250,16 +1265,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D12" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E12" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1267,16 +1282,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="D13" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E13" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1284,16 +1299,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D14" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E14" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1301,16 +1316,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E15" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1318,16 +1333,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="D16" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="E16" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1488,7 +1503,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C26">
         <v>288</v>
@@ -1505,7 +1520,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C27">
         <v>110</v>
@@ -1522,7 +1537,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C28">
         <v>109</v>
@@ -1539,7 +1554,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C29">
         <v>109</v>
@@ -1556,7 +1571,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C30">
         <v>94</v>
@@ -1573,7 +1588,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -1590,7 +1605,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1607,7 +1622,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1624,7 +1639,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -1641,7 +1656,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1657,85 +1672,85 @@
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36">
-        <v>213239.3333333333</v>
+      <c r="B36" t="s">
+        <v>216</v>
       </c>
       <c r="C36">
-        <v>213239.3333333333</v>
+        <v>112</v>
       </c>
       <c r="D36">
-        <v>213239.3333333333</v>
+        <v>111</v>
       </c>
       <c r="E36">
-        <v>213239.3333333333</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B37">
-        <v>28627.66666666667</v>
+      <c r="B37" t="s">
+        <v>216</v>
       </c>
       <c r="C37">
-        <v>28627.66666666667</v>
+        <v>111</v>
       </c>
       <c r="D37">
-        <v>28627.66666666667</v>
+        <v>111</v>
       </c>
       <c r="E37">
-        <v>28627.66666666667</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B38">
-        <v>46063</v>
+      <c r="B38" t="s">
+        <v>216</v>
       </c>
       <c r="C38">
-        <v>46063</v>
+        <v>111</v>
       </c>
       <c r="D38">
-        <v>46063</v>
+        <v>108</v>
       </c>
       <c r="E38">
-        <v>46063</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B39">
-        <v>23828</v>
+      <c r="B39" t="s">
+        <v>216</v>
       </c>
       <c r="C39">
-        <v>23828</v>
+        <v>116</v>
       </c>
       <c r="D39">
-        <v>23828</v>
+        <v>108</v>
       </c>
       <c r="E39">
-        <v>23828</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B40">
-        <v>8538</v>
+      <c r="B40" t="s">
+        <v>216</v>
       </c>
       <c r="C40">
-        <v>8538</v>
+        <v>106</v>
       </c>
       <c r="D40">
-        <v>8538</v>
+        <v>108</v>
       </c>
       <c r="E40">
-        <v>8538</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1743,16 +1758,16 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="C41">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="D41">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="E41">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1760,16 +1775,16 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>21988.00000000001</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="C42">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="D42">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="E42">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1777,16 +1792,16 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="C43">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="D43">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="E43">
-        <v>27262</v>
+        <v>46063</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1794,16 +1809,16 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="C44">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="D44">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="E44">
-        <v>2804</v>
+        <v>23828</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1811,16 +1826,16 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="C45">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="D45">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="E45">
-        <v>1331</v>
+        <v>8538</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1828,16 +1843,16 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="C46">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="D46">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="E46">
-        <v>7375</v>
+        <v>5048</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1845,16 +1860,16 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>8805</v>
+        <v>21988.00000000001</v>
       </c>
       <c r="C47">
-        <v>8805</v>
+        <v>21988</v>
       </c>
       <c r="D47">
-        <v>8805</v>
+        <v>21988</v>
       </c>
       <c r="E47">
-        <v>8805</v>
+        <v>21988</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1862,16 +1877,16 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="C48">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="D48">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="E48">
-        <v>1218</v>
+        <v>27262</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1879,16 +1894,16 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="C49">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="D49">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="E49">
-        <v>1673</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1896,16 +1911,16 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="C50">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="D50">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="E50">
-        <v>2401</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1913,16 +1928,16 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="C51">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="D51">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="E51">
-        <v>2488</v>
+        <v>7375</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1930,16 +1945,16 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="C52">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="D52">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="E52">
-        <v>2148</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1947,16 +1962,16 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="C53">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="D53">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="E53">
-        <v>3242</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1964,16 +1979,16 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="C54">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="D54">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="E54">
-        <v>3637</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1981,16 +1996,16 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="C55">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="D55">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="E55">
-        <v>301</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1998,16 +2013,16 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="C56">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="D56">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="E56">
-        <v>537</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2015,101 +2030,101 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="C57">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="D57">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="E57">
-        <v>300</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B58" t="s">
-        <v>211</v>
+      <c r="B58">
+        <v>3242</v>
       </c>
       <c r="C58">
-        <v>285733.3218235314</v>
+        <v>3242</v>
       </c>
       <c r="D58">
-        <v>274161.0000038777</v>
+        <v>3242</v>
       </c>
       <c r="E58">
-        <v>275663.3373324008</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B59" t="s">
-        <v>211</v>
+      <c r="B59">
+        <v>3637</v>
       </c>
       <c r="C59">
-        <v>36057.66373063793</v>
+        <v>3637</v>
       </c>
       <c r="D59">
-        <v>33344.22909790605</v>
+        <v>3637</v>
       </c>
       <c r="E59">
-        <v>34286.84568702983</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B60" t="s">
-        <v>211</v>
+      <c r="B60">
+        <v>301</v>
       </c>
       <c r="C60">
-        <v>66822.51137331135</v>
+        <v>301</v>
       </c>
       <c r="D60">
-        <v>61855.23107261454</v>
+        <v>301</v>
       </c>
       <c r="E60">
-        <v>63948.66570649843</v>
+        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B61" t="s">
-        <v>211</v>
+      <c r="B61">
+        <v>537</v>
       </c>
       <c r="C61">
-        <v>33156.30459804353</v>
+        <v>537</v>
       </c>
       <c r="D61">
-        <v>33335.50923218194</v>
+        <v>537</v>
       </c>
       <c r="E61">
-        <v>33397.07322472375</v>
+        <v>537</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B62" t="s">
-        <v>211</v>
+      <c r="B62">
+        <v>300</v>
       </c>
       <c r="C62">
-        <v>9986.417617537509</v>
+        <v>300</v>
       </c>
       <c r="D62">
-        <v>10194.62059102478</v>
+        <v>300</v>
       </c>
       <c r="E62">
-        <v>10338.40358091756</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2117,16 +2132,16 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C63">
-        <v>8306.813376518987</v>
+        <v>285733.3218235314</v>
       </c>
       <c r="D63">
-        <v>6946.591660718233</v>
+        <v>274161.0000038777</v>
       </c>
       <c r="E63">
-        <v>8135.667377017133</v>
+        <v>275663.3373324008</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2134,16 +2149,16 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C64">
-        <v>29427.44116169451</v>
+        <v>36057.66373063793</v>
       </c>
       <c r="D64">
-        <v>30953.22576377643</v>
+        <v>33344.22909790605</v>
       </c>
       <c r="E64">
-        <v>31386.31536916655</v>
+        <v>34286.84568702983</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2151,16 +2166,16 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C65">
-        <v>37145.33462606892</v>
+        <v>66822.51137331135</v>
       </c>
       <c r="D65">
-        <v>39041.11738664036</v>
+        <v>61855.23107261454</v>
       </c>
       <c r="E65">
-        <v>40239.51136715176</v>
+        <v>63948.66570649843</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2168,16 +2183,16 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C66">
-        <v>5309.478782988256</v>
+        <v>33156.30459804353</v>
       </c>
       <c r="D66">
-        <v>5060.408660766857</v>
+        <v>33335.50923218194</v>
       </c>
       <c r="E66">
-        <v>5201.12526897965</v>
+        <v>33397.07322472375</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2185,16 +2200,16 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C67">
-        <v>5521.895631861405</v>
+        <v>9986.417617537509</v>
       </c>
       <c r="D67">
-        <v>6073.616715538182</v>
+        <v>10194.62059102478</v>
       </c>
       <c r="E67">
-        <v>6265.692004112236</v>
+        <v>10338.40358091756</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2202,16 +2217,16 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C68">
-        <v>7012.74256878429</v>
+        <v>8306.813376518987</v>
       </c>
       <c r="D68">
-        <v>6467.15326810131</v>
+        <v>6946.591660718233</v>
       </c>
       <c r="E68">
-        <v>6547.602648720247</v>
+        <v>8135.667377017133</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2219,16 +2234,16 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C69">
-        <v>7317.313641591267</v>
+        <v>29427.44116169451</v>
       </c>
       <c r="D69">
-        <v>7240.499364931959</v>
+        <v>30953.22576377643</v>
       </c>
       <c r="E69">
-        <v>7309.076098225414</v>
+        <v>31386.31536916655</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2236,16 +2251,16 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C70">
-        <v>2166.404734331622</v>
+        <v>37145.33462606892</v>
       </c>
       <c r="D70">
-        <v>2013.947393383935</v>
+        <v>39041.11738664036</v>
       </c>
       <c r="E70">
-        <v>2067.009181064854</v>
+        <v>40239.51136715176</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2253,16 +2268,16 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C71">
-        <v>3081.965248662672</v>
+        <v>5309.478782988256</v>
       </c>
       <c r="D71">
-        <v>3137.447595991872</v>
+        <v>5060.408660766857</v>
       </c>
       <c r="E71">
-        <v>3186.615419267629</v>
+        <v>5201.12526897965</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2270,16 +2285,16 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C72">
-        <v>443.1341918519325</v>
+        <v>5521.895631861405</v>
       </c>
       <c r="D72">
-        <v>421.887538681912</v>
+        <v>6073.616715538182</v>
       </c>
       <c r="E72">
-        <v>433.4544189987498</v>
+        <v>6265.692004112236</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2287,16 +2302,16 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C73">
-        <v>2895.085614458657</v>
+        <v>7012.74256878429</v>
       </c>
       <c r="D73">
-        <v>2909.362870154178</v>
+        <v>6467.15326810131</v>
       </c>
       <c r="E73">
-        <v>2924.168116891962</v>
+        <v>6547.602648720247</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2304,16 +2319,16 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C74">
-        <v>3653.831655445544</v>
+        <v>7317.313641591267</v>
       </c>
       <c r="D74">
-        <v>3598.638480494133</v>
+        <v>7240.499364931959</v>
       </c>
       <c r="E74">
-        <v>3616.404971165329</v>
+        <v>7309.076098225414</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2321,16 +2336,16 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C75">
-        <v>3542.454003930634</v>
+        <v>2166.404734331622</v>
       </c>
       <c r="D75">
-        <v>3648.230892236539</v>
+        <v>2013.947393383935</v>
       </c>
       <c r="E75">
-        <v>3678.324608989895</v>
+        <v>2067.009181064854</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2338,16 +2353,16 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C76">
-        <v>4257.401768859199</v>
+        <v>3081.965248662672</v>
       </c>
       <c r="D76">
-        <v>4324.862744573556</v>
+        <v>3137.447595991872</v>
       </c>
       <c r="E76">
-        <v>4363.718311116243</v>
+        <v>3186.615419267629</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2355,16 +2370,16 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C77">
-        <v>881.1481005457115</v>
+        <v>443.1341918519325</v>
       </c>
       <c r="D77">
-        <v>922.4946308419028</v>
+        <v>421.887538681912</v>
       </c>
       <c r="E77">
-        <v>951.6553445648265</v>
+        <v>433.4544189987498</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2372,16 +2387,16 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C78">
-        <v>911.7413777070067</v>
+        <v>2895.085614458657</v>
       </c>
       <c r="D78">
-        <v>868.7478168054034</v>
+        <v>2909.362870154178</v>
       </c>
       <c r="E78">
-        <v>883.9572064300576</v>
+        <v>2924.168116891962</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2389,16 +2404,16 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>3653.831655445544</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>3598.638480494133</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>3616.404971165329</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2406,16 +2421,16 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C80">
-        <v>310887.0551086462</v>
+        <v>3542.454003930634</v>
       </c>
       <c r="D80">
-        <v>290797.302000507</v>
+        <v>3648.230892236539</v>
       </c>
       <c r="E80">
-        <v>292306.0034436272</v>
+        <v>3678.324608989895</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2423,16 +2438,16 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C81">
-        <v>51074.32436027069</v>
+        <v>4257.401768859199</v>
       </c>
       <c r="D81">
-        <v>26072.86402002085</v>
+        <v>4324.862744573556</v>
       </c>
       <c r="E81">
-        <v>44744.53526801307</v>
+        <v>4363.718311116243</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2440,16 +2455,16 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C82">
-        <v>84109.82719823082</v>
+        <v>881.1481005457115</v>
       </c>
       <c r="D82">
-        <v>77937.73156609248</v>
+        <v>922.4946308419028</v>
       </c>
       <c r="E82">
-        <v>84581.97612214876</v>
+        <v>951.6553445648265</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2457,16 +2472,16 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C83">
-        <v>39310.49274971832</v>
+        <v>911.7413777070067</v>
       </c>
       <c r="D83">
-        <v>38683.92515358835</v>
+        <v>868.7478168054034</v>
       </c>
       <c r="E83">
-        <v>38875.73769831542</v>
+        <v>883.9572064300576</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2474,16 +2489,16 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C84">
-        <v>11932.38400809033</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>10681.35241281803</v>
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>11035.70441498311</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2491,16 +2506,16 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C85">
-        <v>9548.28031721313</v>
+        <v>310887.0551086462</v>
       </c>
       <c r="D85">
-        <v>7703.305735153427</v>
+        <v>290797.302000507</v>
       </c>
       <c r="E85">
-        <v>8161.797271070729</v>
+        <v>292306.0034436272</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2508,16 +2523,16 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C86">
-        <v>35810.66989709945</v>
+        <v>51074.32436027069</v>
       </c>
       <c r="D86">
-        <v>36601.69575249061</v>
+        <v>26072.86402002085</v>
       </c>
       <c r="E86">
-        <v>39241.8615517352</v>
+        <v>44744.53526801307</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2525,16 +2540,16 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C87">
-        <v>40274.91199119319</v>
+        <v>84109.82719823082</v>
       </c>
       <c r="D87">
-        <v>41351.35312049399</v>
+        <v>77937.73156609248</v>
       </c>
       <c r="E87">
-        <v>44632.82113421193</v>
+        <v>84581.97612214876</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2542,16 +2557,16 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C88">
-        <v>5702.582508173264</v>
+        <v>39310.49274971832</v>
       </c>
       <c r="D88">
-        <v>5197.04316560074</v>
+        <v>38683.92515358835</v>
       </c>
       <c r="E88">
-        <v>5490.350510109492</v>
+        <v>38875.73769831542</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2559,16 +2574,16 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C89">
-        <v>6531.454941380145</v>
+        <v>11932.38400809033</v>
       </c>
       <c r="D89">
-        <v>6914.424310549415</v>
+        <v>10681.35241281803</v>
       </c>
       <c r="E89">
-        <v>7565.494786531661</v>
+        <v>11035.70441498311</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2576,16 +2591,16 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C90">
-        <v>11086.07248419944</v>
+        <v>9548.28031721313</v>
       </c>
       <c r="D90">
-        <v>9081.046501582416</v>
+        <v>7703.305735153427</v>
       </c>
       <c r="E90">
-        <v>9712.39919620127</v>
+        <v>8161.797271070729</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2593,16 +2608,16 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C91">
-        <v>11235.01770760014</v>
+        <v>35810.66989709945</v>
       </c>
       <c r="D91">
-        <v>7294.264487669744</v>
+        <v>36601.69575249061</v>
       </c>
       <c r="E91">
-        <v>7393.954728795917</v>
+        <v>39241.8615517352</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2610,16 +2625,16 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C92">
-        <v>2313.18743770475</v>
+        <v>40274.91199119319</v>
       </c>
       <c r="D92">
-        <v>2050.379609518187</v>
+        <v>41351.35312049399</v>
       </c>
       <c r="E92">
-        <v>2158.015018647229</v>
+        <v>44632.82113421193</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2627,16 +2642,16 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C93">
-        <v>4487.422497745161</v>
+        <v>5702.582508173264</v>
       </c>
       <c r="D93">
-        <v>3251.340662315742</v>
+        <v>5197.04316560074</v>
       </c>
       <c r="E93">
-        <v>3680.595601936531</v>
+        <v>5490.350510109492</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2644,16 +2659,16 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C94">
-        <v>3291.571394333075</v>
+        <v>6531.454941380145</v>
       </c>
       <c r="D94">
-        <v>453.0691373312048</v>
+        <v>6914.424310549415</v>
       </c>
       <c r="E94">
-        <v>505.4945456516502</v>
+        <v>7565.494786531661</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2661,16 +2676,16 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C95">
-        <v>2962.271032197586</v>
+        <v>11086.07248419944</v>
       </c>
       <c r="D95">
-        <v>2922.939603860779</v>
+        <v>9081.046501582416</v>
       </c>
       <c r="E95">
-        <v>2944.717615440521</v>
+        <v>9712.39919620127</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2678,16 +2693,16 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C96">
-        <v>3978.851277647058</v>
+        <v>11235.01770760014</v>
       </c>
       <c r="D96">
-        <v>1566.476580450332</v>
+        <v>7294.264487669744</v>
       </c>
       <c r="E96">
-        <v>1592.42779801514</v>
+        <v>7393.954728795917</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2695,16 +2710,16 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C97">
-        <v>3624.875154413226</v>
+        <v>2313.18743770475</v>
       </c>
       <c r="D97">
-        <v>3677.660725632635</v>
+        <v>2050.379609518187</v>
       </c>
       <c r="E97">
-        <v>3727.402937205914</v>
+        <v>2158.015018647229</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2712,16 +2727,16 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C98">
-        <v>4499.453713305816</v>
+        <v>4487.422497745161</v>
       </c>
       <c r="D98">
-        <v>4389.339541465134</v>
+        <v>3251.340662315742</v>
       </c>
       <c r="E98">
-        <v>4489.156966460471</v>
+        <v>3680.595601936531</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2729,16 +2744,16 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C99">
-        <v>1176.375213333053</v>
+        <v>3291.571394333075</v>
       </c>
       <c r="D99">
-        <v>1229.853805184373</v>
+        <v>453.0691373312048</v>
       </c>
       <c r="E99">
-        <v>1330.656790249233</v>
+        <v>505.4945456516502</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2746,16 +2761,16 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C100">
-        <v>1013.219479989464</v>
+        <v>2962.271032197586</v>
       </c>
       <c r="D100">
-        <v>873.6169022987777</v>
+        <v>2922.939603860779</v>
       </c>
       <c r="E100">
-        <v>911.1327501980686</v>
+        <v>2944.717615440521</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2763,16 +2778,16 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C101">
-        <v>857.2621118872319</v>
+        <v>3978.851277647058</v>
       </c>
       <c r="D101">
-        <v>772.2734198315197</v>
+        <v>1566.476580450332</v>
       </c>
       <c r="E101">
-        <v>801.0018403865388</v>
+        <v>1592.42779801514</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2780,16 +2795,16 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C102">
-        <v>345179.8540918057</v>
+        <v>3624.875154413226</v>
       </c>
       <c r="D102">
-        <v>306070.7824845224</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E102">
-        <v>311915.8222954976</v>
+        <v>3727.402937205914</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2797,16 +2812,16 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C103">
-        <v>57843.05696310467</v>
+        <v>4499.453713305816</v>
       </c>
       <c r="D103">
-        <v>41761.14805054816</v>
+        <v>4389.339541465134</v>
       </c>
       <c r="E103">
-        <v>48660.60638720006</v>
+        <v>4489.156966460471</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2814,16 +2829,16 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C104">
-        <v>106400.8113634808</v>
+        <v>1176.375213333053</v>
       </c>
       <c r="D104">
-        <v>97376.26626200562</v>
+        <v>1229.853805184373</v>
       </c>
       <c r="E104">
-        <v>107457.7153467231</v>
+        <v>1330.656790249233</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2831,16 +2846,16 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C105">
-        <v>47754.67592555143</v>
+        <v>1013.219479989464</v>
       </c>
       <c r="D105">
-        <v>46917.82385382168</v>
+        <v>873.6169022987777</v>
       </c>
       <c r="E105">
-        <v>47285.0706371487</v>
+        <v>911.1327501980686</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2848,16 +2863,16 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C106">
-        <v>13642.04328300475</v>
+        <v>857.2621118872319</v>
       </c>
       <c r="D106">
-        <v>12594.12090677959</v>
+        <v>772.2734198315197</v>
       </c>
       <c r="E106">
-        <v>14151.68818183644</v>
+        <v>801.0018403865388</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2865,16 +2880,16 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C107">
-        <v>10166.68671320246</v>
+        <v>345179.8540918057</v>
       </c>
       <c r="D107">
-        <v>7870.660600118454</v>
+        <v>306070.7824845224</v>
       </c>
       <c r="E107">
-        <v>8448.569974010888</v>
+        <v>311915.8222954976</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2882,16 +2897,16 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C108">
-        <v>40056.29615048355</v>
+        <v>57843.05696310467</v>
       </c>
       <c r="D108">
-        <v>39938.78970433185</v>
+        <v>41761.14805054816</v>
       </c>
       <c r="E108">
-        <v>44520.15917103966</v>
+        <v>48660.60638720006</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2899,16 +2914,16 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C109">
-        <v>42099.78280750295</v>
+        <v>106400.8113634808</v>
       </c>
       <c r="D109">
-        <v>42299.87775020443</v>
+        <v>97376.26626200562</v>
       </c>
       <c r="E109">
-        <v>47328.28098195308</v>
+        <v>107457.7153467231</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2916,16 +2931,16 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C110">
-        <v>6780.581746217548</v>
+        <v>47754.67592555143</v>
       </c>
       <c r="D110">
-        <v>5344.462556042371</v>
+        <v>46917.82385382168</v>
       </c>
       <c r="E110">
-        <v>5852.587839854697</v>
+        <v>47285.0706371487</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2933,16 +2948,16 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C111">
-        <v>7052.041776574091</v>
+        <v>13642.04328300475</v>
       </c>
       <c r="D111">
-        <v>2387.833946905571</v>
+        <v>12594.12090677959</v>
       </c>
       <c r="E111">
-        <v>2653.360912751024</v>
+        <v>14151.68818183644</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2950,16 +2965,16 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C112">
-        <v>12491.64080553533</v>
+        <v>10166.68671320246</v>
       </c>
       <c r="D112">
-        <v>7553.961214696117</v>
+        <v>7870.660600118454</v>
       </c>
       <c r="E112">
-        <v>8823.015551678049</v>
+        <v>8448.569974010888</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2967,16 +2982,16 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C113">
-        <v>11918.07029478611</v>
+        <v>40056.29615048355</v>
       </c>
       <c r="D113">
-        <v>10755.76769609013</v>
+        <v>39938.78970433185</v>
       </c>
       <c r="E113">
-        <v>11073.8263395291</v>
+        <v>44520.15917103966</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2984,16 +2999,16 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C114">
-        <v>2510.791313969085</v>
+        <v>42099.78280750295</v>
       </c>
       <c r="D114">
-        <v>2080.311820058766</v>
+        <v>42299.87775020443</v>
       </c>
       <c r="E114">
-        <v>2225.787307207039</v>
+        <v>47328.28098195308</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3001,16 +3016,16 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C115">
-        <v>5559.189168957029</v>
+        <v>6780.581746217548</v>
       </c>
       <c r="D115">
-        <v>3507.429258284409</v>
+        <v>5344.462556042371</v>
       </c>
       <c r="E115">
-        <v>4514.632917614302</v>
+        <v>5852.587839854697</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3018,16 +3033,16 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C116">
-        <v>3740.698985412615</v>
+        <v>7052.041776574091</v>
       </c>
       <c r="D116">
-        <v>456.0519360615073</v>
+        <v>2387.833946905571</v>
       </c>
       <c r="E116">
-        <v>595.516072795263</v>
+        <v>2653.360912751024</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3035,16 +3050,16 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C117">
-        <v>3025.982972811596</v>
+        <v>12491.64080553533</v>
       </c>
       <c r="D117">
-        <v>2930.200017528361</v>
+        <v>7553.961214696117</v>
       </c>
       <c r="E117">
-        <v>2972.156458241908</v>
+        <v>8823.015551678049</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3052,16 +3067,16 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C118">
-        <v>4384.134004159239</v>
+        <v>11918.07029478611</v>
       </c>
       <c r="D118">
-        <v>3877.68979844253</v>
+        <v>10755.76769609013</v>
       </c>
       <c r="E118">
-        <v>3984.413723700878</v>
+        <v>11073.8263395291</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3069,16 +3084,16 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C119">
-        <v>3818.113674370041</v>
+        <v>2510.791313969085</v>
       </c>
       <c r="D119">
-        <v>3677.660725632635</v>
+        <v>2080.311820058766</v>
       </c>
       <c r="E119">
-        <v>3773.270697207371</v>
+        <v>2225.787307207039</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3086,16 +3101,16 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C120">
-        <v>5697.549039481555</v>
+        <v>5559.189168957029</v>
       </c>
       <c r="D120">
-        <v>4449.270708440607</v>
+        <v>3507.429258284409</v>
       </c>
       <c r="E120">
-        <v>4794.85366801385</v>
+        <v>4514.632917614302</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3103,16 +3118,16 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C121">
-        <v>1675.03137312741</v>
+        <v>3740.698985412615</v>
       </c>
       <c r="D121">
-        <v>1815.4386330182</v>
+        <v>456.0519360615073</v>
       </c>
       <c r="E121">
-        <v>2049.263941768266</v>
+        <v>595.516072795263</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3120,16 +3135,16 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C122">
-        <v>1388.615296125427</v>
+        <v>3025.982972811596</v>
       </c>
       <c r="D122">
-        <v>898.8243487684732</v>
+        <v>2930.200017528361</v>
       </c>
       <c r="E122">
-        <v>1101.853615098803</v>
+        <v>2972.156458241908</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3137,16 +3152,16 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C123">
-        <v>915.4210068592286</v>
+        <v>4384.134004159239</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>3877.68979844253</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>3984.413723700878</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3154,16 +3169,16 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C124">
-        <v>379833.2126030341</v>
+        <v>3818.113674370041</v>
       </c>
       <c r="D124">
-        <v>323789.1870151541</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E124">
-        <v>342305.1273678984</v>
+        <v>3773.270697207371</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3171,16 +3186,16 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C125">
-        <v>66636.46327624648</v>
+        <v>5697.549039481555</v>
       </c>
       <c r="D125">
-        <v>57885.11081377808</v>
+        <v>4449.270708440607</v>
       </c>
       <c r="E125">
-        <v>65450.5214985832</v>
+        <v>4794.85366801385</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3188,16 +3203,16 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C126">
-        <v>122447.4212601383</v>
+        <v>1675.03137312741</v>
       </c>
       <c r="D126">
-        <v>106273.0478090824</v>
+        <v>1815.4386330182</v>
       </c>
       <c r="E126">
-        <v>119530.3850553175</v>
+        <v>2049.263941768266</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3205,16 +3220,16 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C127">
-        <v>55098.14072490651</v>
+        <v>1388.615296125427</v>
       </c>
       <c r="D127">
-        <v>53997.08352943832</v>
+        <v>898.8243487684732</v>
       </c>
       <c r="E127">
-        <v>54429.29718809373</v>
+        <v>1101.853615098803</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3222,16 +3237,16 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C128">
-        <v>17436.20392355449</v>
+        <v>915.4210068592286</v>
       </c>
       <c r="D128">
-        <v>19678.07818882393</v>
+        <v>0</v>
       </c>
       <c r="E128">
-        <v>23411.63616688988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3239,16 +3254,16 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C129">
-        <v>11477.1443269179</v>
+        <v>379833.2126030341</v>
       </c>
       <c r="D129">
-        <v>7941.17271971979</v>
+        <v>323789.1870151541</v>
       </c>
       <c r="E129">
-        <v>8685.454438123739</v>
+        <v>342305.1273678984</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3256,16 +3271,16 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C130">
-        <v>44788.85407568982</v>
+        <v>66636.46327624648</v>
       </c>
       <c r="D130">
-        <v>42290.86139964137</v>
+        <v>57885.11081377808</v>
       </c>
       <c r="E130">
-        <v>48116.24030242601</v>
+        <v>65450.5214985832</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3273,16 +3288,16 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C131">
-        <v>43854.83257609577</v>
+        <v>122447.4212601383</v>
       </c>
       <c r="D131">
-        <v>42446.11108034404</v>
+        <v>106273.0478090824</v>
       </c>
       <c r="E131">
-        <v>48048.47217811201</v>
+        <v>119530.3850553175</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3290,16 +3305,16 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C132">
-        <v>7818.02330571639</v>
+        <v>55098.14072490651</v>
       </c>
       <c r="D132">
-        <v>5653.095564499369</v>
+        <v>53997.08352943832</v>
       </c>
       <c r="E132">
-        <v>6625.371912088781</v>
+        <v>54429.29718809373</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3307,16 +3322,16 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C133">
-        <v>8085.182658295945</v>
+        <v>17436.20392355449</v>
       </c>
       <c r="D133">
-        <v>7503.614943774021</v>
+        <v>19678.07818882393</v>
       </c>
       <c r="E133">
-        <v>8938.0868588093</v>
+        <v>23411.63616688988</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3324,16 +3339,16 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C134">
-        <v>14492.94704346139</v>
+        <v>11477.1443269179</v>
       </c>
       <c r="D134">
-        <v>11209.84775023005</v>
+        <v>7941.17271971979</v>
       </c>
       <c r="E134">
-        <v>10752.42132399964</v>
+        <v>8685.454438123739</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3341,16 +3356,16 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C135">
-        <v>14025.08468897277</v>
+        <v>44788.85407568982</v>
       </c>
       <c r="D135">
-        <v>11232.84453326727</v>
+        <v>42290.86139964137</v>
       </c>
       <c r="E135">
-        <v>12584.87999504888</v>
+        <v>48116.24030242601</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3358,16 +3373,16 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C136">
-        <v>2660.082565212768</v>
+        <v>43854.83257609577</v>
       </c>
       <c r="D136">
-        <v>2118.88338047299</v>
+        <v>42446.11108034404</v>
       </c>
       <c r="E136">
-        <v>2317.74860784036</v>
+        <v>48048.47217811201</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3375,16 +3390,16 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C137">
-        <v>6699.919359426849</v>
+        <v>7818.02330571639</v>
       </c>
       <c r="D137">
-        <v>3926.964562863937</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E137">
-        <v>5419.280756815793</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3392,16 +3407,16 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C138">
-        <v>4240.498957073307</v>
+        <v>8085.182658295945</v>
       </c>
       <c r="D138">
-        <v>2799.802017040321</v>
+        <v>7503.614943774021</v>
       </c>
       <c r="E138">
-        <v>3370.629266244694</v>
+        <v>8938.0868588093</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3409,16 +3424,16 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C139">
-        <v>3104.11640049039</v>
+        <v>14492.94704346139</v>
       </c>
       <c r="D139">
-        <v>2945.585161856526</v>
+        <v>11209.84775023005</v>
       </c>
       <c r="E139">
-        <v>3032.000269374993</v>
+        <v>10752.42132399964</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3426,16 +3441,16 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C140">
-        <v>4758.923090909089</v>
+        <v>14025.08468897277</v>
       </c>
       <c r="D140">
-        <v>4052.36859619171</v>
+        <v>11232.84453326727</v>
       </c>
       <c r="E140">
-        <v>4241.271500156832</v>
+        <v>12584.87999504888</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3443,16 +3458,16 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C141">
-        <v>4582.423026269129</v>
+        <v>2660.082565212768</v>
       </c>
       <c r="D141">
-        <v>3677.660725632635</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E141">
-        <v>3936.041511138754</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3460,16 +3475,16 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C142">
-        <v>8274.311032145955</v>
+        <v>6699.919359426849</v>
       </c>
       <c r="D142">
-        <v>4554.906523253632</v>
+        <v>3926.964562863937</v>
       </c>
       <c r="E142">
-        <v>6530.74208924048</v>
+        <v>5419.280756815793</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3477,16 +3492,16 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C143">
-        <v>2362.496887971177</v>
+        <v>4240.498957073307</v>
       </c>
       <c r="D143">
-        <v>4552.94161730676</v>
+        <v>2799.802017040321</v>
       </c>
       <c r="E143">
-        <v>7699.768813994026</v>
+        <v>3370.629266244694</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3494,16 +3509,16 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C144">
-        <v>1764.352253203638</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D144">
-        <v>974.5725435688446</v>
+        <v>2945.585161856526</v>
       </c>
       <c r="E144">
-        <v>1393.90973989574</v>
+        <v>3032.000269374993</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3511,16 +3526,16 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C145">
-        <v>921.2368963564281</v>
+        <v>4758.923090909089</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>4052.36859619171</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>4241.271500156832</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3528,16 +3543,16 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C146">
-        <v>409436.7691592983</v>
+        <v>4582.423026269129</v>
       </c>
       <c r="D146">
-        <v>355341.7534723968</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E146">
-        <v>387999.3260030203</v>
+        <v>3936.041511138754</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3545,16 +3560,16 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C147">
-        <v>66424.65479531829</v>
+        <v>8274.311032145955</v>
       </c>
       <c r="D147">
-        <v>67311.96044664056</v>
+        <v>4554.906523253632</v>
       </c>
       <c r="E147">
-        <v>76231.77993843338</v>
+        <v>6530.74208924048</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3562,16 +3577,16 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C148">
-        <v>125858.7401545331</v>
+        <v>2362.496887971177</v>
       </c>
       <c r="D148">
-        <v>95923.88790038624</v>
+        <v>4552.94161730676</v>
       </c>
       <c r="E148">
-        <v>124140.5773429784</v>
+        <v>7699.768813994026</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3579,16 +3594,16 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C149">
-        <v>55158.37308241575</v>
+        <v>1764.352253203638</v>
       </c>
       <c r="D149">
-        <v>54194.17670445503</v>
+        <v>974.5725435688446</v>
       </c>
       <c r="E149">
-        <v>54731.6463609033</v>
+        <v>1393.90973989574</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3596,16 +3611,16 @@
         <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C150">
-        <v>18810.64774314864</v>
+        <v>921.2368963564281</v>
       </c>
       <c r="D150">
-        <v>26985.75868185313</v>
+        <v>0</v>
       </c>
       <c r="E150">
-        <v>33814.25416223275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -3613,16 +3628,16 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C151">
-        <v>11786.58854248258</v>
+        <v>409436.7691592983</v>
       </c>
       <c r="D151">
-        <v>9267.503482344102</v>
+        <v>355341.7534723968</v>
       </c>
       <c r="E151">
-        <v>10151.93626108859</v>
+        <v>387999.3260030203</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3630,16 +3645,16 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C152">
-        <v>41809.31820607139</v>
+        <v>66424.65479531829</v>
       </c>
       <c r="D152">
-        <v>39732.01918427406</v>
+        <v>67311.96044664056</v>
       </c>
       <c r="E152">
-        <v>46033.76592047335</v>
+        <v>76231.77993843338</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3647,16 +3662,16 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C153">
-        <v>44322.79570608526</v>
+        <v>125858.7401545331</v>
       </c>
       <c r="D153">
-        <v>42997.62304068729</v>
+        <v>95923.88790038624</v>
       </c>
       <c r="E153">
-        <v>49150.09462369821</v>
+        <v>124140.5773429784</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3664,16 +3679,16 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C154">
-        <v>7830.871226366395</v>
+        <v>55158.37308241575</v>
       </c>
       <c r="D154">
-        <v>5653.095564499369</v>
+        <v>54194.17670445503</v>
       </c>
       <c r="E154">
-        <v>6625.371912088781</v>
+        <v>54731.6463609033</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3681,16 +3696,16 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C155">
-        <v>8817.535269776827</v>
+        <v>18810.64774314864</v>
       </c>
       <c r="D155">
-        <v>9011.059942949789</v>
+        <v>26985.75868185313</v>
       </c>
       <c r="E155">
-        <v>10838.71267389012</v>
+        <v>33814.25416223275</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3698,16 +3713,16 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C156">
-        <v>15730.7337703995</v>
+        <v>11786.58854248258</v>
       </c>
       <c r="D156">
-        <v>12870.92751701806</v>
+        <v>9267.503482344102</v>
       </c>
       <c r="E156">
-        <v>16028.57827823479</v>
+        <v>10151.93626108859</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3715,16 +3730,16 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C157">
-        <v>14763.70638988416</v>
+        <v>41809.31820607139</v>
       </c>
       <c r="D157">
-        <v>11353.82086139094</v>
+        <v>39732.01918427406</v>
       </c>
       <c r="E157">
-        <v>15744.22408353954</v>
+        <v>46033.76592047335</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3732,16 +3747,16 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C158">
-        <v>2664.581838046233</v>
+        <v>44322.79570608526</v>
       </c>
       <c r="D158">
-        <v>2118.88338047299</v>
+        <v>42997.62304068729</v>
       </c>
       <c r="E158">
-        <v>2317.74860784036</v>
+        <v>49150.09462369821</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3749,16 +3764,16 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C159">
-        <v>7118.299388486004</v>
+        <v>7830.871226366395</v>
       </c>
       <c r="D159">
-        <v>4387.796042371227</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E159">
-        <v>6214.950571608244</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3766,16 +3781,16 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C160">
-        <v>1256.930682890124</v>
+        <v>8817.535269776827</v>
       </c>
       <c r="D160">
-        <v>634.2799162905493</v>
+        <v>9011.059942949789</v>
       </c>
       <c r="E160">
-        <v>1060.520130278657</v>
+        <v>10838.71267389012</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3783,16 +3798,16 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C161">
-        <v>3104.11640049039</v>
+        <v>15730.7337703995</v>
       </c>
       <c r="D161">
-        <v>2953.473502833881</v>
+        <v>12870.92751701806</v>
       </c>
       <c r="E161">
-        <v>3032.074436227733</v>
+        <v>16028.57827823479</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3800,16 +3815,16 @@
         <v>164</v>
       </c>
       <c r="B162" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>14763.70638988416</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>11353.82086139094</v>
       </c>
       <c r="E162">
-        <v>1927.316250691574</v>
+        <v>15744.22408353954</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3817,16 +3832,16 @@
         <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C163">
-        <v>4982.658106436934</v>
+        <v>2664.581838046233</v>
       </c>
       <c r="D163">
-        <v>3682.745087885083</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E163">
-        <v>4606.149113368056</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3834,16 +3849,16 @@
         <v>166</v>
       </c>
       <c r="B164" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C164">
-        <v>9858.7475739898</v>
+        <v>7118.299388486004</v>
       </c>
       <c r="D164">
-        <v>4988.549100871839</v>
+        <v>4387.796042371227</v>
       </c>
       <c r="E164">
-        <v>9051.622561655677</v>
+        <v>6214.950571608244</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3851,16 +3866,16 @@
         <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C165">
-        <v>3049.962402814945</v>
+        <v>1256.930682890124</v>
       </c>
       <c r="D165">
-        <v>7885.799173422068</v>
+        <v>634.2799162905493</v>
       </c>
       <c r="E165">
-        <v>14476.78741030169</v>
+        <v>1060.520130278657</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3868,16 +3883,16 @@
         <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C166">
-        <v>1932.537890358078</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D166">
-        <v>1092.439628676345</v>
+        <v>2953.473502833881</v>
       </c>
       <c r="E166">
-        <v>1729.767824059069</v>
+        <v>3032.074436227733</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3885,16 +3900,16 @@
         <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C167">
-        <v>927.0527858536279</v>
+        <v>0</v>
       </c>
       <c r="D167">
-        <v>885.4644642160963</v>
+        <v>0</v>
       </c>
       <c r="E167">
-        <v>854.6967352460968</v>
+        <v>1927.316250691574</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3902,16 +3917,16 @@
         <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C168">
-        <v>425667.2304377211</v>
+        <v>4982.658106436934</v>
       </c>
       <c r="D168">
-        <v>379452.4458343688</v>
+        <v>3682.745087885083</v>
       </c>
       <c r="E168">
-        <v>422462.404769241</v>
+        <v>4606.149113368056</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3919,16 +3934,16 @@
         <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C169">
-        <v>74824.1776942108</v>
+        <v>9858.7475739898</v>
       </c>
       <c r="D169">
-        <v>75532.04105321791</v>
+        <v>4988.549100871839</v>
       </c>
       <c r="E169">
-        <v>86492.52473873404</v>
+        <v>9051.622561655677</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3936,16 +3951,16 @@
         <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C170">
-        <v>128549.8642605276</v>
+        <v>3049.962402814945</v>
       </c>
       <c r="D170">
-        <v>114702.4949950556</v>
+        <v>7885.799173422068</v>
       </c>
       <c r="E170">
-        <v>134200.4554046213</v>
+        <v>14476.78741030169</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3953,16 +3968,16 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C171">
-        <v>55242.88725228325</v>
+        <v>1932.537890358078</v>
       </c>
       <c r="D171">
-        <v>54348.67956945477</v>
+        <v>1092.439628676345</v>
       </c>
       <c r="E171">
-        <v>54823.8158790419</v>
+        <v>1729.767824059069</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3970,16 +3985,16 @@
         <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C172">
-        <v>21186.42152206995</v>
+        <v>927.0527858536279</v>
       </c>
       <c r="D172">
-        <v>32192.86399794241</v>
+        <v>885.4644642160963</v>
       </c>
       <c r="E172">
-        <v>40091.29523030741</v>
+        <v>854.6967352460968</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -3987,16 +4002,16 @@
         <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C173">
-        <v>12108.98627481771</v>
+        <v>425667.2304377211</v>
       </c>
       <c r="D173">
-        <v>9710.044517252907</v>
+        <v>379452.4458343688</v>
       </c>
       <c r="E173">
-        <v>9820.712234959921</v>
+        <v>422462.404769241</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4004,16 +4019,16 @@
         <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C174">
-        <v>44818.4592191087</v>
+        <v>74824.1776942108</v>
       </c>
       <c r="D174">
-        <v>43318.43942297382</v>
+        <v>75532.04105321791</v>
       </c>
       <c r="E174">
-        <v>50430.2444258372</v>
+        <v>86492.52473873404</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -4021,16 +4036,16 @@
         <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C175">
-        <v>45410.20682375576</v>
+        <v>128549.8642605276</v>
       </c>
       <c r="D175">
-        <v>44140.29328236685</v>
+        <v>114702.4949950556</v>
       </c>
       <c r="E175">
-        <v>50777.920807722</v>
+        <v>134200.4554046213</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4038,16 +4053,16 @@
         <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C176">
-        <v>7877.356799130208</v>
+        <v>55242.88725228325</v>
       </c>
       <c r="D176">
-        <v>5653.095564499369</v>
+        <v>54348.67956945477</v>
       </c>
       <c r="E176">
-        <v>6662.276843942194</v>
+        <v>54823.8158790419</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4055,16 +4070,16 @@
         <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C177">
-        <v>7081.366168574467</v>
+        <v>21186.42152206995</v>
       </c>
       <c r="D177">
-        <v>7237.854347805022</v>
+        <v>32192.86399794241</v>
       </c>
       <c r="E177">
-        <v>8761.01660377788</v>
+        <v>40091.29523030741</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -4072,16 +4087,16 @@
         <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C178">
-        <v>17240.04215367412</v>
+        <v>12108.98627481771</v>
       </c>
       <c r="D178">
-        <v>13942.82778271549</v>
+        <v>9710.044517252907</v>
       </c>
       <c r="E178">
-        <v>14713.17492592106</v>
+        <v>9820.712234959921</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -4089,16 +4104,16 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C179">
-        <v>17324.03456184319</v>
+        <v>44818.4592191087</v>
       </c>
       <c r="D179">
-        <v>13476.54727078326</v>
+        <v>43318.43942297382</v>
       </c>
       <c r="E179">
-        <v>22628.13038686703</v>
+        <v>50430.2444258372</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -4106,16 +4121,16 @@
         <v>182</v>
       </c>
       <c r="B180" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C180">
-        <v>2689.033001442709</v>
+        <v>45410.20682375576</v>
       </c>
       <c r="D180">
-        <v>2118.88338047299</v>
+        <v>44140.29328236685</v>
       </c>
       <c r="E180">
-        <v>2326.478289412053</v>
+        <v>50777.920807722</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4123,16 +4138,16 @@
         <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C181">
-        <v>7330.001934671265</v>
+        <v>7877.356799130208</v>
       </c>
       <c r="D181">
-        <v>4696.892936408833</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E181">
-        <v>6336.909947377137</v>
+        <v>6662.276843942194</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -4140,16 +4155,16 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C182">
-        <v>3666.34991690552</v>
+        <v>7081.366168574467</v>
       </c>
       <c r="D182">
-        <v>2659.16265449915</v>
+        <v>7237.854347805022</v>
       </c>
       <c r="E182">
-        <v>3251.428044629679</v>
+        <v>8761.01660377788</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -4157,16 +4172,16 @@
         <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C183">
-        <v>3110.615608057638</v>
+        <v>17240.04215367412</v>
       </c>
       <c r="D183">
-        <v>2966.871688417814</v>
+        <v>13942.82778271549</v>
       </c>
       <c r="E183">
-        <v>3044.077493176301</v>
+        <v>14713.17492592106</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4174,16 +4189,16 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C184">
-        <v>4955.203939982344</v>
+        <v>17324.03456184319</v>
       </c>
       <c r="D184">
-        <v>4437.491921939725</v>
+        <v>13476.54727078326</v>
       </c>
       <c r="E184">
-        <v>4802.656681354792</v>
+        <v>22628.13038686703</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -4191,16 +4206,16 @@
         <v>187</v>
       </c>
       <c r="B185" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C185">
-        <v>5584.532853170555</v>
+        <v>2689.033001442709</v>
       </c>
       <c r="D185">
-        <v>3696.358431113311</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E185">
-        <v>5041.150517084573</v>
+        <v>2326.478289412053</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -4208,16 +4223,16 @@
         <v>188</v>
       </c>
       <c r="B186" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C186">
-        <v>12228.85287007065</v>
+        <v>7330.001934671265</v>
       </c>
       <c r="D186">
-        <v>5315.793599021267</v>
+        <v>4696.892936408833</v>
       </c>
       <c r="E186">
-        <v>10793.64798057903</v>
+        <v>6336.909947377137</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -4225,16 +4240,16 @@
         <v>189</v>
       </c>
       <c r="B187" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C187">
-        <v>3909.407627315059</v>
+        <v>3666.34991690552</v>
       </c>
       <c r="D187">
-        <v>12148.67547071851</v>
+        <v>2659.16265449915</v>
       </c>
       <c r="E187">
-        <v>24644.07599310096</v>
+        <v>3251.428044629679</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -4242,16 +4257,16 @@
         <v>190</v>
       </c>
       <c r="B188" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C188">
-        <v>2078.961774546943</v>
+        <v>3110.615608057638</v>
       </c>
       <c r="D188">
-        <v>1179.897477494976</v>
+        <v>2966.871688417814</v>
       </c>
       <c r="E188">
-        <v>1832.168256550158</v>
+        <v>3044.077493176301</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -4259,16 +4274,16 @@
         <v>191</v>
       </c>
       <c r="B189" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C189">
-        <v>932.8686753508275</v>
+        <v>4955.203939982344</v>
       </c>
       <c r="D189">
-        <v>920.6062716110156</v>
+        <v>4437.491921939725</v>
       </c>
       <c r="E189">
-        <v>0</v>
+        <v>4802.656681354792</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -4276,16 +4291,16 @@
         <v>192</v>
       </c>
       <c r="B190" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C190">
-        <v>195705.6</v>
+        <v>5584.532853170555</v>
       </c>
       <c r="D190">
-        <v>184867.2</v>
+        <v>3696.358431113311</v>
       </c>
       <c r="E190">
-        <v>187784</v>
+        <v>5041.150517084573</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4293,16 +4308,16 @@
         <v>193</v>
       </c>
       <c r="B191" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C191">
-        <v>223624</v>
+        <v>12228.85287007065</v>
       </c>
       <c r="D191">
-        <v>205627.2</v>
+        <v>5315.793599021267</v>
       </c>
       <c r="E191">
-        <v>214700.8</v>
+        <v>10793.64798057903</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4310,16 +4325,16 @@
         <v>194</v>
       </c>
       <c r="B192" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C192">
-        <v>253637.6</v>
+        <v>3909.407627315059</v>
       </c>
       <c r="D192">
-        <v>224994.4</v>
+        <v>12148.67547071851</v>
       </c>
       <c r="E192">
-        <v>242126.4</v>
+        <v>24644.07599310096</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4327,16 +4342,16 @@
         <v>195</v>
       </c>
       <c r="B193" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C193">
-        <v>284854.4</v>
+        <v>2078.961774546943</v>
       </c>
       <c r="D193">
-        <v>242956.8</v>
+        <v>1179.897477494976</v>
       </c>
       <c r="E193">
-        <v>270748</v>
+        <v>1832.168256550158</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4344,16 +4359,16 @@
         <v>196</v>
       </c>
       <c r="B194" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C194">
-        <v>275764.8</v>
+        <v>932.8686753508275</v>
       </c>
       <c r="D194">
-        <v>258018.4</v>
+        <v>920.6062716110156</v>
       </c>
       <c r="E194">
-        <v>296766.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -4361,16 +4376,16 @@
         <v>197</v>
       </c>
       <c r="B195" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C195">
-        <v>285775.2</v>
+        <v>195705.6</v>
       </c>
       <c r="D195">
-        <v>276530.4</v>
+        <v>184867.2</v>
       </c>
       <c r="E195">
-        <v>326134.4</v>
+        <v>187784</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -4378,16 +4393,16 @@
         <v>198</v>
       </c>
       <c r="B196" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C196">
-        <v>181481.6</v>
+        <v>223624</v>
       </c>
       <c r="D196">
-        <v>171418.4</v>
+        <v>205627.2</v>
       </c>
       <c r="E196">
-        <v>173696</v>
+        <v>214700.8</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4395,16 +4410,16 @@
         <v>199</v>
       </c>
       <c r="B197" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C197">
-        <v>206952</v>
+        <v>253637.6</v>
       </c>
       <c r="D197">
-        <v>183019.2</v>
+        <v>224994.4</v>
       </c>
       <c r="E197">
-        <v>189584.8</v>
+        <v>242126.4</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4412,16 +4427,16 @@
         <v>200</v>
       </c>
       <c r="B198" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C198">
-        <v>236529.6</v>
+        <v>284854.4</v>
       </c>
       <c r="D198">
-        <v>204145.6</v>
+        <v>242956.8</v>
       </c>
       <c r="E198">
-        <v>217076.8</v>
+        <v>270748</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4429,16 +4444,16 @@
         <v>201</v>
       </c>
       <c r="B199" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C199">
-        <v>266166.4</v>
+        <v>275764.8</v>
       </c>
       <c r="D199">
-        <v>221178.4</v>
+        <v>258018.4</v>
       </c>
       <c r="E199">
-        <v>243465.6</v>
+        <v>296766.4</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4446,16 +4461,16 @@
         <v>202</v>
       </c>
       <c r="B200" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C200">
-        <v>266616</v>
+        <v>285775.2</v>
       </c>
       <c r="D200">
-        <v>234677.6</v>
+        <v>276530.4</v>
       </c>
       <c r="E200">
-        <v>267149.6</v>
+        <v>326134.4</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4463,16 +4478,16 @@
         <v>203</v>
       </c>
       <c r="B201" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C201">
-        <v>275787.2</v>
+        <v>181481.6</v>
       </c>
       <c r="D201">
-        <v>252004</v>
+        <v>171418.4</v>
       </c>
       <c r="E201">
-        <v>295416</v>
+        <v>173696</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4480,16 +4495,16 @@
         <v>204</v>
       </c>
       <c r="B202" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C202">
-        <v>166797.6</v>
+        <v>206952</v>
       </c>
       <c r="D202">
-        <v>173032.8</v>
+        <v>183019.2</v>
       </c>
       <c r="E202">
-        <v>175456.8</v>
+        <v>189584.8</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4497,16 +4512,16 @@
         <v>205</v>
       </c>
       <c r="B203" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C203">
-        <v>187860.8</v>
+        <v>236529.6</v>
       </c>
       <c r="D203">
-        <v>192721.6</v>
+        <v>204145.6</v>
       </c>
       <c r="E203">
-        <v>199666.4</v>
+        <v>217076.8</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4514,16 +4529,16 @@
         <v>206</v>
       </c>
       <c r="B204" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C204">
-        <v>214399.2</v>
+        <v>266166.4</v>
       </c>
       <c r="D204">
-        <v>208928.8</v>
+        <v>221178.4</v>
       </c>
       <c r="E204">
-        <v>221102.4</v>
+        <v>243465.6</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4531,16 +4546,16 @@
         <v>207</v>
       </c>
       <c r="B205" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C205">
-        <v>240393.6</v>
+        <v>266616</v>
       </c>
       <c r="D205">
-        <v>232657.6</v>
+        <v>234677.6</v>
       </c>
       <c r="E205">
-        <v>254091.2</v>
+        <v>267149.6</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4548,16 +4563,16 @@
         <v>208</v>
       </c>
       <c r="B206" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="C206">
-        <v>266132</v>
+        <v>275787.2</v>
       </c>
       <c r="D206">
-        <v>251892</v>
+        <v>252004</v>
       </c>
       <c r="E206">
-        <v>284350.4</v>
+        <v>295416</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -4565,15 +4580,100 @@
         <v>209</v>
       </c>
       <c r="B207" t="s">
+        <v>216</v>
+      </c>
+      <c r="C207">
+        <v>166797.6</v>
+      </c>
+      <c r="D207">
+        <v>173032.8</v>
+      </c>
+      <c r="E207">
+        <v>175456.8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B208" t="s">
+        <v>216</v>
+      </c>
+      <c r="C208">
+        <v>187860.8</v>
+      </c>
+      <c r="D208">
+        <v>192721.6</v>
+      </c>
+      <c r="E208">
+        <v>199666.4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C207">
+      <c r="B209" t="s">
+        <v>216</v>
+      </c>
+      <c r="C209">
+        <v>214399.2</v>
+      </c>
+      <c r="D209">
+        <v>208928.8</v>
+      </c>
+      <c r="E209">
+        <v>221102.4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B210" t="s">
+        <v>216</v>
+      </c>
+      <c r="C210">
+        <v>240393.6</v>
+      </c>
+      <c r="D210">
+        <v>232657.6</v>
+      </c>
+      <c r="E210">
+        <v>254091.2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B211" t="s">
+        <v>216</v>
+      </c>
+      <c r="C211">
+        <v>266132</v>
+      </c>
+      <c r="D211">
+        <v>251892</v>
+      </c>
+      <c r="E211">
+        <v>284350.4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B212" t="s">
+        <v>216</v>
+      </c>
+      <c r="C212">
         <v>277836.8</v>
       </c>
-      <c r="D207">
+      <c r="D212">
         <v>271554.4</v>
       </c>
-      <c r="E207">
+      <c r="E212">
         <v>316714.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - add_percentage_growth_by_sector_row
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df.xlsx
+++ b/create_forecast_basic/utils/monitoring_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="258">
   <si>
     <t>2020</t>
   </si>
@@ -128,6 +128,81 @@
   </si>
   <si>
     <t>percentage growth univ 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth Arab 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall 2020-2025</t>
+  </si>
+  <si>
+    <t>percentage growth Arab 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall 2025-2030</t>
+  </si>
+  <si>
+    <t>percentage growth Arab 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall 2030-2035</t>
+  </si>
+  <si>
+    <t>percentage growth Arab 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall 2035-2040</t>
+  </si>
+  <si>
+    <t>percentage growth Arab 2050-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish 2050-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian 2050-2045</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox 2050-2045</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall 2050-2045</t>
   </si>
   <si>
     <t>percentage growth BaseProjections age20_29 2025-2030</t>
@@ -1070,7 +1145,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1095,16 +1170,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="C2" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1112,16 +1187,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1129,16 +1204,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1146,16 +1221,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C5" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1248,16 +1323,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="C11" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="D11" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1265,16 +1340,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1282,16 +1357,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="E13" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1299,16 +1374,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>248</v>
       </c>
       <c r="D14" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1316,16 +1391,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="C15" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="E15" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1333,16 +1408,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="E16" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1503,7 +1578,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C26">
         <v>288</v>
@@ -1520,7 +1595,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C27">
         <v>110</v>
@@ -1537,7 +1612,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C28">
         <v>109</v>
@@ -1554,7 +1629,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C29">
         <v>109</v>
@@ -1571,7 +1646,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C30">
         <v>94</v>
@@ -1588,7 +1663,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -1605,7 +1680,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1622,7 +1697,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1639,7 +1714,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -1656,7 +1731,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1672,9 +1747,6 @@
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B36" t="s">
-        <v>216</v>
-      </c>
       <c r="C36">
         <v>112</v>
       </c>
@@ -1682,449 +1754,377 @@
         <v>111</v>
       </c>
       <c r="E36">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
-        <v>216</v>
-      </c>
       <c r="C37">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D37">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E37">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
-        <v>216</v>
-      </c>
       <c r="C38">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B39" t="s">
-        <v>216</v>
-      </c>
       <c r="C39">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D39">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="E39">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B40" t="s">
-        <v>216</v>
-      </c>
       <c r="C40">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D40">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E40">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B41">
-        <v>213239.3333333333</v>
-      </c>
       <c r="C41">
-        <v>213239.3333333333</v>
+        <v>111</v>
       </c>
       <c r="D41">
-        <v>213239.3333333333</v>
+        <v>108</v>
       </c>
       <c r="E41">
-        <v>213239.3333333333</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B42">
-        <v>28627.66666666667</v>
-      </c>
       <c r="C42">
-        <v>28627.66666666667</v>
+        <v>114</v>
       </c>
       <c r="D42">
-        <v>28627.66666666667</v>
+        <v>108</v>
       </c>
       <c r="E42">
-        <v>28627.66666666667</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B43">
-        <v>46063</v>
-      </c>
       <c r="C43">
-        <v>46063</v>
+        <v>108</v>
       </c>
       <c r="D43">
-        <v>46063</v>
+        <v>108</v>
       </c>
       <c r="E43">
-        <v>46063</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B44">
-        <v>23828</v>
-      </c>
       <c r="C44">
-        <v>23828</v>
+        <v>114</v>
       </c>
       <c r="D44">
-        <v>23828</v>
+        <v>116</v>
       </c>
       <c r="E44">
-        <v>23828</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B45">
-        <v>8538</v>
-      </c>
       <c r="C45">
-        <v>8538</v>
+        <v>113</v>
       </c>
       <c r="D45">
-        <v>8538</v>
+        <v>110</v>
       </c>
       <c r="E45">
-        <v>8538</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B46">
-        <v>5048</v>
-      </c>
       <c r="C46">
-        <v>5048</v>
+        <v>111</v>
       </c>
       <c r="D46">
-        <v>5048</v>
+        <v>108</v>
       </c>
       <c r="E46">
-        <v>5048</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B47">
-        <v>21988.00000000001</v>
-      </c>
       <c r="C47">
-        <v>21988</v>
+        <v>115</v>
       </c>
       <c r="D47">
-        <v>21988</v>
+        <v>108</v>
       </c>
       <c r="E47">
-        <v>21988</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B48">
-        <v>27262</v>
-      </c>
       <c r="C48">
-        <v>27262</v>
+        <v>107</v>
       </c>
       <c r="D48">
-        <v>27262</v>
+        <v>107</v>
       </c>
       <c r="E48">
-        <v>27262</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B49">
-        <v>2804</v>
-      </c>
       <c r="C49">
-        <v>2804</v>
+        <v>113</v>
       </c>
       <c r="D49">
-        <v>2804</v>
+        <v>115</v>
       </c>
       <c r="E49">
-        <v>2804</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B50">
-        <v>1331</v>
-      </c>
       <c r="C50">
-        <v>1331</v>
+        <v>109</v>
       </c>
       <c r="D50">
-        <v>1331</v>
+        <v>106</v>
       </c>
       <c r="E50">
-        <v>1331</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B51">
-        <v>7375</v>
-      </c>
       <c r="C51">
-        <v>7375</v>
+        <v>111</v>
       </c>
       <c r="D51">
-        <v>7375</v>
+        <v>108</v>
       </c>
       <c r="E51">
-        <v>7375</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B52">
-        <v>8805</v>
-      </c>
       <c r="C52">
-        <v>8805</v>
+        <v>115</v>
       </c>
       <c r="D52">
-        <v>8805</v>
+        <v>107</v>
       </c>
       <c r="E52">
-        <v>8805</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B53">
-        <v>1218</v>
-      </c>
       <c r="C53">
-        <v>1218</v>
+        <v>106</v>
       </c>
       <c r="D53">
-        <v>1218</v>
+        <v>106</v>
       </c>
       <c r="E53">
-        <v>1218</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B54">
-        <v>1673</v>
-      </c>
       <c r="C54">
-        <v>1673</v>
+        <v>109</v>
       </c>
       <c r="D54">
-        <v>1673</v>
+        <v>113</v>
       </c>
       <c r="E54">
-        <v>1673</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B55">
-        <v>2401</v>
-      </c>
       <c r="C55">
-        <v>2401</v>
+        <v>103</v>
       </c>
       <c r="D55">
-        <v>2401</v>
+        <v>100</v>
       </c>
       <c r="E55">
-        <v>2401</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B56">
-        <v>2488</v>
-      </c>
       <c r="C56">
-        <v>2488</v>
+        <v>99</v>
       </c>
       <c r="D56">
-        <v>2488</v>
+        <v>95</v>
       </c>
       <c r="E56">
-        <v>2488</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B57">
-        <v>2148</v>
-      </c>
       <c r="C57">
-        <v>2148</v>
+        <v>93</v>
       </c>
       <c r="D57">
-        <v>2148</v>
+        <v>96</v>
       </c>
       <c r="E57">
-        <v>2148</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B58">
-        <v>3242</v>
-      </c>
       <c r="C58">
-        <v>3242</v>
+        <v>94</v>
       </c>
       <c r="D58">
-        <v>3242</v>
+        <v>94</v>
       </c>
       <c r="E58">
-        <v>3242</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B59">
-        <v>3637</v>
-      </c>
       <c r="C59">
-        <v>3637</v>
+        <v>95</v>
       </c>
       <c r="D59">
-        <v>3637</v>
+        <v>87</v>
       </c>
       <c r="E59">
-        <v>3637</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B60">
-        <v>301</v>
-      </c>
       <c r="C60">
-        <v>301</v>
+        <v>100</v>
       </c>
       <c r="D60">
-        <v>301</v>
+        <v>95</v>
       </c>
       <c r="E60">
-        <v>301</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B61">
-        <v>537</v>
+      <c r="B61" t="s">
+        <v>241</v>
       </c>
       <c r="C61">
-        <v>537</v>
+        <v>112</v>
       </c>
       <c r="D61">
-        <v>537</v>
+        <v>111</v>
       </c>
       <c r="E61">
-        <v>537</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B62">
-        <v>300</v>
+      <c r="B62" t="s">
+        <v>241</v>
       </c>
       <c r="C62">
-        <v>300</v>
+        <v>111</v>
       </c>
       <c r="D62">
-        <v>300</v>
+        <v>111</v>
       </c>
       <c r="E62">
-        <v>300</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2132,16 +2132,16 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C63">
-        <v>285733.3218235314</v>
+        <v>111</v>
       </c>
       <c r="D63">
-        <v>274161.0000038777</v>
+        <v>108</v>
       </c>
       <c r="E63">
-        <v>275663.3373324008</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2149,16 +2149,16 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C64">
-        <v>36057.66373063793</v>
+        <v>116</v>
       </c>
       <c r="D64">
-        <v>33344.22909790605</v>
+        <v>108</v>
       </c>
       <c r="E64">
-        <v>34286.84568702983</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2166,390 +2166,390 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C65">
-        <v>66822.51137331135</v>
+        <v>106</v>
       </c>
       <c r="D65">
-        <v>61855.23107261454</v>
+        <v>108</v>
       </c>
       <c r="E65">
-        <v>63948.66570649843</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B66" t="s">
-        <v>216</v>
+      <c r="B66">
+        <v>213239.3333333333</v>
       </c>
       <c r="C66">
-        <v>33156.30459804353</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="D66">
-        <v>33335.50923218194</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="E66">
-        <v>33397.07322472375</v>
+        <v>213239.3333333333</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B67" t="s">
-        <v>216</v>
+      <c r="B67">
+        <v>28627.66666666667</v>
       </c>
       <c r="C67">
-        <v>9986.417617537509</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="D67">
-        <v>10194.62059102478</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="E67">
-        <v>10338.40358091756</v>
+        <v>28627.66666666667</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B68" t="s">
-        <v>216</v>
+      <c r="B68">
+        <v>46063</v>
       </c>
       <c r="C68">
-        <v>8306.813376518987</v>
+        <v>46063</v>
       </c>
       <c r="D68">
-        <v>6946.591660718233</v>
+        <v>46063</v>
       </c>
       <c r="E68">
-        <v>8135.667377017133</v>
+        <v>46063</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B69" t="s">
-        <v>216</v>
+      <c r="B69">
+        <v>23828</v>
       </c>
       <c r="C69">
-        <v>29427.44116169451</v>
+        <v>23828</v>
       </c>
       <c r="D69">
-        <v>30953.22576377643</v>
+        <v>23828</v>
       </c>
       <c r="E69">
-        <v>31386.31536916655</v>
+        <v>23828</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B70" t="s">
-        <v>216</v>
+      <c r="B70">
+        <v>8538</v>
       </c>
       <c r="C70">
-        <v>37145.33462606892</v>
+        <v>8538</v>
       </c>
       <c r="D70">
-        <v>39041.11738664036</v>
+        <v>8538</v>
       </c>
       <c r="E70">
-        <v>40239.51136715176</v>
+        <v>8538</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B71" t="s">
-        <v>216</v>
+      <c r="B71">
+        <v>5048</v>
       </c>
       <c r="C71">
-        <v>5309.478782988256</v>
+        <v>5048</v>
       </c>
       <c r="D71">
-        <v>5060.408660766857</v>
+        <v>5048</v>
       </c>
       <c r="E71">
-        <v>5201.12526897965</v>
+        <v>5048</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B72" t="s">
-        <v>216</v>
+      <c r="B72">
+        <v>21988.00000000001</v>
       </c>
       <c r="C72">
-        <v>5521.895631861405</v>
+        <v>21988</v>
       </c>
       <c r="D72">
-        <v>6073.616715538182</v>
+        <v>21988</v>
       </c>
       <c r="E72">
-        <v>6265.692004112236</v>
+        <v>21988</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B73" t="s">
-        <v>216</v>
+      <c r="B73">
+        <v>27262</v>
       </c>
       <c r="C73">
-        <v>7012.74256878429</v>
+        <v>27262</v>
       </c>
       <c r="D73">
-        <v>6467.15326810131</v>
+        <v>27262</v>
       </c>
       <c r="E73">
-        <v>6547.602648720247</v>
+        <v>27262</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B74" t="s">
-        <v>216</v>
+      <c r="B74">
+        <v>2804</v>
       </c>
       <c r="C74">
-        <v>7317.313641591267</v>
+        <v>2804</v>
       </c>
       <c r="D74">
-        <v>7240.499364931959</v>
+        <v>2804</v>
       </c>
       <c r="E74">
-        <v>7309.076098225414</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B75" t="s">
-        <v>216</v>
+      <c r="B75">
+        <v>1331</v>
       </c>
       <c r="C75">
-        <v>2166.404734331622</v>
+        <v>1331</v>
       </c>
       <c r="D75">
-        <v>2013.947393383935</v>
+        <v>1331</v>
       </c>
       <c r="E75">
-        <v>2067.009181064854</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B76" t="s">
-        <v>216</v>
+      <c r="B76">
+        <v>7375</v>
       </c>
       <c r="C76">
-        <v>3081.965248662672</v>
+        <v>7375</v>
       </c>
       <c r="D76">
-        <v>3137.447595991872</v>
+        <v>7375</v>
       </c>
       <c r="E76">
-        <v>3186.615419267629</v>
+        <v>7375</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B77" t="s">
-        <v>216</v>
+      <c r="B77">
+        <v>8805</v>
       </c>
       <c r="C77">
-        <v>443.1341918519325</v>
+        <v>8805</v>
       </c>
       <c r="D77">
-        <v>421.887538681912</v>
+        <v>8805</v>
       </c>
       <c r="E77">
-        <v>433.4544189987498</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B78" t="s">
-        <v>216</v>
+      <c r="B78">
+        <v>1218</v>
       </c>
       <c r="C78">
-        <v>2895.085614458657</v>
+        <v>1218</v>
       </c>
       <c r="D78">
-        <v>2909.362870154178</v>
+        <v>1218</v>
       </c>
       <c r="E78">
-        <v>2924.168116891962</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B79" t="s">
-        <v>216</v>
+      <c r="B79">
+        <v>1673</v>
       </c>
       <c r="C79">
-        <v>3653.831655445544</v>
+        <v>1673</v>
       </c>
       <c r="D79">
-        <v>3598.638480494133</v>
+        <v>1673</v>
       </c>
       <c r="E79">
-        <v>3616.404971165329</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B80" t="s">
-        <v>216</v>
+      <c r="B80">
+        <v>2401</v>
       </c>
       <c r="C80">
-        <v>3542.454003930634</v>
+        <v>2401</v>
       </c>
       <c r="D80">
-        <v>3648.230892236539</v>
+        <v>2401</v>
       </c>
       <c r="E80">
-        <v>3678.324608989895</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B81" t="s">
-        <v>216</v>
+      <c r="B81">
+        <v>2488</v>
       </c>
       <c r="C81">
-        <v>4257.401768859199</v>
+        <v>2488</v>
       </c>
       <c r="D81">
-        <v>4324.862744573556</v>
+        <v>2488</v>
       </c>
       <c r="E81">
-        <v>4363.718311116243</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B82" t="s">
-        <v>216</v>
+      <c r="B82">
+        <v>2148</v>
       </c>
       <c r="C82">
-        <v>881.1481005457115</v>
+        <v>2148</v>
       </c>
       <c r="D82">
-        <v>922.4946308419028</v>
+        <v>2148</v>
       </c>
       <c r="E82">
-        <v>951.6553445648265</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B83" t="s">
-        <v>216</v>
+      <c r="B83">
+        <v>3242</v>
       </c>
       <c r="C83">
-        <v>911.7413777070067</v>
+        <v>3242</v>
       </c>
       <c r="D83">
-        <v>868.7478168054034</v>
+        <v>3242</v>
       </c>
       <c r="E83">
-        <v>883.9572064300576</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B84" t="s">
-        <v>216</v>
+      <c r="B84">
+        <v>3637</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>3637</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>3637</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B85" t="s">
-        <v>216</v>
+      <c r="B85">
+        <v>301</v>
       </c>
       <c r="C85">
-        <v>310887.0551086462</v>
+        <v>301</v>
       </c>
       <c r="D85">
-        <v>290797.302000507</v>
+        <v>301</v>
       </c>
       <c r="E85">
-        <v>292306.0034436272</v>
+        <v>301</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B86" t="s">
-        <v>216</v>
+      <c r="B86">
+        <v>537</v>
       </c>
       <c r="C86">
-        <v>51074.32436027069</v>
+        <v>537</v>
       </c>
       <c r="D86">
-        <v>26072.86402002085</v>
+        <v>537</v>
       </c>
       <c r="E86">
-        <v>44744.53526801307</v>
+        <v>537</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B87" t="s">
-        <v>216</v>
+      <c r="B87">
+        <v>300</v>
       </c>
       <c r="C87">
-        <v>84109.82719823082</v>
+        <v>300</v>
       </c>
       <c r="D87">
-        <v>77937.73156609248</v>
+        <v>300</v>
       </c>
       <c r="E87">
-        <v>84581.97612214876</v>
+        <v>300</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2557,16 +2557,16 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C88">
-        <v>39310.49274971832</v>
+        <v>285733.3218235314</v>
       </c>
       <c r="D88">
-        <v>38683.92515358835</v>
+        <v>274161.0000038777</v>
       </c>
       <c r="E88">
-        <v>38875.73769831542</v>
+        <v>275663.3373324008</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2574,16 +2574,16 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C89">
-        <v>11932.38400809033</v>
+        <v>36057.66373063793</v>
       </c>
       <c r="D89">
-        <v>10681.35241281803</v>
+        <v>33344.22909790605</v>
       </c>
       <c r="E89">
-        <v>11035.70441498311</v>
+        <v>34286.84568702983</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2591,16 +2591,16 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C90">
-        <v>9548.28031721313</v>
+        <v>66822.51137331135</v>
       </c>
       <c r="D90">
-        <v>7703.305735153427</v>
+        <v>61855.23107261454</v>
       </c>
       <c r="E90">
-        <v>8161.797271070729</v>
+        <v>63948.66570649843</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2608,16 +2608,16 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C91">
-        <v>35810.66989709945</v>
+        <v>33156.30459804353</v>
       </c>
       <c r="D91">
-        <v>36601.69575249061</v>
+        <v>33335.50923218194</v>
       </c>
       <c r="E91">
-        <v>39241.8615517352</v>
+        <v>33397.07322472375</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2625,16 +2625,16 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C92">
-        <v>40274.91199119319</v>
+        <v>9986.417617537509</v>
       </c>
       <c r="D92">
-        <v>41351.35312049399</v>
+        <v>10194.62059102478</v>
       </c>
       <c r="E92">
-        <v>44632.82113421193</v>
+        <v>10338.40358091756</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2642,16 +2642,16 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C93">
-        <v>5702.582508173264</v>
+        <v>8306.813376518987</v>
       </c>
       <c r="D93">
-        <v>5197.04316560074</v>
+        <v>6946.591660718233</v>
       </c>
       <c r="E93">
-        <v>5490.350510109492</v>
+        <v>8135.667377017133</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2659,16 +2659,16 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C94">
-        <v>6531.454941380145</v>
+        <v>29427.44116169451</v>
       </c>
       <c r="D94">
-        <v>6914.424310549415</v>
+        <v>30953.22576377643</v>
       </c>
       <c r="E94">
-        <v>7565.494786531661</v>
+        <v>31386.31536916655</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2676,16 +2676,16 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C95">
-        <v>11086.07248419944</v>
+        <v>37145.33462606892</v>
       </c>
       <c r="D95">
-        <v>9081.046501582416</v>
+        <v>39041.11738664036</v>
       </c>
       <c r="E95">
-        <v>9712.39919620127</v>
+        <v>40239.51136715176</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2693,16 +2693,16 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C96">
-        <v>11235.01770760014</v>
+        <v>5309.478782988256</v>
       </c>
       <c r="D96">
-        <v>7294.264487669744</v>
+        <v>5060.408660766857</v>
       </c>
       <c r="E96">
-        <v>7393.954728795917</v>
+        <v>5201.12526897965</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2710,16 +2710,16 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C97">
-        <v>2313.18743770475</v>
+        <v>5521.895631861405</v>
       </c>
       <c r="D97">
-        <v>2050.379609518187</v>
+        <v>6073.616715538182</v>
       </c>
       <c r="E97">
-        <v>2158.015018647229</v>
+        <v>6265.692004112236</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2727,16 +2727,16 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C98">
-        <v>4487.422497745161</v>
+        <v>7012.74256878429</v>
       </c>
       <c r="D98">
-        <v>3251.340662315742</v>
+        <v>6467.15326810131</v>
       </c>
       <c r="E98">
-        <v>3680.595601936531</v>
+        <v>6547.602648720247</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2744,16 +2744,16 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C99">
-        <v>3291.571394333075</v>
+        <v>7317.313641591267</v>
       </c>
       <c r="D99">
-        <v>453.0691373312048</v>
+        <v>7240.499364931959</v>
       </c>
       <c r="E99">
-        <v>505.4945456516502</v>
+        <v>7309.076098225414</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2761,16 +2761,16 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C100">
-        <v>2962.271032197586</v>
+        <v>2166.404734331622</v>
       </c>
       <c r="D100">
-        <v>2922.939603860779</v>
+        <v>2013.947393383935</v>
       </c>
       <c r="E100">
-        <v>2944.717615440521</v>
+        <v>2067.009181064854</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2778,16 +2778,16 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C101">
-        <v>3978.851277647058</v>
+        <v>3081.965248662672</v>
       </c>
       <c r="D101">
-        <v>1566.476580450332</v>
+        <v>3137.447595991872</v>
       </c>
       <c r="E101">
-        <v>1592.42779801514</v>
+        <v>3186.615419267629</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2795,16 +2795,16 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C102">
-        <v>3624.875154413226</v>
+        <v>443.1341918519325</v>
       </c>
       <c r="D102">
-        <v>3677.660725632635</v>
+        <v>421.887538681912</v>
       </c>
       <c r="E102">
-        <v>3727.402937205914</v>
+        <v>433.4544189987498</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2812,16 +2812,16 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C103">
-        <v>4499.453713305816</v>
+        <v>2895.085614458657</v>
       </c>
       <c r="D103">
-        <v>4389.339541465134</v>
+        <v>2909.362870154178</v>
       </c>
       <c r="E103">
-        <v>4489.156966460471</v>
+        <v>2924.168116891962</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2829,16 +2829,16 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C104">
-        <v>1176.375213333053</v>
+        <v>3653.831655445544</v>
       </c>
       <c r="D104">
-        <v>1229.853805184373</v>
+        <v>3598.638480494133</v>
       </c>
       <c r="E104">
-        <v>1330.656790249233</v>
+        <v>3616.404971165329</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2846,16 +2846,16 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C105">
-        <v>1013.219479989464</v>
+        <v>3542.454003930634</v>
       </c>
       <c r="D105">
-        <v>873.6169022987777</v>
+        <v>3648.230892236539</v>
       </c>
       <c r="E105">
-        <v>911.1327501980686</v>
+        <v>3678.324608989895</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2863,16 +2863,16 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C106">
-        <v>857.2621118872319</v>
+        <v>4257.401768859199</v>
       </c>
       <c r="D106">
-        <v>772.2734198315197</v>
+        <v>4324.862744573556</v>
       </c>
       <c r="E106">
-        <v>801.0018403865388</v>
+        <v>4363.718311116243</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2880,16 +2880,16 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C107">
-        <v>345179.8540918057</v>
+        <v>881.1481005457115</v>
       </c>
       <c r="D107">
-        <v>306070.7824845224</v>
+        <v>922.4946308419028</v>
       </c>
       <c r="E107">
-        <v>311915.8222954976</v>
+        <v>951.6553445648265</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2897,16 +2897,16 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C108">
-        <v>57843.05696310467</v>
+        <v>911.7413777070067</v>
       </c>
       <c r="D108">
-        <v>41761.14805054816</v>
+        <v>868.7478168054034</v>
       </c>
       <c r="E108">
-        <v>48660.60638720006</v>
+        <v>883.9572064300576</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2914,16 +2914,16 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C109">
-        <v>106400.8113634808</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>97376.26626200562</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>107457.7153467231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2931,16 +2931,16 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C110">
-        <v>47754.67592555143</v>
+        <v>310887.0551086462</v>
       </c>
       <c r="D110">
-        <v>46917.82385382168</v>
+        <v>290797.302000507</v>
       </c>
       <c r="E110">
-        <v>47285.0706371487</v>
+        <v>292306.0034436272</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2948,16 +2948,16 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C111">
-        <v>13642.04328300475</v>
+        <v>51074.32436027069</v>
       </c>
       <c r="D111">
-        <v>12594.12090677959</v>
+        <v>26072.86402002085</v>
       </c>
       <c r="E111">
-        <v>14151.68818183644</v>
+        <v>44744.53526801307</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2965,16 +2965,16 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C112">
-        <v>10166.68671320246</v>
+        <v>84109.82719823082</v>
       </c>
       <c r="D112">
-        <v>7870.660600118454</v>
+        <v>77937.73156609248</v>
       </c>
       <c r="E112">
-        <v>8448.569974010888</v>
+        <v>84581.97612214876</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2982,16 +2982,16 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C113">
-        <v>40056.29615048355</v>
+        <v>39310.49274971832</v>
       </c>
       <c r="D113">
-        <v>39938.78970433185</v>
+        <v>38683.92515358835</v>
       </c>
       <c r="E113">
-        <v>44520.15917103966</v>
+        <v>38875.73769831542</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2999,16 +2999,16 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C114">
-        <v>42099.78280750295</v>
+        <v>11932.38400809033</v>
       </c>
       <c r="D114">
-        <v>42299.87775020443</v>
+        <v>10681.35241281803</v>
       </c>
       <c r="E114">
-        <v>47328.28098195308</v>
+        <v>11035.70441498311</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3016,16 +3016,16 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C115">
-        <v>6780.581746217548</v>
+        <v>9548.28031721313</v>
       </c>
       <c r="D115">
-        <v>5344.462556042371</v>
+        <v>7703.305735153427</v>
       </c>
       <c r="E115">
-        <v>5852.587839854697</v>
+        <v>8161.797271070729</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3033,16 +3033,16 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C116">
-        <v>7052.041776574091</v>
+        <v>35810.66989709945</v>
       </c>
       <c r="D116">
-        <v>2387.833946905571</v>
+        <v>36601.69575249061</v>
       </c>
       <c r="E116">
-        <v>2653.360912751024</v>
+        <v>39241.8615517352</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3050,16 +3050,16 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C117">
-        <v>12491.64080553533</v>
+        <v>40274.91199119319</v>
       </c>
       <c r="D117">
-        <v>7553.961214696117</v>
+        <v>41351.35312049399</v>
       </c>
       <c r="E117">
-        <v>8823.015551678049</v>
+        <v>44632.82113421193</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3067,16 +3067,16 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C118">
-        <v>11918.07029478611</v>
+        <v>5702.582508173264</v>
       </c>
       <c r="D118">
-        <v>10755.76769609013</v>
+        <v>5197.04316560074</v>
       </c>
       <c r="E118">
-        <v>11073.8263395291</v>
+        <v>5490.350510109492</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3084,16 +3084,16 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C119">
-        <v>2510.791313969085</v>
+        <v>6531.454941380145</v>
       </c>
       <c r="D119">
-        <v>2080.311820058766</v>
+        <v>6914.424310549415</v>
       </c>
       <c r="E119">
-        <v>2225.787307207039</v>
+        <v>7565.494786531661</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3101,16 +3101,16 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C120">
-        <v>5559.189168957029</v>
+        <v>11086.07248419944</v>
       </c>
       <c r="D120">
-        <v>3507.429258284409</v>
+        <v>9081.046501582416</v>
       </c>
       <c r="E120">
-        <v>4514.632917614302</v>
+        <v>9712.39919620127</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3118,16 +3118,16 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C121">
-        <v>3740.698985412615</v>
+        <v>11235.01770760014</v>
       </c>
       <c r="D121">
-        <v>456.0519360615073</v>
+        <v>7294.264487669744</v>
       </c>
       <c r="E121">
-        <v>595.516072795263</v>
+        <v>7393.954728795917</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3135,16 +3135,16 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C122">
-        <v>3025.982972811596</v>
+        <v>2313.18743770475</v>
       </c>
       <c r="D122">
-        <v>2930.200017528361</v>
+        <v>2050.379609518187</v>
       </c>
       <c r="E122">
-        <v>2972.156458241908</v>
+        <v>2158.015018647229</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3152,16 +3152,16 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C123">
-        <v>4384.134004159239</v>
+        <v>4487.422497745161</v>
       </c>
       <c r="D123">
-        <v>3877.68979844253</v>
+        <v>3251.340662315742</v>
       </c>
       <c r="E123">
-        <v>3984.413723700878</v>
+        <v>3680.595601936531</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3169,16 +3169,16 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C124">
-        <v>3818.113674370041</v>
+        <v>3291.571394333075</v>
       </c>
       <c r="D124">
-        <v>3677.660725632635</v>
+        <v>453.0691373312048</v>
       </c>
       <c r="E124">
-        <v>3773.270697207371</v>
+        <v>505.4945456516502</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3186,16 +3186,16 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C125">
-        <v>5697.549039481555</v>
+        <v>2962.271032197586</v>
       </c>
       <c r="D125">
-        <v>4449.270708440607</v>
+        <v>2922.939603860779</v>
       </c>
       <c r="E125">
-        <v>4794.85366801385</v>
+        <v>2944.717615440521</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3203,16 +3203,16 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C126">
-        <v>1675.03137312741</v>
+        <v>3978.851277647058</v>
       </c>
       <c r="D126">
-        <v>1815.4386330182</v>
+        <v>1566.476580450332</v>
       </c>
       <c r="E126">
-        <v>2049.263941768266</v>
+        <v>1592.42779801514</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3220,16 +3220,16 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C127">
-        <v>1388.615296125427</v>
+        <v>3624.875154413226</v>
       </c>
       <c r="D127">
-        <v>898.8243487684732</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E127">
-        <v>1101.853615098803</v>
+        <v>3727.402937205914</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3237,16 +3237,16 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C128">
-        <v>915.4210068592286</v>
+        <v>4499.453713305816</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>4389.339541465134</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>4489.156966460471</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3254,16 +3254,16 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C129">
-        <v>379833.2126030341</v>
+        <v>1176.375213333053</v>
       </c>
       <c r="D129">
-        <v>323789.1870151541</v>
+        <v>1229.853805184373</v>
       </c>
       <c r="E129">
-        <v>342305.1273678984</v>
+        <v>1330.656790249233</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3271,16 +3271,16 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C130">
-        <v>66636.46327624648</v>
+        <v>1013.219479989464</v>
       </c>
       <c r="D130">
-        <v>57885.11081377808</v>
+        <v>873.6169022987777</v>
       </c>
       <c r="E130">
-        <v>65450.5214985832</v>
+        <v>911.1327501980686</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3288,16 +3288,16 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C131">
-        <v>122447.4212601383</v>
+        <v>857.2621118872319</v>
       </c>
       <c r="D131">
-        <v>106273.0478090824</v>
+        <v>772.2734198315197</v>
       </c>
       <c r="E131">
-        <v>119530.3850553175</v>
+        <v>801.0018403865388</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3305,16 +3305,16 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C132">
-        <v>55098.14072490651</v>
+        <v>345179.8540918057</v>
       </c>
       <c r="D132">
-        <v>53997.08352943832</v>
+        <v>306070.7824845224</v>
       </c>
       <c r="E132">
-        <v>54429.29718809373</v>
+        <v>311915.8222954976</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3322,16 +3322,16 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C133">
-        <v>17436.20392355449</v>
+        <v>57843.05696310467</v>
       </c>
       <c r="D133">
-        <v>19678.07818882393</v>
+        <v>41761.14805054816</v>
       </c>
       <c r="E133">
-        <v>23411.63616688988</v>
+        <v>48660.60638720006</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3339,16 +3339,16 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C134">
-        <v>11477.1443269179</v>
+        <v>106400.8113634808</v>
       </c>
       <c r="D134">
-        <v>7941.17271971979</v>
+        <v>97376.26626200562</v>
       </c>
       <c r="E134">
-        <v>8685.454438123739</v>
+        <v>107457.7153467231</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3356,16 +3356,16 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C135">
-        <v>44788.85407568982</v>
+        <v>47754.67592555143</v>
       </c>
       <c r="D135">
-        <v>42290.86139964137</v>
+        <v>46917.82385382168</v>
       </c>
       <c r="E135">
-        <v>48116.24030242601</v>
+        <v>47285.0706371487</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3373,16 +3373,16 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C136">
-        <v>43854.83257609577</v>
+        <v>13642.04328300475</v>
       </c>
       <c r="D136">
-        <v>42446.11108034404</v>
+        <v>12594.12090677959</v>
       </c>
       <c r="E136">
-        <v>48048.47217811201</v>
+        <v>14151.68818183644</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3390,16 +3390,16 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C137">
-        <v>7818.02330571639</v>
+        <v>10166.68671320246</v>
       </c>
       <c r="D137">
-        <v>5653.095564499369</v>
+        <v>7870.660600118454</v>
       </c>
       <c r="E137">
-        <v>6625.371912088781</v>
+        <v>8448.569974010888</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3407,16 +3407,16 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C138">
-        <v>8085.182658295945</v>
+        <v>40056.29615048355</v>
       </c>
       <c r="D138">
-        <v>7503.614943774021</v>
+        <v>39938.78970433185</v>
       </c>
       <c r="E138">
-        <v>8938.0868588093</v>
+        <v>44520.15917103966</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3424,16 +3424,16 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C139">
-        <v>14492.94704346139</v>
+        <v>42099.78280750295</v>
       </c>
       <c r="D139">
-        <v>11209.84775023005</v>
+        <v>42299.87775020443</v>
       </c>
       <c r="E139">
-        <v>10752.42132399964</v>
+        <v>47328.28098195308</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3441,16 +3441,16 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C140">
-        <v>14025.08468897277</v>
+        <v>6780.581746217548</v>
       </c>
       <c r="D140">
-        <v>11232.84453326727</v>
+        <v>5344.462556042371</v>
       </c>
       <c r="E140">
-        <v>12584.87999504888</v>
+        <v>5852.587839854697</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3458,16 +3458,16 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C141">
-        <v>2660.082565212768</v>
+        <v>7052.041776574091</v>
       </c>
       <c r="D141">
-        <v>2118.88338047299</v>
+        <v>2387.833946905571</v>
       </c>
       <c r="E141">
-        <v>2317.74860784036</v>
+        <v>2653.360912751024</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3475,16 +3475,16 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C142">
-        <v>6699.919359426849</v>
+        <v>12491.64080553533</v>
       </c>
       <c r="D142">
-        <v>3926.964562863937</v>
+        <v>7553.961214696117</v>
       </c>
       <c r="E142">
-        <v>5419.280756815793</v>
+        <v>8823.015551678049</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3492,16 +3492,16 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C143">
-        <v>4240.498957073307</v>
+        <v>11918.07029478611</v>
       </c>
       <c r="D143">
-        <v>2799.802017040321</v>
+        <v>10755.76769609013</v>
       </c>
       <c r="E143">
-        <v>3370.629266244694</v>
+        <v>11073.8263395291</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3509,16 +3509,16 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C144">
-        <v>3104.11640049039</v>
+        <v>2510.791313969085</v>
       </c>
       <c r="D144">
-        <v>2945.585161856526</v>
+        <v>2080.311820058766</v>
       </c>
       <c r="E144">
-        <v>3032.000269374993</v>
+        <v>2225.787307207039</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3526,16 +3526,16 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C145">
-        <v>4758.923090909089</v>
+        <v>5559.189168957029</v>
       </c>
       <c r="D145">
-        <v>4052.36859619171</v>
+        <v>3507.429258284409</v>
       </c>
       <c r="E145">
-        <v>4241.271500156832</v>
+        <v>4514.632917614302</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3543,16 +3543,16 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C146">
-        <v>4582.423026269129</v>
+        <v>3740.698985412615</v>
       </c>
       <c r="D146">
-        <v>3677.660725632635</v>
+        <v>456.0519360615073</v>
       </c>
       <c r="E146">
-        <v>3936.041511138754</v>
+        <v>595.516072795263</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3560,16 +3560,16 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C147">
-        <v>8274.311032145955</v>
+        <v>3025.982972811596</v>
       </c>
       <c r="D147">
-        <v>4554.906523253632</v>
+        <v>2930.200017528361</v>
       </c>
       <c r="E147">
-        <v>6530.74208924048</v>
+        <v>2972.156458241908</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3577,16 +3577,16 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C148">
-        <v>2362.496887971177</v>
+        <v>4384.134004159239</v>
       </c>
       <c r="D148">
-        <v>4552.94161730676</v>
+        <v>3877.68979844253</v>
       </c>
       <c r="E148">
-        <v>7699.768813994026</v>
+        <v>3984.413723700878</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3594,16 +3594,16 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C149">
-        <v>1764.352253203638</v>
+        <v>3818.113674370041</v>
       </c>
       <c r="D149">
-        <v>974.5725435688446</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E149">
-        <v>1393.90973989574</v>
+        <v>3773.270697207371</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3611,16 +3611,16 @@
         <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C150">
-        <v>921.2368963564281</v>
+        <v>5697.549039481555</v>
       </c>
       <c r="D150">
-        <v>0</v>
+        <v>4449.270708440607</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>4794.85366801385</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -3628,16 +3628,16 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C151">
-        <v>409436.7691592983</v>
+        <v>1675.03137312741</v>
       </c>
       <c r="D151">
-        <v>355341.7534723968</v>
+        <v>1815.4386330182</v>
       </c>
       <c r="E151">
-        <v>387999.3260030203</v>
+        <v>2049.263941768266</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3645,16 +3645,16 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C152">
-        <v>66424.65479531829</v>
+        <v>1388.615296125427</v>
       </c>
       <c r="D152">
-        <v>67311.96044664056</v>
+        <v>898.8243487684732</v>
       </c>
       <c r="E152">
-        <v>76231.77993843338</v>
+        <v>1101.853615098803</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3662,16 +3662,16 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C153">
-        <v>125858.7401545331</v>
+        <v>915.4210068592286</v>
       </c>
       <c r="D153">
-        <v>95923.88790038624</v>
+        <v>0</v>
       </c>
       <c r="E153">
-        <v>124140.5773429784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3679,16 +3679,16 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C154">
-        <v>55158.37308241575</v>
+        <v>379833.2126030341</v>
       </c>
       <c r="D154">
-        <v>54194.17670445503</v>
+        <v>323789.1870151541</v>
       </c>
       <c r="E154">
-        <v>54731.6463609033</v>
+        <v>342305.1273678984</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3696,16 +3696,16 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C155">
-        <v>18810.64774314864</v>
+        <v>66636.46327624648</v>
       </c>
       <c r="D155">
-        <v>26985.75868185313</v>
+        <v>57885.11081377808</v>
       </c>
       <c r="E155">
-        <v>33814.25416223275</v>
+        <v>65450.5214985832</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3713,16 +3713,16 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C156">
-        <v>11786.58854248258</v>
+        <v>122447.4212601383</v>
       </c>
       <c r="D156">
-        <v>9267.503482344102</v>
+        <v>106273.0478090824</v>
       </c>
       <c r="E156">
-        <v>10151.93626108859</v>
+        <v>119530.3850553175</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3730,16 +3730,16 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C157">
-        <v>41809.31820607139</v>
+        <v>55098.14072490651</v>
       </c>
       <c r="D157">
-        <v>39732.01918427406</v>
+        <v>53997.08352943832</v>
       </c>
       <c r="E157">
-        <v>46033.76592047335</v>
+        <v>54429.29718809373</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3747,16 +3747,16 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C158">
-        <v>44322.79570608526</v>
+        <v>17436.20392355449</v>
       </c>
       <c r="D158">
-        <v>42997.62304068729</v>
+        <v>19678.07818882393</v>
       </c>
       <c r="E158">
-        <v>49150.09462369821</v>
+        <v>23411.63616688988</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3764,16 +3764,16 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C159">
-        <v>7830.871226366395</v>
+        <v>11477.1443269179</v>
       </c>
       <c r="D159">
-        <v>5653.095564499369</v>
+        <v>7941.17271971979</v>
       </c>
       <c r="E159">
-        <v>6625.371912088781</v>
+        <v>8685.454438123739</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3781,16 +3781,16 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C160">
-        <v>8817.535269776827</v>
+        <v>44788.85407568982</v>
       </c>
       <c r="D160">
-        <v>9011.059942949789</v>
+        <v>42290.86139964137</v>
       </c>
       <c r="E160">
-        <v>10838.71267389012</v>
+        <v>48116.24030242601</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3798,16 +3798,16 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C161">
-        <v>15730.7337703995</v>
+        <v>43854.83257609577</v>
       </c>
       <c r="D161">
-        <v>12870.92751701806</v>
+        <v>42446.11108034404</v>
       </c>
       <c r="E161">
-        <v>16028.57827823479</v>
+        <v>48048.47217811201</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3815,16 +3815,16 @@
         <v>164</v>
       </c>
       <c r="B162" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C162">
-        <v>14763.70638988416</v>
+        <v>7818.02330571639</v>
       </c>
       <c r="D162">
-        <v>11353.82086139094</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E162">
-        <v>15744.22408353954</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3832,16 +3832,16 @@
         <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C163">
-        <v>2664.581838046233</v>
+        <v>8085.182658295945</v>
       </c>
       <c r="D163">
-        <v>2118.88338047299</v>
+        <v>7503.614943774021</v>
       </c>
       <c r="E163">
-        <v>2317.74860784036</v>
+        <v>8938.0868588093</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3849,16 +3849,16 @@
         <v>166</v>
       </c>
       <c r="B164" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C164">
-        <v>7118.299388486004</v>
+        <v>14492.94704346139</v>
       </c>
       <c r="D164">
-        <v>4387.796042371227</v>
+        <v>11209.84775023005</v>
       </c>
       <c r="E164">
-        <v>6214.950571608244</v>
+        <v>10752.42132399964</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3866,16 +3866,16 @@
         <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C165">
-        <v>1256.930682890124</v>
+        <v>14025.08468897277</v>
       </c>
       <c r="D165">
-        <v>634.2799162905493</v>
+        <v>11232.84453326727</v>
       </c>
       <c r="E165">
-        <v>1060.520130278657</v>
+        <v>12584.87999504888</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3883,16 +3883,16 @@
         <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C166">
-        <v>3104.11640049039</v>
+        <v>2660.082565212768</v>
       </c>
       <c r="D166">
-        <v>2953.473502833881</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E166">
-        <v>3032.074436227733</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3900,16 +3900,16 @@
         <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>6699.919359426849</v>
       </c>
       <c r="D167">
-        <v>0</v>
+        <v>3926.964562863937</v>
       </c>
       <c r="E167">
-        <v>1927.316250691574</v>
+        <v>5419.280756815793</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3917,16 +3917,16 @@
         <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C168">
-        <v>4982.658106436934</v>
+        <v>4240.498957073307</v>
       </c>
       <c r="D168">
-        <v>3682.745087885083</v>
+        <v>2799.802017040321</v>
       </c>
       <c r="E168">
-        <v>4606.149113368056</v>
+        <v>3370.629266244694</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3934,16 +3934,16 @@
         <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C169">
-        <v>9858.7475739898</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D169">
-        <v>4988.549100871839</v>
+        <v>2945.585161856526</v>
       </c>
       <c r="E169">
-        <v>9051.622561655677</v>
+        <v>3032.000269374993</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3951,16 +3951,16 @@
         <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C170">
-        <v>3049.962402814945</v>
+        <v>4758.923090909089</v>
       </c>
       <c r="D170">
-        <v>7885.799173422068</v>
+        <v>4052.36859619171</v>
       </c>
       <c r="E170">
-        <v>14476.78741030169</v>
+        <v>4241.271500156832</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3968,16 +3968,16 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C171">
-        <v>1932.537890358078</v>
+        <v>4582.423026269129</v>
       </c>
       <c r="D171">
-        <v>1092.439628676345</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E171">
-        <v>1729.767824059069</v>
+        <v>3936.041511138754</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3985,16 +3985,16 @@
         <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C172">
-        <v>927.0527858536279</v>
+        <v>8274.311032145955</v>
       </c>
       <c r="D172">
-        <v>885.4644642160963</v>
+        <v>4554.906523253632</v>
       </c>
       <c r="E172">
-        <v>854.6967352460968</v>
+        <v>6530.74208924048</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4002,16 +4002,16 @@
         <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C173">
-        <v>425667.2304377211</v>
+        <v>2362.496887971177</v>
       </c>
       <c r="D173">
-        <v>379452.4458343688</v>
+        <v>4552.94161730676</v>
       </c>
       <c r="E173">
-        <v>422462.404769241</v>
+        <v>7699.768813994026</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4019,16 +4019,16 @@
         <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C174">
-        <v>74824.1776942108</v>
+        <v>1764.352253203638</v>
       </c>
       <c r="D174">
-        <v>75532.04105321791</v>
+        <v>974.5725435688446</v>
       </c>
       <c r="E174">
-        <v>86492.52473873404</v>
+        <v>1393.90973989574</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -4036,16 +4036,16 @@
         <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C175">
-        <v>128549.8642605276</v>
+        <v>921.2368963564281</v>
       </c>
       <c r="D175">
-        <v>114702.4949950556</v>
+        <v>0</v>
       </c>
       <c r="E175">
-        <v>134200.4554046213</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4053,16 +4053,16 @@
         <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C176">
-        <v>55242.88725228325</v>
+        <v>409436.7691592983</v>
       </c>
       <c r="D176">
-        <v>54348.67956945477</v>
+        <v>355341.7534723968</v>
       </c>
       <c r="E176">
-        <v>54823.8158790419</v>
+        <v>387999.3260030203</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4070,16 +4070,16 @@
         <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C177">
-        <v>21186.42152206995</v>
+        <v>66424.65479531829</v>
       </c>
       <c r="D177">
-        <v>32192.86399794241</v>
+        <v>67311.96044664056</v>
       </c>
       <c r="E177">
-        <v>40091.29523030741</v>
+        <v>76231.77993843338</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -4087,16 +4087,16 @@
         <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C178">
-        <v>12108.98627481771</v>
+        <v>125858.7401545331</v>
       </c>
       <c r="D178">
-        <v>9710.044517252907</v>
+        <v>95923.88790038624</v>
       </c>
       <c r="E178">
-        <v>9820.712234959921</v>
+        <v>124140.5773429784</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -4104,16 +4104,16 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C179">
-        <v>44818.4592191087</v>
+        <v>55158.37308241575</v>
       </c>
       <c r="D179">
-        <v>43318.43942297382</v>
+        <v>54194.17670445503</v>
       </c>
       <c r="E179">
-        <v>50430.2444258372</v>
+        <v>54731.6463609033</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -4121,16 +4121,16 @@
         <v>182</v>
       </c>
       <c r="B180" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C180">
-        <v>45410.20682375576</v>
+        <v>18810.64774314864</v>
       </c>
       <c r="D180">
-        <v>44140.29328236685</v>
+        <v>26985.75868185313</v>
       </c>
       <c r="E180">
-        <v>50777.920807722</v>
+        <v>33814.25416223275</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4138,16 +4138,16 @@
         <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C181">
-        <v>7877.356799130208</v>
+        <v>11786.58854248258</v>
       </c>
       <c r="D181">
-        <v>5653.095564499369</v>
+        <v>9267.503482344102</v>
       </c>
       <c r="E181">
-        <v>6662.276843942194</v>
+        <v>10151.93626108859</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -4155,16 +4155,16 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C182">
-        <v>7081.366168574467</v>
+        <v>41809.31820607139</v>
       </c>
       <c r="D182">
-        <v>7237.854347805022</v>
+        <v>39732.01918427406</v>
       </c>
       <c r="E182">
-        <v>8761.01660377788</v>
+        <v>46033.76592047335</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -4172,16 +4172,16 @@
         <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C183">
-        <v>17240.04215367412</v>
+        <v>44322.79570608526</v>
       </c>
       <c r="D183">
-        <v>13942.82778271549</v>
+        <v>42997.62304068729</v>
       </c>
       <c r="E183">
-        <v>14713.17492592106</v>
+        <v>49150.09462369821</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4189,16 +4189,16 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C184">
-        <v>17324.03456184319</v>
+        <v>7830.871226366395</v>
       </c>
       <c r="D184">
-        <v>13476.54727078326</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E184">
-        <v>22628.13038686703</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -4206,16 +4206,16 @@
         <v>187</v>
       </c>
       <c r="B185" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C185">
-        <v>2689.033001442709</v>
+        <v>8817.535269776827</v>
       </c>
       <c r="D185">
-        <v>2118.88338047299</v>
+        <v>9011.059942949789</v>
       </c>
       <c r="E185">
-        <v>2326.478289412053</v>
+        <v>10838.71267389012</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -4223,16 +4223,16 @@
         <v>188</v>
       </c>
       <c r="B186" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C186">
-        <v>7330.001934671265</v>
+        <v>15730.7337703995</v>
       </c>
       <c r="D186">
-        <v>4696.892936408833</v>
+        <v>12870.92751701806</v>
       </c>
       <c r="E186">
-        <v>6336.909947377137</v>
+        <v>16028.57827823479</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -4240,16 +4240,16 @@
         <v>189</v>
       </c>
       <c r="B187" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C187">
-        <v>3666.34991690552</v>
+        <v>14763.70638988416</v>
       </c>
       <c r="D187">
-        <v>2659.16265449915</v>
+        <v>11353.82086139094</v>
       </c>
       <c r="E187">
-        <v>3251.428044629679</v>
+        <v>15744.22408353954</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -4257,16 +4257,16 @@
         <v>190</v>
       </c>
       <c r="B188" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C188">
-        <v>3110.615608057638</v>
+        <v>2664.581838046233</v>
       </c>
       <c r="D188">
-        <v>2966.871688417814</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E188">
-        <v>3044.077493176301</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -4274,16 +4274,16 @@
         <v>191</v>
       </c>
       <c r="B189" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C189">
-        <v>4955.203939982344</v>
+        <v>7118.299388486004</v>
       </c>
       <c r="D189">
-        <v>4437.491921939725</v>
+        <v>4387.796042371227</v>
       </c>
       <c r="E189">
-        <v>4802.656681354792</v>
+        <v>6214.950571608244</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -4291,16 +4291,16 @@
         <v>192</v>
       </c>
       <c r="B190" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C190">
-        <v>5584.532853170555</v>
+        <v>1256.930682890124</v>
       </c>
       <c r="D190">
-        <v>3696.358431113311</v>
+        <v>634.2799162905493</v>
       </c>
       <c r="E190">
-        <v>5041.150517084573</v>
+        <v>1060.520130278657</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4308,16 +4308,16 @@
         <v>193</v>
       </c>
       <c r="B191" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C191">
-        <v>12228.85287007065</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D191">
-        <v>5315.793599021267</v>
+        <v>2953.473502833881</v>
       </c>
       <c r="E191">
-        <v>10793.64798057903</v>
+        <v>3032.074436227733</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4325,16 +4325,16 @@
         <v>194</v>
       </c>
       <c r="B192" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C192">
-        <v>3909.407627315059</v>
+        <v>0</v>
       </c>
       <c r="D192">
-        <v>12148.67547071851</v>
+        <v>0</v>
       </c>
       <c r="E192">
-        <v>24644.07599310096</v>
+        <v>1927.316250691574</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4342,16 +4342,16 @@
         <v>195</v>
       </c>
       <c r="B193" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C193">
-        <v>2078.961774546943</v>
+        <v>4982.658106436934</v>
       </c>
       <c r="D193">
-        <v>1179.897477494976</v>
+        <v>3682.745087885083</v>
       </c>
       <c r="E193">
-        <v>1832.168256550158</v>
+        <v>4606.149113368056</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4359,16 +4359,16 @@
         <v>196</v>
       </c>
       <c r="B194" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C194">
-        <v>932.8686753508275</v>
+        <v>9858.7475739898</v>
       </c>
       <c r="D194">
-        <v>920.6062716110156</v>
+        <v>4988.549100871839</v>
       </c>
       <c r="E194">
-        <v>0</v>
+        <v>9051.622561655677</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -4376,16 +4376,16 @@
         <v>197</v>
       </c>
       <c r="B195" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C195">
-        <v>195705.6</v>
+        <v>3049.962402814945</v>
       </c>
       <c r="D195">
-        <v>184867.2</v>
+        <v>7885.799173422068</v>
       </c>
       <c r="E195">
-        <v>187784</v>
+        <v>14476.78741030169</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -4393,16 +4393,16 @@
         <v>198</v>
       </c>
       <c r="B196" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C196">
-        <v>223624</v>
+        <v>1932.537890358078</v>
       </c>
       <c r="D196">
-        <v>205627.2</v>
+        <v>1092.439628676345</v>
       </c>
       <c r="E196">
-        <v>214700.8</v>
+        <v>1729.767824059069</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4410,16 +4410,16 @@
         <v>199</v>
       </c>
       <c r="B197" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C197">
-        <v>253637.6</v>
+        <v>927.0527858536279</v>
       </c>
       <c r="D197">
-        <v>224994.4</v>
+        <v>885.4644642160963</v>
       </c>
       <c r="E197">
-        <v>242126.4</v>
+        <v>854.6967352460968</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4427,16 +4427,16 @@
         <v>200</v>
       </c>
       <c r="B198" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C198">
-        <v>284854.4</v>
+        <v>425667.2304377211</v>
       </c>
       <c r="D198">
-        <v>242956.8</v>
+        <v>379452.4458343688</v>
       </c>
       <c r="E198">
-        <v>270748</v>
+        <v>422462.404769241</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4444,16 +4444,16 @@
         <v>201</v>
       </c>
       <c r="B199" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C199">
-        <v>275764.8</v>
+        <v>74824.1776942108</v>
       </c>
       <c r="D199">
-        <v>258018.4</v>
+        <v>75532.04105321791</v>
       </c>
       <c r="E199">
-        <v>296766.4</v>
+        <v>86492.52473873404</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4461,16 +4461,16 @@
         <v>202</v>
       </c>
       <c r="B200" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C200">
-        <v>285775.2</v>
+        <v>128549.8642605276</v>
       </c>
       <c r="D200">
-        <v>276530.4</v>
+        <v>114702.4949950556</v>
       </c>
       <c r="E200">
-        <v>326134.4</v>
+        <v>134200.4554046213</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4478,16 +4478,16 @@
         <v>203</v>
       </c>
       <c r="B201" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C201">
-        <v>181481.6</v>
+        <v>55242.88725228325</v>
       </c>
       <c r="D201">
-        <v>171418.4</v>
+        <v>54348.67956945477</v>
       </c>
       <c r="E201">
-        <v>173696</v>
+        <v>54823.8158790419</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4495,16 +4495,16 @@
         <v>204</v>
       </c>
       <c r="B202" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C202">
-        <v>206952</v>
+        <v>21186.42152206995</v>
       </c>
       <c r="D202">
-        <v>183019.2</v>
+        <v>32192.86399794241</v>
       </c>
       <c r="E202">
-        <v>189584.8</v>
+        <v>40091.29523030741</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4512,16 +4512,16 @@
         <v>205</v>
       </c>
       <c r="B203" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C203">
-        <v>236529.6</v>
+        <v>12108.98627481771</v>
       </c>
       <c r="D203">
-        <v>204145.6</v>
+        <v>9710.044517252907</v>
       </c>
       <c r="E203">
-        <v>217076.8</v>
+        <v>9820.712234959921</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4529,16 +4529,16 @@
         <v>206</v>
       </c>
       <c r="B204" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C204">
-        <v>266166.4</v>
+        <v>44818.4592191087</v>
       </c>
       <c r="D204">
-        <v>221178.4</v>
+        <v>43318.43942297382</v>
       </c>
       <c r="E204">
-        <v>243465.6</v>
+        <v>50430.2444258372</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4546,16 +4546,16 @@
         <v>207</v>
       </c>
       <c r="B205" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C205">
-        <v>266616</v>
+        <v>45410.20682375576</v>
       </c>
       <c r="D205">
-        <v>234677.6</v>
+        <v>44140.29328236685</v>
       </c>
       <c r="E205">
-        <v>267149.6</v>
+        <v>50777.920807722</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4563,16 +4563,16 @@
         <v>208</v>
       </c>
       <c r="B206" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C206">
-        <v>275787.2</v>
+        <v>7877.356799130208</v>
       </c>
       <c r="D206">
-        <v>252004</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E206">
-        <v>295416</v>
+        <v>6662.276843942194</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -4580,16 +4580,16 @@
         <v>209</v>
       </c>
       <c r="B207" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C207">
-        <v>166797.6</v>
+        <v>7081.366168574467</v>
       </c>
       <c r="D207">
-        <v>173032.8</v>
+        <v>7237.854347805022</v>
       </c>
       <c r="E207">
-        <v>175456.8</v>
+        <v>8761.01660377788</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -4597,16 +4597,16 @@
         <v>210</v>
       </c>
       <c r="B208" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C208">
-        <v>187860.8</v>
+        <v>17240.04215367412</v>
       </c>
       <c r="D208">
-        <v>192721.6</v>
+        <v>13942.82778271549</v>
       </c>
       <c r="E208">
-        <v>199666.4</v>
+        <v>14713.17492592106</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -4614,16 +4614,16 @@
         <v>211</v>
       </c>
       <c r="B209" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C209">
-        <v>214399.2</v>
+        <v>17324.03456184319</v>
       </c>
       <c r="D209">
-        <v>208928.8</v>
+        <v>13476.54727078326</v>
       </c>
       <c r="E209">
-        <v>221102.4</v>
+        <v>22628.13038686703</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -4631,16 +4631,16 @@
         <v>212</v>
       </c>
       <c r="B210" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C210">
-        <v>240393.6</v>
+        <v>2689.033001442709</v>
       </c>
       <c r="D210">
-        <v>232657.6</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E210">
-        <v>254091.2</v>
+        <v>2326.478289412053</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -4648,16 +4648,16 @@
         <v>213</v>
       </c>
       <c r="B211" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C211">
-        <v>266132</v>
+        <v>7330.001934671265</v>
       </c>
       <c r="D211">
-        <v>251892</v>
+        <v>4696.892936408833</v>
       </c>
       <c r="E211">
-        <v>284350.4</v>
+        <v>6336.909947377137</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -4665,15 +4665,440 @@
         <v>214</v>
       </c>
       <c r="B212" t="s">
+        <v>241</v>
+      </c>
+      <c r="C212">
+        <v>3666.34991690552</v>
+      </c>
+      <c r="D212">
+        <v>2659.16265449915</v>
+      </c>
+      <c r="E212">
+        <v>3251.428044629679</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B213" t="s">
+        <v>241</v>
+      </c>
+      <c r="C213">
+        <v>3110.615608057638</v>
+      </c>
+      <c r="D213">
+        <v>2966.871688417814</v>
+      </c>
+      <c r="E213">
+        <v>3044.077493176301</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C212">
+      <c r="B214" t="s">
+        <v>241</v>
+      </c>
+      <c r="C214">
+        <v>4955.203939982344</v>
+      </c>
+      <c r="D214">
+        <v>4437.491921939725</v>
+      </c>
+      <c r="E214">
+        <v>4802.656681354792</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B215" t="s">
+        <v>241</v>
+      </c>
+      <c r="C215">
+        <v>5584.532853170555</v>
+      </c>
+      <c r="D215">
+        <v>3696.358431113311</v>
+      </c>
+      <c r="E215">
+        <v>5041.150517084573</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B216" t="s">
+        <v>241</v>
+      </c>
+      <c r="C216">
+        <v>12228.85287007065</v>
+      </c>
+      <c r="D216">
+        <v>5315.793599021267</v>
+      </c>
+      <c r="E216">
+        <v>10793.64798057903</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B217" t="s">
+        <v>241</v>
+      </c>
+      <c r="C217">
+        <v>3909.407627315059</v>
+      </c>
+      <c r="D217">
+        <v>12148.67547071851</v>
+      </c>
+      <c r="E217">
+        <v>24644.07599310096</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B218" t="s">
+        <v>241</v>
+      </c>
+      <c r="C218">
+        <v>2078.961774546943</v>
+      </c>
+      <c r="D218">
+        <v>1179.897477494976</v>
+      </c>
+      <c r="E218">
+        <v>1832.168256550158</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B219" t="s">
+        <v>241</v>
+      </c>
+      <c r="C219">
+        <v>932.8686753508275</v>
+      </c>
+      <c r="D219">
+        <v>920.6062716110156</v>
+      </c>
+      <c r="E219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B220" t="s">
+        <v>241</v>
+      </c>
+      <c r="C220">
+        <v>195705.6</v>
+      </c>
+      <c r="D220">
+        <v>184867.2</v>
+      </c>
+      <c r="E220">
+        <v>187784</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B221" t="s">
+        <v>241</v>
+      </c>
+      <c r="C221">
+        <v>223624</v>
+      </c>
+      <c r="D221">
+        <v>205627.2</v>
+      </c>
+      <c r="E221">
+        <v>214700.8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B222" t="s">
+        <v>241</v>
+      </c>
+      <c r="C222">
+        <v>253637.6</v>
+      </c>
+      <c r="D222">
+        <v>224994.4</v>
+      </c>
+      <c r="E222">
+        <v>242126.4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B223" t="s">
+        <v>241</v>
+      </c>
+      <c r="C223">
+        <v>284854.4</v>
+      </c>
+      <c r="D223">
+        <v>242956.8</v>
+      </c>
+      <c r="E223">
+        <v>270748</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B224" t="s">
+        <v>241</v>
+      </c>
+      <c r="C224">
+        <v>275764.8</v>
+      </c>
+      <c r="D224">
+        <v>258018.4</v>
+      </c>
+      <c r="E224">
+        <v>296766.4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B225" t="s">
+        <v>241</v>
+      </c>
+      <c r="C225">
+        <v>285775.2</v>
+      </c>
+      <c r="D225">
+        <v>276530.4</v>
+      </c>
+      <c r="E225">
+        <v>326134.4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B226" t="s">
+        <v>241</v>
+      </c>
+      <c r="C226">
+        <v>181481.6</v>
+      </c>
+      <c r="D226">
+        <v>171418.4</v>
+      </c>
+      <c r="E226">
+        <v>173696</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B227" t="s">
+        <v>241</v>
+      </c>
+      <c r="C227">
+        <v>206952</v>
+      </c>
+      <c r="D227">
+        <v>183019.2</v>
+      </c>
+      <c r="E227">
+        <v>189584.8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B228" t="s">
+        <v>241</v>
+      </c>
+      <c r="C228">
+        <v>236529.6</v>
+      </c>
+      <c r="D228">
+        <v>204145.6</v>
+      </c>
+      <c r="E228">
+        <v>217076.8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B229" t="s">
+        <v>241</v>
+      </c>
+      <c r="C229">
+        <v>266166.4</v>
+      </c>
+      <c r="D229">
+        <v>221178.4</v>
+      </c>
+      <c r="E229">
+        <v>243465.6</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B230" t="s">
+        <v>241</v>
+      </c>
+      <c r="C230">
+        <v>266616</v>
+      </c>
+      <c r="D230">
+        <v>234677.6</v>
+      </c>
+      <c r="E230">
+        <v>267149.6</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B231" t="s">
+        <v>241</v>
+      </c>
+      <c r="C231">
+        <v>275787.2</v>
+      </c>
+      <c r="D231">
+        <v>252004</v>
+      </c>
+      <c r="E231">
+        <v>295416</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B232" t="s">
+        <v>241</v>
+      </c>
+      <c r="C232">
+        <v>166797.6</v>
+      </c>
+      <c r="D232">
+        <v>173032.8</v>
+      </c>
+      <c r="E232">
+        <v>175456.8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B233" t="s">
+        <v>241</v>
+      </c>
+      <c r="C233">
+        <v>187860.8</v>
+      </c>
+      <c r="D233">
+        <v>192721.6</v>
+      </c>
+      <c r="E233">
+        <v>199666.4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B234" t="s">
+        <v>241</v>
+      </c>
+      <c r="C234">
+        <v>214399.2</v>
+      </c>
+      <c r="D234">
+        <v>208928.8</v>
+      </c>
+      <c r="E234">
+        <v>221102.4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B235" t="s">
+        <v>241</v>
+      </c>
+      <c r="C235">
+        <v>240393.6</v>
+      </c>
+      <c r="D235">
+        <v>232657.6</v>
+      </c>
+      <c r="E235">
+        <v>254091.2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B236" t="s">
+        <v>241</v>
+      </c>
+      <c r="C236">
+        <v>266132</v>
+      </c>
+      <c r="D236">
+        <v>251892</v>
+      </c>
+      <c r="E236">
+        <v>284350.4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B237" t="s">
+        <v>241</v>
+      </c>
+      <c r="C237">
         <v>277836.8</v>
       </c>
-      <c r="D212">
+      <c r="D237">
         <v>271554.4</v>
       </c>
-      <c r="E212">
+      <c r="E237">
         <v>316714.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DP: create_forecast_basic - utils - monitoring_df.ipynb - fix add_percentage_growth_by_sector_row: current_year == previous_year
</commit_message>
<xml_diff>
--- a/create_forecast_basic/utils/monitoring_df.xlsx
+++ b/create_forecast_basic/utils/monitoring_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="263">
   <si>
     <t>2020</t>
   </si>
@@ -190,19 +190,34 @@
     <t>percentage growth arabs_behined_seperation_wall 2035-2040</t>
   </si>
   <si>
-    <t>percentage growth Arab 2050-2045</t>
-  </si>
-  <si>
-    <t>percentage growth Jewish 2050-2045</t>
-  </si>
-  <si>
-    <t>percentage growth Palestinian 2050-2045</t>
-  </si>
-  <si>
-    <t>percentage growth U_Orthodox 2050-2045</t>
-  </si>
-  <si>
-    <t>percentage growth arabs_behined_seperation_wall 2050-2045</t>
+    <t>percentage growth Arab 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall 2040-2045</t>
+  </si>
+  <si>
+    <t>percentage growth Arab 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth Jewish 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth Palestinian 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth U_Orthodox 2045-2050</t>
+  </si>
+  <si>
+    <t>percentage growth arabs_behined_seperation_wall 2045-2050</t>
   </si>
   <si>
     <t>percentage growth BaseProjections age20_29 2025-2030</t>
@@ -1145,7 +1160,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E237"/>
+  <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1170,16 +1185,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1187,16 +1202,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="E3" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1204,16 +1219,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D4" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E4" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1221,16 +1236,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D5" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E5" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1323,16 +1338,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C11" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E11" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1340,16 +1355,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D12" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E12" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1357,16 +1372,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C13" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D13" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="E13" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1374,16 +1389,16 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="D14" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="E14" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1391,16 +1406,16 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C15" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D15" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E15" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1408,16 +1423,16 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="E16" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1578,16 +1593,16 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C26">
-        <v>288</v>
+        <v>288.1410644079083</v>
       </c>
       <c r="D26">
-        <v>283</v>
+        <v>283.9696620191286</v>
       </c>
       <c r="E26">
-        <v>285</v>
+        <v>285.6774324006337</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1595,16 +1610,16 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C27">
-        <v>110</v>
+        <v>110.4611796870228</v>
       </c>
       <c r="D27">
-        <v>109</v>
+        <v>109.2979336473809</v>
       </c>
       <c r="E27">
-        <v>110</v>
+        <v>110.4035195766238</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1612,16 +1627,16 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C28">
-        <v>109</v>
+        <v>109.975617699839</v>
       </c>
       <c r="D28">
-        <v>108</v>
+        <v>108.6019787529929</v>
       </c>
       <c r="E28">
-        <v>109</v>
+        <v>109.721890131482</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1629,16 +1644,16 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C29">
-        <v>109</v>
+        <v>109.051601597595</v>
       </c>
       <c r="D29">
-        <v>107</v>
+        <v>107.611918043502</v>
       </c>
       <c r="E29">
-        <v>109</v>
+        <v>109.0300322919788</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1646,16 +1661,16 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C30">
-        <v>94</v>
+        <v>94.67184495473032</v>
       </c>
       <c r="D30">
-        <v>93</v>
+        <v>93.61444029023103</v>
       </c>
       <c r="E30">
-        <v>92</v>
+        <v>92.48650039603555</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1663,7 +1678,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -1680,7 +1695,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1697,7 +1712,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C33">
         <v>100</v>
@@ -1714,7 +1729,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C34">
         <v>100</v>
@@ -1731,7 +1746,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C35">
         <v>100</v>
@@ -1748,13 +1763,13 @@
         <v>38</v>
       </c>
       <c r="C36">
-        <v>112</v>
+        <v>112.3202972412109</v>
       </c>
       <c r="D36">
-        <v>111</v>
+        <v>111.3030700683594</v>
       </c>
       <c r="E36">
-        <v>111</v>
+        <v>111.842399597168</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1762,13 +1777,13 @@
         <v>39</v>
       </c>
       <c r="C37">
-        <v>114</v>
+        <v>114.3151168823242</v>
       </c>
       <c r="D37">
-        <v>107</v>
+        <v>107.5494537353516</v>
       </c>
       <c r="E37">
-        <v>109</v>
+        <v>109.3707275390625</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1790,13 +1805,13 @@
         <v>41</v>
       </c>
       <c r="C39">
-        <v>122</v>
+        <v>122.9322967529297</v>
       </c>
       <c r="D39">
-        <v>120</v>
+        <v>120.7884521484375</v>
       </c>
       <c r="E39">
-        <v>123</v>
+        <v>123.14892578125</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1804,13 +1819,13 @@
         <v>42</v>
       </c>
       <c r="C40">
-        <v>114</v>
+        <v>114.5723495483398</v>
       </c>
       <c r="D40">
-        <v>113</v>
+        <v>113.2040252685547</v>
       </c>
       <c r="E40">
-        <v>113</v>
+        <v>113.7573547363281</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1818,13 +1833,13 @@
         <v>43</v>
       </c>
       <c r="C41">
-        <v>111</v>
+        <v>111.661750793457</v>
       </c>
       <c r="D41">
-        <v>108</v>
+        <v>108.5102615356445</v>
       </c>
       <c r="E41">
-        <v>109</v>
+        <v>109.7856826782227</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1832,13 +1847,13 @@
         <v>44</v>
       </c>
       <c r="C42">
-        <v>114</v>
+        <v>114.0274200439453</v>
       </c>
       <c r="D42">
-        <v>108</v>
+        <v>108.323356628418</v>
       </c>
       <c r="E42">
-        <v>111</v>
+        <v>111.0597229003906</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1846,13 +1861,13 @@
         <v>45</v>
       </c>
       <c r="C43">
-        <v>108</v>
+        <v>108.2132720947266</v>
       </c>
       <c r="D43">
-        <v>108</v>
+        <v>108.2132720947266</v>
       </c>
       <c r="E43">
-        <v>108</v>
+        <v>108.2132720947266</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1860,13 +1875,13 @@
         <v>46</v>
       </c>
       <c r="C44">
-        <v>114</v>
+        <v>114.3493194580078</v>
       </c>
       <c r="D44">
-        <v>116</v>
+        <v>116.0060729980469</v>
       </c>
       <c r="E44">
-        <v>119</v>
+        <v>119.6857528686523</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1874,13 +1889,13 @@
         <v>47</v>
       </c>
       <c r="C45">
-        <v>113</v>
+        <v>113.9139022827148</v>
       </c>
       <c r="D45">
-        <v>110</v>
+        <v>110.5818710327148</v>
       </c>
       <c r="E45">
-        <v>111</v>
+        <v>111.8965606689453</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1888,13 +1903,13 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>111</v>
+        <v>111.4065017700195</v>
       </c>
       <c r="D46">
-        <v>108</v>
+        <v>108.8073043823242</v>
       </c>
       <c r="E46">
-        <v>110</v>
+        <v>110.0499496459961</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1902,13 +1917,13 @@
         <v>49</v>
       </c>
       <c r="C47">
-        <v>115</v>
+        <v>115.2005615234375</v>
       </c>
       <c r="D47">
-        <v>108</v>
+        <v>108.5818710327148</v>
       </c>
       <c r="E47">
-        <v>110</v>
+        <v>110.9671173095703</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1916,13 +1931,13 @@
         <v>50</v>
       </c>
       <c r="C48">
-        <v>107</v>
+        <v>107.2044982910156</v>
       </c>
       <c r="D48">
-        <v>107</v>
+        <v>107.2044982910156</v>
       </c>
       <c r="E48">
-        <v>107</v>
+        <v>107.2044982910156</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1930,13 +1945,13 @@
         <v>51</v>
       </c>
       <c r="C49">
-        <v>113</v>
+        <v>113.8025817871094</v>
       </c>
       <c r="D49">
-        <v>115</v>
+        <v>115.0981063842773</v>
       </c>
       <c r="E49">
-        <v>118</v>
+        <v>118.8546524047852</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1944,13 +1959,13 @@
         <v>52</v>
       </c>
       <c r="C50">
-        <v>109</v>
+        <v>109.2754135131836</v>
       </c>
       <c r="D50">
-        <v>106</v>
+        <v>106.5745468139648</v>
       </c>
       <c r="E50">
-        <v>107</v>
+        <v>107.8064422607422</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1958,13 +1973,13 @@
         <v>53</v>
       </c>
       <c r="C51">
-        <v>111</v>
+        <v>111.4402313232422</v>
       </c>
       <c r="D51">
-        <v>108</v>
+        <v>108.4855270385742</v>
       </c>
       <c r="E51">
-        <v>110</v>
+        <v>110.432861328125</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1972,13 +1987,13 @@
         <v>54</v>
       </c>
       <c r="C52">
-        <v>115</v>
+        <v>115.7983703613281</v>
       </c>
       <c r="D52">
-        <v>107</v>
+        <v>107.3515243530273</v>
       </c>
       <c r="E52">
-        <v>109</v>
+        <v>109.9095687866211</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1986,13 +2001,13 @@
         <v>55</v>
       </c>
       <c r="C53">
-        <v>106</v>
+        <v>106.3913955688477</v>
       </c>
       <c r="D53">
-        <v>106</v>
+        <v>106.3913955688477</v>
       </c>
       <c r="E53">
-        <v>106</v>
+        <v>106.3913955688477</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2000,13 +2015,13 @@
         <v>56</v>
       </c>
       <c r="C54">
-        <v>109</v>
+        <v>109.6991577148438</v>
       </c>
       <c r="D54">
-        <v>113</v>
+        <v>113.7160949707031</v>
       </c>
       <c r="E54">
-        <v>118</v>
+        <v>118.3788070678711</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2014,13 +2029,13 @@
         <v>57</v>
       </c>
       <c r="C55">
-        <v>103</v>
+        <v>103.6191787719727</v>
       </c>
       <c r="D55">
-        <v>100</v>
+        <v>100.9641647338867</v>
       </c>
       <c r="E55">
-        <v>102</v>
+        <v>102.7881393432617</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2028,13 +2043,13 @@
         <v>58</v>
       </c>
       <c r="C56">
-        <v>99</v>
+        <v>108.0526351928711</v>
       </c>
       <c r="D56">
-        <v>95</v>
+        <v>107.7009811401367</v>
       </c>
       <c r="E56">
-        <v>93</v>
+        <v>109.5689926147461</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2042,13 +2057,13 @@
         <v>59</v>
       </c>
       <c r="C57">
-        <v>93</v>
+        <v>108.9937896728516</v>
       </c>
       <c r="D57">
-        <v>96</v>
+        <v>104.2914199829102</v>
       </c>
       <c r="E57">
-        <v>94</v>
+        <v>106.7485198974609</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2056,13 +2071,13 @@
         <v>60</v>
       </c>
       <c r="C58">
-        <v>94</v>
+        <v>105.8768997192383</v>
       </c>
       <c r="D58">
-        <v>94</v>
+        <v>105.8768997192383</v>
       </c>
       <c r="E58">
-        <v>94</v>
+        <v>105.8768997192383</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2070,13 +2085,13 @@
         <v>61</v>
       </c>
       <c r="C59">
-        <v>95</v>
+        <v>105.8174667358398</v>
       </c>
       <c r="D59">
-        <v>87</v>
+        <v>114.2177886962891</v>
       </c>
       <c r="E59">
-        <v>85</v>
+        <v>117.9976348876953</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2084,183 +2099,168 @@
         <v>62</v>
       </c>
       <c r="C60">
-        <v>100</v>
+        <v>100.2247543334961</v>
       </c>
       <c r="D60">
-        <v>95</v>
+        <v>99.93392944335938</v>
       </c>
       <c r="E60">
-        <v>93</v>
+        <v>101.6650161743164</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B61" t="s">
-        <v>241</v>
-      </c>
       <c r="C61">
-        <v>112</v>
+        <v>100.3374252319336</v>
       </c>
       <c r="D61">
-        <v>111</v>
+        <v>105.1654663085938</v>
       </c>
       <c r="E61">
-        <v>114</v>
+        <v>106.7888488769531</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B62" t="s">
-        <v>241</v>
-      </c>
       <c r="C62">
-        <v>111</v>
+        <v>107.3705596923828</v>
       </c>
       <c r="D62">
-        <v>111</v>
+        <v>103.8991165161133</v>
       </c>
       <c r="E62">
-        <v>113</v>
+        <v>106.160888671875</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B63" t="s">
-        <v>241</v>
-      </c>
       <c r="C63">
-        <v>111</v>
+        <v>105.9054794311523</v>
       </c>
       <c r="D63">
-        <v>108</v>
+        <v>105.9054794311523</v>
       </c>
       <c r="E63">
-        <v>110</v>
+        <v>105.9054794311523</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B64" t="s">
-        <v>241</v>
-      </c>
       <c r="C64">
-        <v>116</v>
+        <v>104.9963073730469</v>
       </c>
       <c r="D64">
-        <v>108</v>
+        <v>114.1932830810547</v>
       </c>
       <c r="E64">
-        <v>110</v>
+        <v>117.6402359008789</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B65" t="s">
-        <v>241</v>
-      </c>
       <c r="C65">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D65">
-        <v>108</v>
+        <v>104.9321594238281</v>
       </c>
       <c r="E65">
-        <v>111</v>
+        <v>106.5721893310547</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B66">
-        <v>213239.3333333333</v>
+      <c r="B66" t="s">
+        <v>246</v>
       </c>
       <c r="C66">
-        <v>213239.3333333333</v>
+        <v>112.8455840496009</v>
       </c>
       <c r="D66">
-        <v>213239.3333333333</v>
+        <v>111.2912114030979</v>
       </c>
       <c r="E66">
-        <v>213239.3333333333</v>
+        <v>114.4679416256547</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B67">
-        <v>28627.66666666667</v>
+      <c r="B67" t="s">
+        <v>246</v>
       </c>
       <c r="C67">
-        <v>28627.66666666667</v>
+        <v>111.0718324025138</v>
       </c>
       <c r="D67">
-        <v>28627.66666666667</v>
+        <v>111.595294236761</v>
       </c>
       <c r="E67">
-        <v>28627.66666666667</v>
+        <v>113.9493834526651</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B68">
-        <v>46063</v>
+      <c r="B68" t="s">
+        <v>246</v>
       </c>
       <c r="C68">
-        <v>46063</v>
+        <v>111.0021464070356</v>
       </c>
       <c r="D68">
-        <v>46063</v>
+        <v>108.2587613381919</v>
       </c>
       <c r="E68">
-        <v>46063</v>
+        <v>110.9620476610768</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B69">
-        <v>23828</v>
+      <c r="B69" t="s">
+        <v>246</v>
       </c>
       <c r="C69">
-        <v>23828</v>
+        <v>116.6204415945845</v>
       </c>
       <c r="D69">
-        <v>23828</v>
+        <v>108.4470054591429</v>
       </c>
       <c r="E69">
-        <v>23828</v>
+        <v>110.8047012503858</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B70">
-        <v>8538</v>
+      <c r="B70" t="s">
+        <v>246</v>
       </c>
       <c r="C70">
-        <v>8538</v>
+        <v>106.4850397874526</v>
       </c>
       <c r="D70">
-        <v>8538</v>
+        <v>108.5232023695318</v>
       </c>
       <c r="E70">
-        <v>8538</v>
+        <v>111.329329828833</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2268,16 +2268,16 @@
         <v>73</v>
       </c>
       <c r="B71">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="C71">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="D71">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
       <c r="E71">
-        <v>5048</v>
+        <v>213239.3333333333</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2285,16 +2285,16 @@
         <v>74</v>
       </c>
       <c r="B72">
-        <v>21988.00000000001</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="C72">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="D72">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
       <c r="E72">
-        <v>21988</v>
+        <v>28627.66666666667</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2302,16 +2302,16 @@
         <v>75</v>
       </c>
       <c r="B73">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="C73">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="D73">
-        <v>27262</v>
+        <v>46063</v>
       </c>
       <c r="E73">
-        <v>27262</v>
+        <v>46063</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2319,16 +2319,16 @@
         <v>76</v>
       </c>
       <c r="B74">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="C74">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="D74">
-        <v>2804</v>
+        <v>23828</v>
       </c>
       <c r="E74">
-        <v>2804</v>
+        <v>23828</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2336,16 +2336,16 @@
         <v>77</v>
       </c>
       <c r="B75">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="C75">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="D75">
-        <v>1331</v>
+        <v>8538</v>
       </c>
       <c r="E75">
-        <v>1331</v>
+        <v>8538</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2353,16 +2353,16 @@
         <v>78</v>
       </c>
       <c r="B76">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="C76">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="D76">
-        <v>7375</v>
+        <v>5048</v>
       </c>
       <c r="E76">
-        <v>7375</v>
+        <v>5048</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2370,16 +2370,16 @@
         <v>79</v>
       </c>
       <c r="B77">
-        <v>8805</v>
+        <v>21988.00000000001</v>
       </c>
       <c r="C77">
-        <v>8805</v>
+        <v>21988</v>
       </c>
       <c r="D77">
-        <v>8805</v>
+        <v>21988</v>
       </c>
       <c r="E77">
-        <v>8805</v>
+        <v>21988</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2387,16 +2387,16 @@
         <v>80</v>
       </c>
       <c r="B78">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="C78">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="D78">
-        <v>1218</v>
+        <v>27262</v>
       </c>
       <c r="E78">
-        <v>1218</v>
+        <v>27262</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2404,16 +2404,16 @@
         <v>81</v>
       </c>
       <c r="B79">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="C79">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="D79">
-        <v>1673</v>
+        <v>2804</v>
       </c>
       <c r="E79">
-        <v>1673</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2421,16 +2421,16 @@
         <v>82</v>
       </c>
       <c r="B80">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="C80">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="D80">
-        <v>2401</v>
+        <v>1331</v>
       </c>
       <c r="E80">
-        <v>2401</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2438,16 +2438,16 @@
         <v>83</v>
       </c>
       <c r="B81">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="C81">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="D81">
-        <v>2488</v>
+        <v>7375</v>
       </c>
       <c r="E81">
-        <v>2488</v>
+        <v>7375</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2455,16 +2455,16 @@
         <v>84</v>
       </c>
       <c r="B82">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="C82">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="D82">
-        <v>2148</v>
+        <v>8805</v>
       </c>
       <c r="E82">
-        <v>2148</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2472,16 +2472,16 @@
         <v>85</v>
       </c>
       <c r="B83">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="C83">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="D83">
-        <v>3242</v>
+        <v>1218</v>
       </c>
       <c r="E83">
-        <v>3242</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2489,16 +2489,16 @@
         <v>86</v>
       </c>
       <c r="B84">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="C84">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="D84">
-        <v>3637</v>
+        <v>1673</v>
       </c>
       <c r="E84">
-        <v>3637</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2506,16 +2506,16 @@
         <v>87</v>
       </c>
       <c r="B85">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="C85">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="D85">
-        <v>301</v>
+        <v>2401</v>
       </c>
       <c r="E85">
-        <v>301</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2523,16 +2523,16 @@
         <v>88</v>
       </c>
       <c r="B86">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="C86">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="D86">
-        <v>537</v>
+        <v>2488</v>
       </c>
       <c r="E86">
-        <v>537</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2540,101 +2540,101 @@
         <v>89</v>
       </c>
       <c r="B87">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="C87">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="D87">
-        <v>300</v>
+        <v>2148</v>
       </c>
       <c r="E87">
-        <v>300</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B88" t="s">
-        <v>241</v>
+      <c r="B88">
+        <v>3242</v>
       </c>
       <c r="C88">
-        <v>285733.3218235314</v>
+        <v>3242</v>
       </c>
       <c r="D88">
-        <v>274161.0000038777</v>
+        <v>3242</v>
       </c>
       <c r="E88">
-        <v>275663.3373324008</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B89" t="s">
-        <v>241</v>
+      <c r="B89">
+        <v>3637</v>
       </c>
       <c r="C89">
-        <v>36057.66373063793</v>
+        <v>3637</v>
       </c>
       <c r="D89">
-        <v>33344.22909790605</v>
+        <v>3637</v>
       </c>
       <c r="E89">
-        <v>34286.84568702983</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B90" t="s">
-        <v>241</v>
+      <c r="B90">
+        <v>301</v>
       </c>
       <c r="C90">
-        <v>66822.51137331135</v>
+        <v>301</v>
       </c>
       <c r="D90">
-        <v>61855.23107261454</v>
+        <v>301</v>
       </c>
       <c r="E90">
-        <v>63948.66570649843</v>
+        <v>301</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B91" t="s">
-        <v>241</v>
+      <c r="B91">
+        <v>537</v>
       </c>
       <c r="C91">
-        <v>33156.30459804353</v>
+        <v>537</v>
       </c>
       <c r="D91">
-        <v>33335.50923218194</v>
+        <v>537</v>
       </c>
       <c r="E91">
-        <v>33397.07322472375</v>
+        <v>537</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B92" t="s">
-        <v>241</v>
+      <c r="B92">
+        <v>300</v>
       </c>
       <c r="C92">
-        <v>9986.417617537509</v>
+        <v>300</v>
       </c>
       <c r="D92">
-        <v>10194.62059102478</v>
+        <v>300</v>
       </c>
       <c r="E92">
-        <v>10338.40358091756</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2642,16 +2642,16 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C93">
-        <v>8306.813376518987</v>
+        <v>285733.3218235314</v>
       </c>
       <c r="D93">
-        <v>6946.591660718233</v>
+        <v>274161.0000038777</v>
       </c>
       <c r="E93">
-        <v>8135.667377017133</v>
+        <v>275663.3373324008</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2659,16 +2659,16 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C94">
-        <v>29427.44116169451</v>
+        <v>36057.66373063793</v>
       </c>
       <c r="D94">
-        <v>30953.22576377643</v>
+        <v>33344.22909790605</v>
       </c>
       <c r="E94">
-        <v>31386.31536916655</v>
+        <v>34286.84568702983</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2676,16 +2676,16 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C95">
-        <v>37145.33462606892</v>
+        <v>66822.51137331135</v>
       </c>
       <c r="D95">
-        <v>39041.11738664036</v>
+        <v>61855.23107261454</v>
       </c>
       <c r="E95">
-        <v>40239.51136715176</v>
+        <v>63948.66570649843</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2693,16 +2693,16 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C96">
-        <v>5309.478782988256</v>
+        <v>33156.30459804353</v>
       </c>
       <c r="D96">
-        <v>5060.408660766857</v>
+        <v>33335.50923218194</v>
       </c>
       <c r="E96">
-        <v>5201.12526897965</v>
+        <v>33397.07322472375</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2710,16 +2710,16 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C97">
-        <v>5521.895631861405</v>
+        <v>9986.417617537509</v>
       </c>
       <c r="D97">
-        <v>6073.616715538182</v>
+        <v>10194.62059102478</v>
       </c>
       <c r="E97">
-        <v>6265.692004112236</v>
+        <v>10338.40358091756</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2727,16 +2727,16 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C98">
-        <v>7012.74256878429</v>
+        <v>8306.813376518987</v>
       </c>
       <c r="D98">
-        <v>6467.15326810131</v>
+        <v>6946.591660718233</v>
       </c>
       <c r="E98">
-        <v>6547.602648720247</v>
+        <v>8135.667377017133</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2744,16 +2744,16 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C99">
-        <v>7317.313641591267</v>
+        <v>29427.44116169451</v>
       </c>
       <c r="D99">
-        <v>7240.499364931959</v>
+        <v>30953.22576377643</v>
       </c>
       <c r="E99">
-        <v>7309.076098225414</v>
+        <v>31386.31536916655</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2761,16 +2761,16 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C100">
-        <v>2166.404734331622</v>
+        <v>37145.33462606892</v>
       </c>
       <c r="D100">
-        <v>2013.947393383935</v>
+        <v>39041.11738664036</v>
       </c>
       <c r="E100">
-        <v>2067.009181064854</v>
+        <v>40239.51136715176</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2778,16 +2778,16 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C101">
-        <v>3081.965248662672</v>
+        <v>5309.478782988256</v>
       </c>
       <c r="D101">
-        <v>3137.447595991872</v>
+        <v>5060.408660766857</v>
       </c>
       <c r="E101">
-        <v>3186.615419267629</v>
+        <v>5201.12526897965</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2795,16 +2795,16 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C102">
-        <v>443.1341918519325</v>
+        <v>5521.895631861405</v>
       </c>
       <c r="D102">
-        <v>421.887538681912</v>
+        <v>6073.616715538182</v>
       </c>
       <c r="E102">
-        <v>433.4544189987498</v>
+        <v>6265.692004112236</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2812,16 +2812,16 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C103">
-        <v>2895.085614458657</v>
+        <v>7012.74256878429</v>
       </c>
       <c r="D103">
-        <v>2909.362870154178</v>
+        <v>6467.15326810131</v>
       </c>
       <c r="E103">
-        <v>2924.168116891962</v>
+        <v>6547.602648720247</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2829,16 +2829,16 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C104">
-        <v>3653.831655445544</v>
+        <v>7317.313641591267</v>
       </c>
       <c r="D104">
-        <v>3598.638480494133</v>
+        <v>7240.499364931959</v>
       </c>
       <c r="E104">
-        <v>3616.404971165329</v>
+        <v>7309.076098225414</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2846,16 +2846,16 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C105">
-        <v>3542.454003930634</v>
+        <v>2166.404734331622</v>
       </c>
       <c r="D105">
-        <v>3648.230892236539</v>
+        <v>2013.947393383935</v>
       </c>
       <c r="E105">
-        <v>3678.324608989895</v>
+        <v>2067.009181064854</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2863,16 +2863,16 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C106">
-        <v>4257.401768859199</v>
+        <v>3081.965248662672</v>
       </c>
       <c r="D106">
-        <v>4324.862744573556</v>
+        <v>3137.447595991872</v>
       </c>
       <c r="E106">
-        <v>4363.718311116243</v>
+        <v>3186.615419267629</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2880,16 +2880,16 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C107">
-        <v>881.1481005457115</v>
+        <v>443.1341918519325</v>
       </c>
       <c r="D107">
-        <v>922.4946308419028</v>
+        <v>421.887538681912</v>
       </c>
       <c r="E107">
-        <v>951.6553445648265</v>
+        <v>433.4544189987498</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2897,16 +2897,16 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C108">
-        <v>911.7413777070067</v>
+        <v>2895.085614458657</v>
       </c>
       <c r="D108">
-        <v>868.7478168054034</v>
+        <v>2909.362870154178</v>
       </c>
       <c r="E108">
-        <v>883.9572064300576</v>
+        <v>2924.168116891962</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2914,16 +2914,16 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>3653.831655445544</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>3598.638480494133</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>3616.404971165329</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2931,16 +2931,16 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C110">
-        <v>310887.0551086462</v>
+        <v>3542.454003930634</v>
       </c>
       <c r="D110">
-        <v>290797.302000507</v>
+        <v>3648.230892236539</v>
       </c>
       <c r="E110">
-        <v>292306.0034436272</v>
+        <v>3678.324608989895</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2948,16 +2948,16 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C111">
-        <v>51074.32436027069</v>
+        <v>4257.401768859199</v>
       </c>
       <c r="D111">
-        <v>26072.86402002085</v>
+        <v>4324.862744573556</v>
       </c>
       <c r="E111">
-        <v>44744.53526801307</v>
+        <v>4363.718311116243</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2965,16 +2965,16 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C112">
-        <v>84109.82719823082</v>
+        <v>881.1481005457115</v>
       </c>
       <c r="D112">
-        <v>77937.73156609248</v>
+        <v>922.4946308419028</v>
       </c>
       <c r="E112">
-        <v>84581.97612214876</v>
+        <v>951.6553445648265</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2982,16 +2982,16 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C113">
-        <v>39310.49274971832</v>
+        <v>911.7413777070067</v>
       </c>
       <c r="D113">
-        <v>38683.92515358835</v>
+        <v>868.7478168054034</v>
       </c>
       <c r="E113">
-        <v>38875.73769831542</v>
+        <v>883.9572064300576</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2999,16 +2999,16 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C114">
-        <v>11932.38400809033</v>
+        <v>0</v>
       </c>
       <c r="D114">
-        <v>10681.35241281803</v>
+        <v>0</v>
       </c>
       <c r="E114">
-        <v>11035.70441498311</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3016,16 +3016,16 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C115">
-        <v>9548.28031721313</v>
+        <v>310887.0551086462</v>
       </c>
       <c r="D115">
-        <v>7703.305735153427</v>
+        <v>290797.302000507</v>
       </c>
       <c r="E115">
-        <v>8161.797271070729</v>
+        <v>292306.0034436272</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3033,16 +3033,16 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C116">
-        <v>35810.66989709945</v>
+        <v>51074.32436027069</v>
       </c>
       <c r="D116">
-        <v>36601.69575249061</v>
+        <v>26072.86402002085</v>
       </c>
       <c r="E116">
-        <v>39241.8615517352</v>
+        <v>44744.53526801307</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3050,16 +3050,16 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C117">
-        <v>40274.91199119319</v>
+        <v>84109.82719823082</v>
       </c>
       <c r="D117">
-        <v>41351.35312049399</v>
+        <v>77937.73156609248</v>
       </c>
       <c r="E117">
-        <v>44632.82113421193</v>
+        <v>84581.97612214876</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3067,16 +3067,16 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C118">
-        <v>5702.582508173264</v>
+        <v>39310.49274971832</v>
       </c>
       <c r="D118">
-        <v>5197.04316560074</v>
+        <v>38683.92515358835</v>
       </c>
       <c r="E118">
-        <v>5490.350510109492</v>
+        <v>38875.73769831542</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3084,16 +3084,16 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C119">
-        <v>6531.454941380145</v>
+        <v>11932.38400809033</v>
       </c>
       <c r="D119">
-        <v>6914.424310549415</v>
+        <v>10681.35241281803</v>
       </c>
       <c r="E119">
-        <v>7565.494786531661</v>
+        <v>11035.70441498311</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3101,16 +3101,16 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C120">
-        <v>11086.07248419944</v>
+        <v>9548.28031721313</v>
       </c>
       <c r="D120">
-        <v>9081.046501582416</v>
+        <v>7703.305735153427</v>
       </c>
       <c r="E120">
-        <v>9712.39919620127</v>
+        <v>8161.797271070729</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3118,16 +3118,16 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C121">
-        <v>11235.01770760014</v>
+        <v>35810.66989709945</v>
       </c>
       <c r="D121">
-        <v>7294.264487669744</v>
+        <v>36601.69575249061</v>
       </c>
       <c r="E121">
-        <v>7393.954728795917</v>
+        <v>39241.8615517352</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3135,16 +3135,16 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C122">
-        <v>2313.18743770475</v>
+        <v>40274.91199119319</v>
       </c>
       <c r="D122">
-        <v>2050.379609518187</v>
+        <v>41351.35312049399</v>
       </c>
       <c r="E122">
-        <v>2158.015018647229</v>
+        <v>44632.82113421193</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3152,16 +3152,16 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C123">
-        <v>4487.422497745161</v>
+        <v>5702.582508173264</v>
       </c>
       <c r="D123">
-        <v>3251.340662315742</v>
+        <v>5197.04316560074</v>
       </c>
       <c r="E123">
-        <v>3680.595601936531</v>
+        <v>5490.350510109492</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3169,16 +3169,16 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C124">
-        <v>3291.571394333075</v>
+        <v>6531.454941380145</v>
       </c>
       <c r="D124">
-        <v>453.0691373312048</v>
+        <v>6914.424310549415</v>
       </c>
       <c r="E124">
-        <v>505.4945456516502</v>
+        <v>7565.494786531661</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3186,16 +3186,16 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C125">
-        <v>2962.271032197586</v>
+        <v>11086.07248419944</v>
       </c>
       <c r="D125">
-        <v>2922.939603860779</v>
+        <v>9081.046501582416</v>
       </c>
       <c r="E125">
-        <v>2944.717615440521</v>
+        <v>9712.39919620127</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3203,16 +3203,16 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C126">
-        <v>3978.851277647058</v>
+        <v>11235.01770760014</v>
       </c>
       <c r="D126">
-        <v>1566.476580450332</v>
+        <v>7294.264487669744</v>
       </c>
       <c r="E126">
-        <v>1592.42779801514</v>
+        <v>7393.954728795917</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3220,16 +3220,16 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C127">
-        <v>3624.875154413226</v>
+        <v>2313.18743770475</v>
       </c>
       <c r="D127">
-        <v>3677.660725632635</v>
+        <v>2050.379609518187</v>
       </c>
       <c r="E127">
-        <v>3727.402937205914</v>
+        <v>2158.015018647229</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3237,16 +3237,16 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C128">
-        <v>4499.453713305816</v>
+        <v>4487.422497745161</v>
       </c>
       <c r="D128">
-        <v>4389.339541465134</v>
+        <v>3251.340662315742</v>
       </c>
       <c r="E128">
-        <v>4489.156966460471</v>
+        <v>3680.595601936531</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3254,16 +3254,16 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C129">
-        <v>1176.375213333053</v>
+        <v>3291.571394333075</v>
       </c>
       <c r="D129">
-        <v>1229.853805184373</v>
+        <v>453.0691373312048</v>
       </c>
       <c r="E129">
-        <v>1330.656790249233</v>
+        <v>505.4945456516502</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3271,16 +3271,16 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C130">
-        <v>1013.219479989464</v>
+        <v>2962.271032197586</v>
       </c>
       <c r="D130">
-        <v>873.6169022987777</v>
+        <v>2922.939603860779</v>
       </c>
       <c r="E130">
-        <v>911.1327501980686</v>
+        <v>2944.717615440521</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3288,16 +3288,16 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C131">
-        <v>857.2621118872319</v>
+        <v>3978.851277647058</v>
       </c>
       <c r="D131">
-        <v>772.2734198315197</v>
+        <v>1566.476580450332</v>
       </c>
       <c r="E131">
-        <v>801.0018403865388</v>
+        <v>1592.42779801514</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3305,16 +3305,16 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C132">
-        <v>345179.8540918057</v>
+        <v>3624.875154413226</v>
       </c>
       <c r="D132">
-        <v>306070.7824845224</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E132">
-        <v>311915.8222954976</v>
+        <v>3727.402937205914</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3322,16 +3322,16 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C133">
-        <v>57843.05696310467</v>
+        <v>4499.453713305816</v>
       </c>
       <c r="D133">
-        <v>41761.14805054816</v>
+        <v>4389.339541465134</v>
       </c>
       <c r="E133">
-        <v>48660.60638720006</v>
+        <v>4489.156966460471</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3339,16 +3339,16 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C134">
-        <v>106400.8113634808</v>
+        <v>1176.375213333053</v>
       </c>
       <c r="D134">
-        <v>97376.26626200562</v>
+        <v>1229.853805184373</v>
       </c>
       <c r="E134">
-        <v>107457.7153467231</v>
+        <v>1330.656790249233</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3356,16 +3356,16 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C135">
-        <v>47754.67592555143</v>
+        <v>1013.219479989464</v>
       </c>
       <c r="D135">
-        <v>46917.82385382168</v>
+        <v>873.6169022987777</v>
       </c>
       <c r="E135">
-        <v>47285.0706371487</v>
+        <v>911.1327501980686</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3373,16 +3373,16 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C136">
-        <v>13642.04328300475</v>
+        <v>857.2621118872319</v>
       </c>
       <c r="D136">
-        <v>12594.12090677959</v>
+        <v>772.2734198315197</v>
       </c>
       <c r="E136">
-        <v>14151.68818183644</v>
+        <v>801.0018403865388</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3390,16 +3390,16 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C137">
-        <v>10166.68671320246</v>
+        <v>345179.8540918057</v>
       </c>
       <c r="D137">
-        <v>7870.660600118454</v>
+        <v>306070.7824845224</v>
       </c>
       <c r="E137">
-        <v>8448.569974010888</v>
+        <v>311915.8222954976</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3407,16 +3407,16 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C138">
-        <v>40056.29615048355</v>
+        <v>57843.05696310467</v>
       </c>
       <c r="D138">
-        <v>39938.78970433185</v>
+        <v>41761.14805054816</v>
       </c>
       <c r="E138">
-        <v>44520.15917103966</v>
+        <v>48660.60638720006</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3424,16 +3424,16 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C139">
-        <v>42099.78280750295</v>
+        <v>106400.8113634808</v>
       </c>
       <c r="D139">
-        <v>42299.87775020443</v>
+        <v>97376.26626200562</v>
       </c>
       <c r="E139">
-        <v>47328.28098195308</v>
+        <v>107457.7153467231</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3441,16 +3441,16 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C140">
-        <v>6780.581746217548</v>
+        <v>47754.67592555143</v>
       </c>
       <c r="D140">
-        <v>5344.462556042371</v>
+        <v>46917.82385382168</v>
       </c>
       <c r="E140">
-        <v>5852.587839854697</v>
+        <v>47285.0706371487</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3458,16 +3458,16 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C141">
-        <v>7052.041776574091</v>
+        <v>13642.04328300475</v>
       </c>
       <c r="D141">
-        <v>2387.833946905571</v>
+        <v>12594.12090677959</v>
       </c>
       <c r="E141">
-        <v>2653.360912751024</v>
+        <v>14151.68818183644</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3475,16 +3475,16 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C142">
-        <v>12491.64080553533</v>
+        <v>10166.68671320246</v>
       </c>
       <c r="D142">
-        <v>7553.961214696117</v>
+        <v>7870.660600118454</v>
       </c>
       <c r="E142">
-        <v>8823.015551678049</v>
+        <v>8448.569974010888</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3492,16 +3492,16 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C143">
-        <v>11918.07029478611</v>
+        <v>40056.29615048355</v>
       </c>
       <c r="D143">
-        <v>10755.76769609013</v>
+        <v>39938.78970433185</v>
       </c>
       <c r="E143">
-        <v>11073.8263395291</v>
+        <v>44520.15917103966</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3509,16 +3509,16 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C144">
-        <v>2510.791313969085</v>
+        <v>42099.78280750295</v>
       </c>
       <c r="D144">
-        <v>2080.311820058766</v>
+        <v>42299.87775020443</v>
       </c>
       <c r="E144">
-        <v>2225.787307207039</v>
+        <v>47328.28098195308</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3526,16 +3526,16 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C145">
-        <v>5559.189168957029</v>
+        <v>6780.581746217548</v>
       </c>
       <c r="D145">
-        <v>3507.429258284409</v>
+        <v>5344.462556042371</v>
       </c>
       <c r="E145">
-        <v>4514.632917614302</v>
+        <v>5852.587839854697</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3543,16 +3543,16 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C146">
-        <v>3740.698985412615</v>
+        <v>7052.041776574091</v>
       </c>
       <c r="D146">
-        <v>456.0519360615073</v>
+        <v>2387.833946905571</v>
       </c>
       <c r="E146">
-        <v>595.516072795263</v>
+        <v>2653.360912751024</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3560,16 +3560,16 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C147">
-        <v>3025.982972811596</v>
+        <v>12491.64080553533</v>
       </c>
       <c r="D147">
-        <v>2930.200017528361</v>
+        <v>7553.961214696117</v>
       </c>
       <c r="E147">
-        <v>2972.156458241908</v>
+        <v>8823.015551678049</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3577,16 +3577,16 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C148">
-        <v>4384.134004159239</v>
+        <v>11918.07029478611</v>
       </c>
       <c r="D148">
-        <v>3877.68979844253</v>
+        <v>10755.76769609013</v>
       </c>
       <c r="E148">
-        <v>3984.413723700878</v>
+        <v>11073.8263395291</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3594,16 +3594,16 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C149">
-        <v>3818.113674370041</v>
+        <v>2510.791313969085</v>
       </c>
       <c r="D149">
-        <v>3677.660725632635</v>
+        <v>2080.311820058766</v>
       </c>
       <c r="E149">
-        <v>3773.270697207371</v>
+        <v>2225.787307207039</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3611,16 +3611,16 @@
         <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C150">
-        <v>5697.549039481555</v>
+        <v>5559.189168957029</v>
       </c>
       <c r="D150">
-        <v>4449.270708440607</v>
+        <v>3507.429258284409</v>
       </c>
       <c r="E150">
-        <v>4794.85366801385</v>
+        <v>4514.632917614302</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -3628,16 +3628,16 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C151">
-        <v>1675.03137312741</v>
+        <v>3740.698985412615</v>
       </c>
       <c r="D151">
-        <v>1815.4386330182</v>
+        <v>456.0519360615073</v>
       </c>
       <c r="E151">
-        <v>2049.263941768266</v>
+        <v>595.516072795263</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3645,16 +3645,16 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C152">
-        <v>1388.615296125427</v>
+        <v>3025.982972811596</v>
       </c>
       <c r="D152">
-        <v>898.8243487684732</v>
+        <v>2930.200017528361</v>
       </c>
       <c r="E152">
-        <v>1101.853615098803</v>
+        <v>2972.156458241908</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3662,16 +3662,16 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C153">
-        <v>915.4210068592286</v>
+        <v>4384.134004159239</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>3877.68979844253</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>3984.413723700878</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3679,16 +3679,16 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C154">
-        <v>379833.2126030341</v>
+        <v>3818.113674370041</v>
       </c>
       <c r="D154">
-        <v>323789.1870151541</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E154">
-        <v>342305.1273678984</v>
+        <v>3773.270697207371</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3696,16 +3696,16 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C155">
-        <v>66636.46327624648</v>
+        <v>5697.549039481555</v>
       </c>
       <c r="D155">
-        <v>57885.11081377808</v>
+        <v>4449.270708440607</v>
       </c>
       <c r="E155">
-        <v>65450.5214985832</v>
+        <v>4794.85366801385</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3713,16 +3713,16 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C156">
-        <v>122447.4212601383</v>
+        <v>1675.03137312741</v>
       </c>
       <c r="D156">
-        <v>106273.0478090824</v>
+        <v>1815.4386330182</v>
       </c>
       <c r="E156">
-        <v>119530.3850553175</v>
+        <v>2049.263941768266</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3730,16 +3730,16 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C157">
-        <v>55098.14072490651</v>
+        <v>1388.615296125427</v>
       </c>
       <c r="D157">
-        <v>53997.08352943832</v>
+        <v>898.8243487684732</v>
       </c>
       <c r="E157">
-        <v>54429.29718809373</v>
+        <v>1101.853615098803</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3747,16 +3747,16 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C158">
-        <v>17436.20392355449</v>
+        <v>915.4210068592286</v>
       </c>
       <c r="D158">
-        <v>19678.07818882393</v>
+        <v>0</v>
       </c>
       <c r="E158">
-        <v>23411.63616688988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3764,16 +3764,16 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C159">
-        <v>11477.1443269179</v>
+        <v>379833.2126030341</v>
       </c>
       <c r="D159">
-        <v>7941.17271971979</v>
+        <v>323789.1870151541</v>
       </c>
       <c r="E159">
-        <v>8685.454438123739</v>
+        <v>342305.1273678984</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3781,16 +3781,16 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C160">
-        <v>44788.85407568982</v>
+        <v>66636.46327624648</v>
       </c>
       <c r="D160">
-        <v>42290.86139964137</v>
+        <v>57885.11081377808</v>
       </c>
       <c r="E160">
-        <v>48116.24030242601</v>
+        <v>65450.5214985832</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3798,16 +3798,16 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C161">
-        <v>43854.83257609577</v>
+        <v>122447.4212601383</v>
       </c>
       <c r="D161">
-        <v>42446.11108034404</v>
+        <v>106273.0478090824</v>
       </c>
       <c r="E161">
-        <v>48048.47217811201</v>
+        <v>119530.3850553175</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3815,16 +3815,16 @@
         <v>164</v>
       </c>
       <c r="B162" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C162">
-        <v>7818.02330571639</v>
+        <v>55098.14072490651</v>
       </c>
       <c r="D162">
-        <v>5653.095564499369</v>
+        <v>53997.08352943832</v>
       </c>
       <c r="E162">
-        <v>6625.371912088781</v>
+        <v>54429.29718809373</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3832,16 +3832,16 @@
         <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C163">
-        <v>8085.182658295945</v>
+        <v>17436.20392355449</v>
       </c>
       <c r="D163">
-        <v>7503.614943774021</v>
+        <v>19678.07818882393</v>
       </c>
       <c r="E163">
-        <v>8938.0868588093</v>
+        <v>23411.63616688988</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3849,16 +3849,16 @@
         <v>166</v>
       </c>
       <c r="B164" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C164">
-        <v>14492.94704346139</v>
+        <v>11477.1443269179</v>
       </c>
       <c r="D164">
-        <v>11209.84775023005</v>
+        <v>7941.17271971979</v>
       </c>
       <c r="E164">
-        <v>10752.42132399964</v>
+        <v>8685.454438123739</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3866,16 +3866,16 @@
         <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C165">
-        <v>14025.08468897277</v>
+        <v>44788.85407568982</v>
       </c>
       <c r="D165">
-        <v>11232.84453326727</v>
+        <v>42290.86139964137</v>
       </c>
       <c r="E165">
-        <v>12584.87999504888</v>
+        <v>48116.24030242601</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3883,16 +3883,16 @@
         <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C166">
-        <v>2660.082565212768</v>
+        <v>43854.83257609577</v>
       </c>
       <c r="D166">
-        <v>2118.88338047299</v>
+        <v>42446.11108034404</v>
       </c>
       <c r="E166">
-        <v>2317.74860784036</v>
+        <v>48048.47217811201</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3900,16 +3900,16 @@
         <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C167">
-        <v>6699.919359426849</v>
+        <v>7818.02330571639</v>
       </c>
       <c r="D167">
-        <v>3926.964562863937</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E167">
-        <v>5419.280756815793</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3917,16 +3917,16 @@
         <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C168">
-        <v>4240.498957073307</v>
+        <v>8085.182658295945</v>
       </c>
       <c r="D168">
-        <v>2799.802017040321</v>
+        <v>7503.614943774021</v>
       </c>
       <c r="E168">
-        <v>3370.629266244694</v>
+        <v>8938.0868588093</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3934,16 +3934,16 @@
         <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C169">
-        <v>3104.11640049039</v>
+        <v>14492.94704346139</v>
       </c>
       <c r="D169">
-        <v>2945.585161856526</v>
+        <v>11209.84775023005</v>
       </c>
       <c r="E169">
-        <v>3032.000269374993</v>
+        <v>10752.42132399964</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3951,16 +3951,16 @@
         <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C170">
-        <v>4758.923090909089</v>
+        <v>14025.08468897277</v>
       </c>
       <c r="D170">
-        <v>4052.36859619171</v>
+        <v>11232.84453326727</v>
       </c>
       <c r="E170">
-        <v>4241.271500156832</v>
+        <v>12584.87999504888</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3968,16 +3968,16 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C171">
-        <v>4582.423026269129</v>
+        <v>2660.082565212768</v>
       </c>
       <c r="D171">
-        <v>3677.660725632635</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E171">
-        <v>3936.041511138754</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -3985,16 +3985,16 @@
         <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C172">
-        <v>8274.311032145955</v>
+        <v>6699.919359426849</v>
       </c>
       <c r="D172">
-        <v>4554.906523253632</v>
+        <v>3926.964562863937</v>
       </c>
       <c r="E172">
-        <v>6530.74208924048</v>
+        <v>5419.280756815793</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4002,16 +4002,16 @@
         <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C173">
-        <v>2362.496887971177</v>
+        <v>4240.498957073307</v>
       </c>
       <c r="D173">
-        <v>4552.94161730676</v>
+        <v>2799.802017040321</v>
       </c>
       <c r="E173">
-        <v>7699.768813994026</v>
+        <v>3370.629266244694</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4019,16 +4019,16 @@
         <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C174">
-        <v>1764.352253203638</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D174">
-        <v>974.5725435688446</v>
+        <v>2945.585161856526</v>
       </c>
       <c r="E174">
-        <v>1393.90973989574</v>
+        <v>3032.000269374993</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -4036,16 +4036,16 @@
         <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C175">
-        <v>921.2368963564281</v>
+        <v>4758.923090909089</v>
       </c>
       <c r="D175">
-        <v>0</v>
+        <v>4052.36859619171</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>4241.271500156832</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4053,16 +4053,16 @@
         <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C176">
-        <v>409436.7691592983</v>
+        <v>4582.423026269129</v>
       </c>
       <c r="D176">
-        <v>355341.7534723968</v>
+        <v>3677.660725632635</v>
       </c>
       <c r="E176">
-        <v>387999.3260030203</v>
+        <v>3936.041511138754</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4070,16 +4070,16 @@
         <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C177">
-        <v>66424.65479531829</v>
+        <v>8274.311032145955</v>
       </c>
       <c r="D177">
-        <v>67311.96044664056</v>
+        <v>4554.906523253632</v>
       </c>
       <c r="E177">
-        <v>76231.77993843338</v>
+        <v>6530.74208924048</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -4087,16 +4087,16 @@
         <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C178">
-        <v>125858.7401545331</v>
+        <v>2362.496887971177</v>
       </c>
       <c r="D178">
-        <v>95923.88790038624</v>
+        <v>4552.94161730676</v>
       </c>
       <c r="E178">
-        <v>124140.5773429784</v>
+        <v>7699.768813994026</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -4104,16 +4104,16 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C179">
-        <v>55158.37308241575</v>
+        <v>1764.352253203638</v>
       </c>
       <c r="D179">
-        <v>54194.17670445503</v>
+        <v>974.5725435688446</v>
       </c>
       <c r="E179">
-        <v>54731.6463609033</v>
+        <v>1393.90973989574</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -4121,16 +4121,16 @@
         <v>182</v>
       </c>
       <c r="B180" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C180">
-        <v>18810.64774314864</v>
+        <v>921.2368963564281</v>
       </c>
       <c r="D180">
-        <v>26985.75868185313</v>
+        <v>0</v>
       </c>
       <c r="E180">
-        <v>33814.25416223275</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4138,16 +4138,16 @@
         <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C181">
-        <v>11786.58854248258</v>
+        <v>409436.7691592983</v>
       </c>
       <c r="D181">
-        <v>9267.503482344102</v>
+        <v>355341.7534723968</v>
       </c>
       <c r="E181">
-        <v>10151.93626108859</v>
+        <v>387999.3260030203</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -4155,16 +4155,16 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C182">
-        <v>41809.31820607139</v>
+        <v>66424.65479531829</v>
       </c>
       <c r="D182">
-        <v>39732.01918427406</v>
+        <v>67311.96044664056</v>
       </c>
       <c r="E182">
-        <v>46033.76592047335</v>
+        <v>76231.77993843338</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -4172,16 +4172,16 @@
         <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C183">
-        <v>44322.79570608526</v>
+        <v>125858.7401545331</v>
       </c>
       <c r="D183">
-        <v>42997.62304068729</v>
+        <v>95923.88790038624</v>
       </c>
       <c r="E183">
-        <v>49150.09462369821</v>
+        <v>124140.5773429784</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4189,16 +4189,16 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C184">
-        <v>7830.871226366395</v>
+        <v>55158.37308241575</v>
       </c>
       <c r="D184">
-        <v>5653.095564499369</v>
+        <v>54194.17670445503</v>
       </c>
       <c r="E184">
-        <v>6625.371912088781</v>
+        <v>54731.6463609033</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -4206,16 +4206,16 @@
         <v>187</v>
       </c>
       <c r="B185" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C185">
-        <v>8817.535269776827</v>
+        <v>18810.64774314864</v>
       </c>
       <c r="D185">
-        <v>9011.059942949789</v>
+        <v>26985.75868185313</v>
       </c>
       <c r="E185">
-        <v>10838.71267389012</v>
+        <v>33814.25416223275</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -4223,16 +4223,16 @@
         <v>188</v>
       </c>
       <c r="B186" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C186">
-        <v>15730.7337703995</v>
+        <v>11786.58854248258</v>
       </c>
       <c r="D186">
-        <v>12870.92751701806</v>
+        <v>9267.503482344102</v>
       </c>
       <c r="E186">
-        <v>16028.57827823479</v>
+        <v>10151.93626108859</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -4240,16 +4240,16 @@
         <v>189</v>
       </c>
       <c r="B187" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C187">
-        <v>14763.70638988416</v>
+        <v>41809.31820607139</v>
       </c>
       <c r="D187">
-        <v>11353.82086139094</v>
+        <v>39732.01918427406</v>
       </c>
       <c r="E187">
-        <v>15744.22408353954</v>
+        <v>46033.76592047335</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -4257,16 +4257,16 @@
         <v>190</v>
       </c>
       <c r="B188" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C188">
-        <v>2664.581838046233</v>
+        <v>44322.79570608526</v>
       </c>
       <c r="D188">
-        <v>2118.88338047299</v>
+        <v>42997.62304068729</v>
       </c>
       <c r="E188">
-        <v>2317.74860784036</v>
+        <v>49150.09462369821</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -4274,16 +4274,16 @@
         <v>191</v>
       </c>
       <c r="B189" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C189">
-        <v>7118.299388486004</v>
+        <v>7830.871226366395</v>
       </c>
       <c r="D189">
-        <v>4387.796042371227</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E189">
-        <v>6214.950571608244</v>
+        <v>6625.371912088781</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -4291,16 +4291,16 @@
         <v>192</v>
       </c>
       <c r="B190" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C190">
-        <v>1256.930682890124</v>
+        <v>8817.535269776827</v>
       </c>
       <c r="D190">
-        <v>634.2799162905493</v>
+        <v>9011.059942949789</v>
       </c>
       <c r="E190">
-        <v>1060.520130278657</v>
+        <v>10838.71267389012</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4308,16 +4308,16 @@
         <v>193</v>
       </c>
       <c r="B191" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C191">
-        <v>3104.11640049039</v>
+        <v>15730.7337703995</v>
       </c>
       <c r="D191">
-        <v>2953.473502833881</v>
+        <v>12870.92751701806</v>
       </c>
       <c r="E191">
-        <v>3032.074436227733</v>
+        <v>16028.57827823479</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4325,16 +4325,16 @@
         <v>194</v>
       </c>
       <c r="B192" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C192">
-        <v>0</v>
+        <v>14763.70638988416</v>
       </c>
       <c r="D192">
-        <v>0</v>
+        <v>11353.82086139094</v>
       </c>
       <c r="E192">
-        <v>1927.316250691574</v>
+        <v>15744.22408353954</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4342,16 +4342,16 @@
         <v>195</v>
       </c>
       <c r="B193" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C193">
-        <v>4982.658106436934</v>
+        <v>2664.581838046233</v>
       </c>
       <c r="D193">
-        <v>3682.745087885083</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E193">
-        <v>4606.149113368056</v>
+        <v>2317.74860784036</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4359,16 +4359,16 @@
         <v>196</v>
       </c>
       <c r="B194" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C194">
-        <v>9858.7475739898</v>
+        <v>7118.299388486004</v>
       </c>
       <c r="D194">
-        <v>4988.549100871839</v>
+        <v>4387.796042371227</v>
       </c>
       <c r="E194">
-        <v>9051.622561655677</v>
+        <v>6214.950571608244</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -4376,16 +4376,16 @@
         <v>197</v>
       </c>
       <c r="B195" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C195">
-        <v>3049.962402814945</v>
+        <v>1256.930682890124</v>
       </c>
       <c r="D195">
-        <v>7885.799173422068</v>
+        <v>634.2799162905493</v>
       </c>
       <c r="E195">
-        <v>14476.78741030169</v>
+        <v>1060.520130278657</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -4393,16 +4393,16 @@
         <v>198</v>
       </c>
       <c r="B196" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C196">
-        <v>1932.537890358078</v>
+        <v>3104.11640049039</v>
       </c>
       <c r="D196">
-        <v>1092.439628676345</v>
+        <v>2953.473502833881</v>
       </c>
       <c r="E196">
-        <v>1729.767824059069</v>
+        <v>3032.074436227733</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4410,16 +4410,16 @@
         <v>199</v>
       </c>
       <c r="B197" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C197">
-        <v>927.0527858536279</v>
+        <v>0</v>
       </c>
       <c r="D197">
-        <v>885.4644642160963</v>
+        <v>0</v>
       </c>
       <c r="E197">
-        <v>854.6967352460968</v>
+        <v>1927.316250691574</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4427,16 +4427,16 @@
         <v>200</v>
       </c>
       <c r="B198" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C198">
-        <v>425667.2304377211</v>
+        <v>4982.658106436934</v>
       </c>
       <c r="D198">
-        <v>379452.4458343688</v>
+        <v>3682.745087885083</v>
       </c>
       <c r="E198">
-        <v>422462.404769241</v>
+        <v>4606.149113368056</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4444,16 +4444,16 @@
         <v>201</v>
       </c>
       <c r="B199" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C199">
-        <v>74824.1776942108</v>
+        <v>9858.7475739898</v>
       </c>
       <c r="D199">
-        <v>75532.04105321791</v>
+        <v>4988.549100871839</v>
       </c>
       <c r="E199">
-        <v>86492.52473873404</v>
+        <v>9051.622561655677</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4461,16 +4461,16 @@
         <v>202</v>
       </c>
       <c r="B200" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C200">
-        <v>128549.8642605276</v>
+        <v>3049.962402814945</v>
       </c>
       <c r="D200">
-        <v>114702.4949950556</v>
+        <v>7885.799173422068</v>
       </c>
       <c r="E200">
-        <v>134200.4554046213</v>
+        <v>14476.78741030169</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4478,16 +4478,16 @@
         <v>203</v>
       </c>
       <c r="B201" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C201">
-        <v>55242.88725228325</v>
+        <v>1932.537890358078</v>
       </c>
       <c r="D201">
-        <v>54348.67956945477</v>
+        <v>1092.439628676345</v>
       </c>
       <c r="E201">
-        <v>54823.8158790419</v>
+        <v>1729.767824059069</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4495,16 +4495,16 @@
         <v>204</v>
       </c>
       <c r="B202" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C202">
-        <v>21186.42152206995</v>
+        <v>927.0527858536279</v>
       </c>
       <c r="D202">
-        <v>32192.86399794241</v>
+        <v>885.4644642160963</v>
       </c>
       <c r="E202">
-        <v>40091.29523030741</v>
+        <v>854.6967352460968</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4512,16 +4512,16 @@
         <v>205</v>
       </c>
       <c r="B203" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C203">
-        <v>12108.98627481771</v>
+        <v>425667.2304377211</v>
       </c>
       <c r="D203">
-        <v>9710.044517252907</v>
+        <v>379452.4458343688</v>
       </c>
       <c r="E203">
-        <v>9820.712234959921</v>
+        <v>422462.404769241</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4529,16 +4529,16 @@
         <v>206</v>
       </c>
       <c r="B204" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C204">
-        <v>44818.4592191087</v>
+        <v>74824.1776942108</v>
       </c>
       <c r="D204">
-        <v>43318.43942297382</v>
+        <v>75532.04105321791</v>
       </c>
       <c r="E204">
-        <v>50430.2444258372</v>
+        <v>86492.52473873404</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4546,16 +4546,16 @@
         <v>207</v>
       </c>
       <c r="B205" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C205">
-        <v>45410.20682375576</v>
+        <v>128549.8642605276</v>
       </c>
       <c r="D205">
-        <v>44140.29328236685</v>
+        <v>114702.4949950556</v>
       </c>
       <c r="E205">
-        <v>50777.920807722</v>
+        <v>134200.4554046213</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4563,16 +4563,16 @@
         <v>208</v>
       </c>
       <c r="B206" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C206">
-        <v>7877.356799130208</v>
+        <v>55242.88725228325</v>
       </c>
       <c r="D206">
-        <v>5653.095564499369</v>
+        <v>54348.67956945477</v>
       </c>
       <c r="E206">
-        <v>6662.276843942194</v>
+        <v>54823.8158790419</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -4580,16 +4580,16 @@
         <v>209</v>
       </c>
       <c r="B207" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C207">
-        <v>7081.366168574467</v>
+        <v>21186.42152206995</v>
       </c>
       <c r="D207">
-        <v>7237.854347805022</v>
+        <v>32192.86399794241</v>
       </c>
       <c r="E207">
-        <v>8761.01660377788</v>
+        <v>40091.29523030741</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -4597,16 +4597,16 @@
         <v>210</v>
       </c>
       <c r="B208" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C208">
-        <v>17240.04215367412</v>
+        <v>12108.98627481771</v>
       </c>
       <c r="D208">
-        <v>13942.82778271549</v>
+        <v>9710.044517252907</v>
       </c>
       <c r="E208">
-        <v>14713.17492592106</v>
+        <v>9820.712234959921</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -4614,16 +4614,16 @@
         <v>211</v>
       </c>
       <c r="B209" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C209">
-        <v>17324.03456184319</v>
+        <v>44818.4592191087</v>
       </c>
       <c r="D209">
-        <v>13476.54727078326</v>
+        <v>43318.43942297382</v>
       </c>
       <c r="E209">
-        <v>22628.13038686703</v>
+        <v>50430.2444258372</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -4631,16 +4631,16 @@
         <v>212</v>
       </c>
       <c r="B210" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C210">
-        <v>2689.033001442709</v>
+        <v>45410.20682375576</v>
       </c>
       <c r="D210">
-        <v>2118.88338047299</v>
+        <v>44140.29328236685</v>
       </c>
       <c r="E210">
-        <v>2326.478289412053</v>
+        <v>50777.920807722</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -4648,16 +4648,16 @@
         <v>213</v>
       </c>
       <c r="B211" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C211">
-        <v>7330.001934671265</v>
+        <v>7877.356799130208</v>
       </c>
       <c r="D211">
-        <v>4696.892936408833</v>
+        <v>5653.095564499369</v>
       </c>
       <c r="E211">
-        <v>6336.909947377137</v>
+        <v>6662.276843942194</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -4665,16 +4665,16 @@
         <v>214</v>
       </c>
       <c r="B212" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C212">
-        <v>3666.34991690552</v>
+        <v>7081.366168574467</v>
       </c>
       <c r="D212">
-        <v>2659.16265449915</v>
+        <v>7237.854347805022</v>
       </c>
       <c r="E212">
-        <v>3251.428044629679</v>
+        <v>8761.01660377788</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -4682,16 +4682,16 @@
         <v>215</v>
       </c>
       <c r="B213" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C213">
-        <v>3110.615608057638</v>
+        <v>17240.04215367412</v>
       </c>
       <c r="D213">
-        <v>2966.871688417814</v>
+        <v>13942.82778271549</v>
       </c>
       <c r="E213">
-        <v>3044.077493176301</v>
+        <v>14713.17492592106</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -4699,16 +4699,16 @@
         <v>216</v>
       </c>
       <c r="B214" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C214">
-        <v>4955.203939982344</v>
+        <v>17324.03456184319</v>
       </c>
       <c r="D214">
-        <v>4437.491921939725</v>
+        <v>13476.54727078326</v>
       </c>
       <c r="E214">
-        <v>4802.656681354792</v>
+        <v>22628.13038686703</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -4716,16 +4716,16 @@
         <v>217</v>
       </c>
       <c r="B215" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C215">
-        <v>5584.532853170555</v>
+        <v>2689.033001442709</v>
       </c>
       <c r="D215">
-        <v>3696.358431113311</v>
+        <v>2118.88338047299</v>
       </c>
       <c r="E215">
-        <v>5041.150517084573</v>
+        <v>2326.478289412053</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -4733,16 +4733,16 @@
         <v>218</v>
       </c>
       <c r="B216" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C216">
-        <v>12228.85287007065</v>
+        <v>7330.001934671265</v>
       </c>
       <c r="D216">
-        <v>5315.793599021267</v>
+        <v>4696.892936408833</v>
       </c>
       <c r="E216">
-        <v>10793.64798057903</v>
+        <v>6336.909947377137</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -4750,16 +4750,16 @@
         <v>219</v>
       </c>
       <c r="B217" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C217">
-        <v>3909.407627315059</v>
+        <v>3666.34991690552</v>
       </c>
       <c r="D217">
-        <v>12148.67547071851</v>
+        <v>2659.16265449915</v>
       </c>
       <c r="E217">
-        <v>24644.07599310096</v>
+        <v>3251.428044629679</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -4767,16 +4767,16 @@
         <v>220</v>
       </c>
       <c r="B218" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C218">
-        <v>2078.961774546943</v>
+        <v>3110.615608057638</v>
       </c>
       <c r="D218">
-        <v>1179.897477494976</v>
+        <v>2966.871688417814</v>
       </c>
       <c r="E218">
-        <v>1832.168256550158</v>
+        <v>3044.077493176301</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -4784,16 +4784,16 @@
         <v>221</v>
       </c>
       <c r="B219" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C219">
-        <v>932.8686753508275</v>
+        <v>4955.203939982344</v>
       </c>
       <c r="D219">
-        <v>920.6062716110156</v>
+        <v>4437.491921939725</v>
       </c>
       <c r="E219">
-        <v>0</v>
+        <v>4802.656681354792</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -4801,16 +4801,16 @@
         <v>222</v>
       </c>
       <c r="B220" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C220">
-        <v>195705.6</v>
+        <v>5584.532853170555</v>
       </c>
       <c r="D220">
-        <v>184867.2</v>
+        <v>3696.358431113311</v>
       </c>
       <c r="E220">
-        <v>187784</v>
+        <v>5041.150517084573</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -4818,16 +4818,16 @@
         <v>223</v>
       </c>
       <c r="B221" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C221">
-        <v>223624</v>
+        <v>12228.85287007065</v>
       </c>
       <c r="D221">
-        <v>205627.2</v>
+        <v>5315.793599021267</v>
       </c>
       <c r="E221">
-        <v>214700.8</v>
+        <v>10793.64798057903</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -4835,16 +4835,16 @@
         <v>224</v>
       </c>
       <c r="B222" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C222">
-        <v>253637.6</v>
+        <v>3909.407627315059</v>
       </c>
       <c r="D222">
-        <v>224994.4</v>
+        <v>12148.67547071851</v>
       </c>
       <c r="E222">
-        <v>242126.4</v>
+        <v>24644.07599310096</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -4852,16 +4852,16 @@
         <v>225</v>
       </c>
       <c r="B223" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C223">
-        <v>284854.4</v>
+        <v>2078.961774546943</v>
       </c>
       <c r="D223">
-        <v>242956.8</v>
+        <v>1179.897477494976</v>
       </c>
       <c r="E223">
-        <v>270748</v>
+        <v>1832.168256550158</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -4869,16 +4869,16 @@
         <v>226</v>
       </c>
       <c r="B224" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C224">
-        <v>275764.8</v>
+        <v>932.8686753508275</v>
       </c>
       <c r="D224">
-        <v>258018.4</v>
+        <v>920.6062716110156</v>
       </c>
       <c r="E224">
-        <v>296766.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -4886,16 +4886,16 @@
         <v>227</v>
       </c>
       <c r="B225" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C225">
-        <v>285775.2</v>
+        <v>195705.6</v>
       </c>
       <c r="D225">
-        <v>276530.4</v>
+        <v>184867.2</v>
       </c>
       <c r="E225">
-        <v>326134.4</v>
+        <v>187784</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -4903,16 +4903,16 @@
         <v>228</v>
       </c>
       <c r="B226" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C226">
-        <v>181481.6</v>
+        <v>223624</v>
       </c>
       <c r="D226">
-        <v>171418.4</v>
+        <v>205627.2</v>
       </c>
       <c r="E226">
-        <v>173696</v>
+        <v>214700.8</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -4920,16 +4920,16 @@
         <v>229</v>
       </c>
       <c r="B227" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C227">
-        <v>206952</v>
+        <v>253637.6</v>
       </c>
       <c r="D227">
-        <v>183019.2</v>
+        <v>224994.4</v>
       </c>
       <c r="E227">
-        <v>189584.8</v>
+        <v>242126.4</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -4937,16 +4937,16 @@
         <v>230</v>
       </c>
       <c r="B228" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C228">
-        <v>236529.6</v>
+        <v>284854.4</v>
       </c>
       <c r="D228">
-        <v>204145.6</v>
+        <v>242956.8</v>
       </c>
       <c r="E228">
-        <v>217076.8</v>
+        <v>270748</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -4954,16 +4954,16 @@
         <v>231</v>
       </c>
       <c r="B229" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C229">
-        <v>266166.4</v>
+        <v>275764.8</v>
       </c>
       <c r="D229">
-        <v>221178.4</v>
+        <v>258018.4</v>
       </c>
       <c r="E229">
-        <v>243465.6</v>
+        <v>296766.4</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -4971,16 +4971,16 @@
         <v>232</v>
       </c>
       <c r="B230" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C230">
-        <v>266616</v>
+        <v>285775.2</v>
       </c>
       <c r="D230">
-        <v>234677.6</v>
+        <v>276530.4</v>
       </c>
       <c r="E230">
-        <v>267149.6</v>
+        <v>326134.4</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -4988,16 +4988,16 @@
         <v>233</v>
       </c>
       <c r="B231" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C231">
-        <v>275787.2</v>
+        <v>181481.6</v>
       </c>
       <c r="D231">
-        <v>252004</v>
+        <v>171418.4</v>
       </c>
       <c r="E231">
-        <v>295416</v>
+        <v>173696</v>
       </c>
     </row>
     <row r="232" spans="1:5">
@@ -5005,16 +5005,16 @@
         <v>234</v>
       </c>
       <c r="B232" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C232">
-        <v>166797.6</v>
+        <v>206952</v>
       </c>
       <c r="D232">
-        <v>173032.8</v>
+        <v>183019.2</v>
       </c>
       <c r="E232">
-        <v>175456.8</v>
+        <v>189584.8</v>
       </c>
     </row>
     <row r="233" spans="1:5">
@@ -5022,16 +5022,16 @@
         <v>235</v>
       </c>
       <c r="B233" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C233">
-        <v>187860.8</v>
+        <v>236529.6</v>
       </c>
       <c r="D233">
-        <v>192721.6</v>
+        <v>204145.6</v>
       </c>
       <c r="E233">
-        <v>199666.4</v>
+        <v>217076.8</v>
       </c>
     </row>
     <row r="234" spans="1:5">
@@ -5039,16 +5039,16 @@
         <v>236</v>
       </c>
       <c r="B234" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C234">
-        <v>214399.2</v>
+        <v>266166.4</v>
       </c>
       <c r="D234">
-        <v>208928.8</v>
+        <v>221178.4</v>
       </c>
       <c r="E234">
-        <v>221102.4</v>
+        <v>243465.6</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -5056,16 +5056,16 @@
         <v>237</v>
       </c>
       <c r="B235" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C235">
-        <v>240393.6</v>
+        <v>266616</v>
       </c>
       <c r="D235">
-        <v>232657.6</v>
+        <v>234677.6</v>
       </c>
       <c r="E235">
-        <v>254091.2</v>
+        <v>267149.6</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -5073,16 +5073,16 @@
         <v>238</v>
       </c>
       <c r="B236" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C236">
-        <v>266132</v>
+        <v>275787.2</v>
       </c>
       <c r="D236">
-        <v>251892</v>
+        <v>252004</v>
       </c>
       <c r="E236">
-        <v>284350.4</v>
+        <v>295416</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -5090,15 +5090,100 @@
         <v>239</v>
       </c>
       <c r="B237" t="s">
+        <v>246</v>
+      </c>
+      <c r="C237">
+        <v>166797.6</v>
+      </c>
+      <c r="D237">
+        <v>173032.8</v>
+      </c>
+      <c r="E237">
+        <v>175456.8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B238" t="s">
+        <v>246</v>
+      </c>
+      <c r="C238">
+        <v>187860.8</v>
+      </c>
+      <c r="D238">
+        <v>192721.6</v>
+      </c>
+      <c r="E238">
+        <v>199666.4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C237">
+      <c r="B239" t="s">
+        <v>246</v>
+      </c>
+      <c r="C239">
+        <v>214399.2</v>
+      </c>
+      <c r="D239">
+        <v>208928.8</v>
+      </c>
+      <c r="E239">
+        <v>221102.4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B240" t="s">
+        <v>246</v>
+      </c>
+      <c r="C240">
+        <v>240393.6</v>
+      </c>
+      <c r="D240">
+        <v>232657.6</v>
+      </c>
+      <c r="E240">
+        <v>254091.2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B241" t="s">
+        <v>246</v>
+      </c>
+      <c r="C241">
+        <v>266132</v>
+      </c>
+      <c r="D241">
+        <v>251892</v>
+      </c>
+      <c r="E241">
+        <v>284350.4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B242" t="s">
+        <v>246</v>
+      </c>
+      <c r="C242">
         <v>277836.8</v>
       </c>
-      <c r="D237">
+      <c r="D242">
         <v>271554.4</v>
       </c>
-      <c r="E237">
+      <c r="E242">
         <v>316714.4</v>
       </c>
     </row>

</xml_diff>